<commit_message>
Adding Valid Anagram, Search in Rotated Sorted Array, Find Minimum in Rotated Sorted Array II, and 3Sum;\
</commit_message>
<xml_diff>
--- a/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -1602,8 +1602,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1737,7 +1737,7 @@
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1754,7 +1754,7 @@
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1771,7 +1771,7 @@
       <c r="A10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -2519,7 +2519,7 @@
       <c r="A54" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="6" t="s">
         <v>209</v>
       </c>
       <c r="C54" s="7" t="s">

</xml_diff>

<commit_message>
Pushing solutions for problems  Missing Number, Coin Change, Counting Bits, and Sum of Two Integers; 0/1 Knapsack implementation with backtracking and memoization
</commit_message>
<xml_diff>
--- a/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -1115,7 +1115,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1144,6 +1144,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -1265,7 +1271,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1310,19 +1316,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1334,7 +1344,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1342,7 +1352,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1602,8 +1612,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1788,7 +1798,7 @@
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1805,13 +1815,13 @@
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -1822,13 +1832,13 @@
       <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="9" t="s">
@@ -1839,13 +1849,13 @@
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="12" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -1856,13 +1866,13 @@
       <c r="A15" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -1873,13 +1883,13 @@
       <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="12" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="9" t="s">
@@ -1890,7 +1900,7 @@
       <c r="A17" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>68</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -1947,7 +1957,7 @@
       <c r="C20" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="12" t="s">
         <v>82</v>
       </c>
       <c r="E20" s="9" t="s">
@@ -2148,7 +2158,7 @@
       <c r="B32" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="13" t="s">
         <v>130</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -2159,13 +2169,13 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>134</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -2176,10 +2186,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C34" s="10" t="s">
@@ -2193,10 +2203,10 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C35" s="10" t="s">
@@ -2216,7 +2226,7 @@
       <c r="B36" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="13" t="s">
         <v>147</v>
       </c>
       <c r="D36" s="8" t="s">
@@ -2264,7 +2274,7 @@
       <c r="A39" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -2278,10 +2288,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -2352,7 +2362,7 @@
       <c r="B44" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="13" t="s">
         <v>180</v>
       </c>
       <c r="D44" s="8" t="s">
@@ -2499,13 +2509,13 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="16" t="s">
         <v>217</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="13" t="s">
         <v>218</v>
       </c>
       <c r="D53" s="8" t="s">
@@ -2618,10 +2628,10 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="15" t="s">
         <v>209</v>
       </c>
       <c r="C60" s="10" t="s">
@@ -2692,7 +2702,7 @@
       <c r="B64" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="13" t="s">
         <v>263</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -2726,7 +2736,7 @@
       <c r="B66" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="13" t="s">
         <v>271</v>
       </c>
       <c r="D66" s="8" t="s">
@@ -2862,7 +2872,7 @@
       <c r="B74" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C74" s="12" t="s">
+      <c r="C74" s="13" t="s">
         <v>303</v>
       </c>
       <c r="D74" s="8" t="s">
@@ -2879,7 +2889,7 @@
       <c r="B75" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C75" s="12" t="s">
+      <c r="C75" s="13" t="s">
         <v>180</v>
       </c>
       <c r="D75" s="8" t="s">
@@ -2913,10 +2923,10 @@
       <c r="B77" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C77" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="D77" s="11" t="s">
+      <c r="D77" s="12" t="s">
         <v>314</v>
       </c>
       <c r="E77" s="9" t="s">
@@ -2924,2779 +2934,2779 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="16"/>
-      <c r="B78" s="17"/>
+      <c r="A78" s="17"/>
+      <c r="B78" s="18"/>
     </row>
     <row r="79" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="B79" s="19" t="s">
+      <c r="B79" s="20" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="20"/>
+      <c r="A80" s="21"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="20"/>
+      <c r="A81" s="21"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="20"/>
+      <c r="A82" s="21"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="20"/>
+      <c r="A83" s="21"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="20"/>
+      <c r="A84" s="21"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="20"/>
+      <c r="A85" s="21"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="20"/>
+      <c r="A86" s="21"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="20"/>
+      <c r="A87" s="21"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="20"/>
+      <c r="A88" s="21"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="20"/>
+      <c r="A89" s="21"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="20"/>
+      <c r="A90" s="21"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="20"/>
+      <c r="A91" s="21"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="20"/>
+      <c r="A92" s="21"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="20"/>
+      <c r="A93" s="21"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="20"/>
+      <c r="A94" s="21"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="20"/>
+      <c r="A95" s="21"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="20"/>
+      <c r="A96" s="21"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="20"/>
+      <c r="A97" s="21"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="20"/>
+      <c r="A98" s="21"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="20"/>
+      <c r="A99" s="21"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="20"/>
+      <c r="A100" s="21"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="20"/>
+      <c r="A101" s="21"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="20"/>
+      <c r="A102" s="21"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="20"/>
+      <c r="A103" s="21"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="20"/>
+      <c r="A104" s="21"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="20"/>
+      <c r="A105" s="21"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="20"/>
+      <c r="A106" s="21"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="20"/>
+      <c r="A107" s="21"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="20"/>
+      <c r="A108" s="21"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="20"/>
+      <c r="A109" s="21"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="20"/>
+      <c r="A110" s="21"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="20"/>
+      <c r="A111" s="21"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="20"/>
+      <c r="A112" s="21"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="20"/>
+      <c r="A113" s="21"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="20"/>
+      <c r="A114" s="21"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="20"/>
+      <c r="A115" s="21"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="20"/>
+      <c r="A116" s="21"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="20"/>
+      <c r="A117" s="21"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="20"/>
+      <c r="A118" s="21"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="20"/>
+      <c r="A119" s="21"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="20"/>
+      <c r="A120" s="21"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="20"/>
+      <c r="A121" s="21"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="20"/>
+      <c r="A122" s="21"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="20"/>
+      <c r="A123" s="21"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="20"/>
+      <c r="A124" s="21"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="20"/>
+      <c r="A125" s="21"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="20"/>
+      <c r="A126" s="21"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="20"/>
+      <c r="A127" s="21"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="20"/>
+      <c r="A128" s="21"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="20"/>
+      <c r="A129" s="21"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="20"/>
+      <c r="A130" s="21"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="20"/>
+      <c r="A131" s="21"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="20"/>
+      <c r="A132" s="21"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="20"/>
+      <c r="A133" s="21"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="20"/>
+      <c r="A134" s="21"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="20"/>
+      <c r="A135" s="21"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="20"/>
+      <c r="A136" s="21"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="20"/>
+      <c r="A137" s="21"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="20"/>
+      <c r="A138" s="21"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="20"/>
+      <c r="A139" s="21"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="20"/>
+      <c r="A140" s="21"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="20"/>
+      <c r="A141" s="21"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="20"/>
+      <c r="A142" s="21"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="20"/>
+      <c r="A143" s="21"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="20"/>
+      <c r="A144" s="21"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="20"/>
+      <c r="A145" s="21"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="20"/>
+      <c r="A146" s="21"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="20"/>
+      <c r="A147" s="21"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="20"/>
+      <c r="A148" s="21"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="20"/>
+      <c r="A149" s="21"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="20"/>
+      <c r="A150" s="21"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="20"/>
+      <c r="A151" s="21"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="20"/>
+      <c r="A152" s="21"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="20"/>
+      <c r="A153" s="21"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="20"/>
+      <c r="A154" s="21"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="20"/>
+      <c r="A155" s="21"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="20"/>
+      <c r="A156" s="21"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="20"/>
+      <c r="A157" s="21"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="20"/>
+      <c r="A158" s="21"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="20"/>
+      <c r="A159" s="21"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="20"/>
+      <c r="A160" s="21"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="20"/>
+      <c r="A161" s="21"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="20"/>
+      <c r="A162" s="21"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="20"/>
+      <c r="A163" s="21"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="20"/>
+      <c r="A164" s="21"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="20"/>
+      <c r="A165" s="21"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="20"/>
+      <c r="A166" s="21"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="20"/>
+      <c r="A167" s="21"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="20"/>
+      <c r="A168" s="21"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="20"/>
+      <c r="A169" s="21"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="20"/>
+      <c r="A170" s="21"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="20"/>
+      <c r="A171" s="21"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="20"/>
+      <c r="A172" s="21"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="20"/>
+      <c r="A173" s="21"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="20"/>
+      <c r="A174" s="21"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="20"/>
+      <c r="A175" s="21"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="20"/>
+      <c r="A176" s="21"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="20"/>
+      <c r="A177" s="21"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="20"/>
+      <c r="A178" s="21"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="20"/>
+      <c r="A179" s="21"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="20"/>
+      <c r="A180" s="21"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="20"/>
+      <c r="A181" s="21"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="20"/>
+      <c r="A182" s="21"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="20"/>
+      <c r="A183" s="21"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="20"/>
+      <c r="A184" s="21"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="20"/>
+      <c r="A185" s="21"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="20"/>
+      <c r="A186" s="21"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="20"/>
+      <c r="A187" s="21"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="20"/>
+      <c r="A188" s="21"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="20"/>
+      <c r="A189" s="21"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="20"/>
+      <c r="A190" s="21"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="20"/>
+      <c r="A191" s="21"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="20"/>
+      <c r="A192" s="21"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="20"/>
+      <c r="A193" s="21"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="20"/>
+      <c r="A194" s="21"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="20"/>
+      <c r="A195" s="21"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="20"/>
+      <c r="A196" s="21"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="20"/>
+      <c r="A197" s="21"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="20"/>
+      <c r="A198" s="21"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="20"/>
+      <c r="A199" s="21"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="20"/>
+      <c r="A200" s="21"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="20"/>
+      <c r="A201" s="21"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="20"/>
+      <c r="A202" s="21"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="20"/>
+      <c r="A203" s="21"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="20"/>
+      <c r="A204" s="21"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="20"/>
+      <c r="A205" s="21"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="20"/>
+      <c r="A206" s="21"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="20"/>
+      <c r="A207" s="21"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="20"/>
+      <c r="A208" s="21"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="20"/>
+      <c r="A209" s="21"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="20"/>
+      <c r="A210" s="21"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="20"/>
+      <c r="A211" s="21"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="20"/>
+      <c r="A212" s="21"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="20"/>
+      <c r="A213" s="21"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="20"/>
+      <c r="A214" s="21"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="20"/>
+      <c r="A215" s="21"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="20"/>
+      <c r="A216" s="21"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="20"/>
+      <c r="A217" s="21"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="20"/>
+      <c r="A218" s="21"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="20"/>
+      <c r="A219" s="21"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="20"/>
+      <c r="A220" s="21"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="20"/>
+      <c r="A221" s="21"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="20"/>
+      <c r="A222" s="21"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="20"/>
+      <c r="A223" s="21"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="20"/>
+      <c r="A224" s="21"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="20"/>
+      <c r="A225" s="21"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="20"/>
+      <c r="A226" s="21"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="20"/>
+      <c r="A227" s="21"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="20"/>
+      <c r="A228" s="21"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="20"/>
+      <c r="A229" s="21"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="20"/>
+      <c r="A230" s="21"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="20"/>
+      <c r="A231" s="21"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="20"/>
+      <c r="A232" s="21"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="20"/>
+      <c r="A233" s="21"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="20"/>
+      <c r="A234" s="21"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="20"/>
+      <c r="A235" s="21"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="20"/>
+      <c r="A236" s="21"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="20"/>
+      <c r="A237" s="21"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="20"/>
+      <c r="A238" s="21"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="20"/>
+      <c r="A239" s="21"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="20"/>
+      <c r="A240" s="21"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="20"/>
+      <c r="A241" s="21"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="20"/>
+      <c r="A242" s="21"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="20"/>
+      <c r="A243" s="21"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="20"/>
+      <c r="A244" s="21"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="20"/>
+      <c r="A245" s="21"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="20"/>
+      <c r="A246" s="21"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="20"/>
+      <c r="A247" s="21"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="20"/>
+      <c r="A248" s="21"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="20"/>
+      <c r="A249" s="21"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="20"/>
+      <c r="A250" s="21"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="20"/>
+      <c r="A251" s="21"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="20"/>
+      <c r="A252" s="21"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="20"/>
+      <c r="A253" s="21"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="20"/>
+      <c r="A254" s="21"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="20"/>
+      <c r="A255" s="21"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="20"/>
+      <c r="A256" s="21"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="20"/>
+      <c r="A257" s="21"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="20"/>
+      <c r="A258" s="21"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="20"/>
+      <c r="A259" s="21"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="20"/>
+      <c r="A260" s="21"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="20"/>
+      <c r="A261" s="21"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="20"/>
+      <c r="A262" s="21"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="20"/>
+      <c r="A263" s="21"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="20"/>
+      <c r="A264" s="21"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="20"/>
+      <c r="A265" s="21"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="20"/>
+      <c r="A266" s="21"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="20"/>
+      <c r="A267" s="21"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="20"/>
+      <c r="A268" s="21"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="20"/>
+      <c r="A269" s="21"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="20"/>
+      <c r="A270" s="21"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="20"/>
+      <c r="A271" s="21"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="20"/>
+      <c r="A272" s="21"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="20"/>
+      <c r="A273" s="21"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="20"/>
+      <c r="A274" s="21"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="20"/>
+      <c r="A275" s="21"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="20"/>
+      <c r="A276" s="21"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="20"/>
+      <c r="A277" s="21"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="20"/>
+      <c r="A278" s="21"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="20"/>
+      <c r="A279" s="21"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="20"/>
+      <c r="A280" s="21"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="20"/>
+      <c r="A281" s="21"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="20"/>
+      <c r="A282" s="21"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="20"/>
+      <c r="A283" s="21"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="20"/>
+      <c r="A284" s="21"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="20"/>
+      <c r="A285" s="21"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="20"/>
+      <c r="A286" s="21"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="20"/>
+      <c r="A287" s="21"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="20"/>
+      <c r="A288" s="21"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="20"/>
+      <c r="A289" s="21"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="20"/>
+      <c r="A290" s="21"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="20"/>
+      <c r="A291" s="21"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="20"/>
+      <c r="A292" s="21"/>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="20"/>
+      <c r="A293" s="21"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="20"/>
+      <c r="A294" s="21"/>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="20"/>
+      <c r="A295" s="21"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="20"/>
+      <c r="A296" s="21"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="20"/>
+      <c r="A297" s="21"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="20"/>
+      <c r="A298" s="21"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="20"/>
+      <c r="A299" s="21"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="20"/>
+      <c r="A300" s="21"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="20"/>
+      <c r="A301" s="21"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="20"/>
+      <c r="A302" s="21"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="20"/>
+      <c r="A303" s="21"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="20"/>
+      <c r="A304" s="21"/>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="20"/>
+      <c r="A305" s="21"/>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="20"/>
+      <c r="A306" s="21"/>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="20"/>
+      <c r="A307" s="21"/>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="20"/>
+      <c r="A308" s="21"/>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="20"/>
+      <c r="A309" s="21"/>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="20"/>
+      <c r="A310" s="21"/>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="20"/>
+      <c r="A311" s="21"/>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="20"/>
+      <c r="A312" s="21"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="20"/>
+      <c r="A313" s="21"/>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="20"/>
+      <c r="A314" s="21"/>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="20"/>
+      <c r="A315" s="21"/>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="20"/>
+      <c r="A316" s="21"/>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="20"/>
+      <c r="A317" s="21"/>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="20"/>
+      <c r="A318" s="21"/>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="20"/>
+      <c r="A319" s="21"/>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="20"/>
+      <c r="A320" s="21"/>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="20"/>
+      <c r="A321" s="21"/>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="20"/>
+      <c r="A322" s="21"/>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="20"/>
+      <c r="A323" s="21"/>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="20"/>
+      <c r="A324" s="21"/>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="20"/>
+      <c r="A325" s="21"/>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="20"/>
+      <c r="A326" s="21"/>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A327" s="20"/>
+      <c r="A327" s="21"/>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="20"/>
+      <c r="A328" s="21"/>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="20"/>
+      <c r="A329" s="21"/>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="20"/>
+      <c r="A330" s="21"/>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="20"/>
+      <c r="A331" s="21"/>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="20"/>
+      <c r="A332" s="21"/>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A333" s="20"/>
+      <c r="A333" s="21"/>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A334" s="20"/>
+      <c r="A334" s="21"/>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="20"/>
+      <c r="A335" s="21"/>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="20"/>
+      <c r="A336" s="21"/>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="20"/>
+      <c r="A337" s="21"/>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="20"/>
+      <c r="A338" s="21"/>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="20"/>
+      <c r="A339" s="21"/>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A340" s="20"/>
+      <c r="A340" s="21"/>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="20"/>
+      <c r="A341" s="21"/>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="20"/>
+      <c r="A342" s="21"/>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A343" s="20"/>
+      <c r="A343" s="21"/>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A344" s="20"/>
+      <c r="A344" s="21"/>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A345" s="20"/>
+      <c r="A345" s="21"/>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="20"/>
+      <c r="A346" s="21"/>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A347" s="20"/>
+      <c r="A347" s="21"/>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A348" s="20"/>
+      <c r="A348" s="21"/>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="20"/>
+      <c r="A349" s="21"/>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="20"/>
+      <c r="A350" s="21"/>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="20"/>
+      <c r="A351" s="21"/>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="20"/>
+      <c r="A352" s="21"/>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="20"/>
+      <c r="A353" s="21"/>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="20"/>
+      <c r="A354" s="21"/>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="20"/>
+      <c r="A355" s="21"/>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="20"/>
+      <c r="A356" s="21"/>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="20"/>
+      <c r="A357" s="21"/>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="20"/>
+      <c r="A358" s="21"/>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="20"/>
+      <c r="A359" s="21"/>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="20"/>
+      <c r="A360" s="21"/>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="20"/>
+      <c r="A361" s="21"/>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="20"/>
+      <c r="A362" s="21"/>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A363" s="20"/>
+      <c r="A363" s="21"/>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A364" s="20"/>
+      <c r="A364" s="21"/>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A365" s="20"/>
+      <c r="A365" s="21"/>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A366" s="20"/>
+      <c r="A366" s="21"/>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A367" s="20"/>
+      <c r="A367" s="21"/>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A368" s="20"/>
+      <c r="A368" s="21"/>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A369" s="20"/>
+      <c r="A369" s="21"/>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A370" s="20"/>
+      <c r="A370" s="21"/>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A371" s="20"/>
+      <c r="A371" s="21"/>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A372" s="20"/>
+      <c r="A372" s="21"/>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A373" s="20"/>
+      <c r="A373" s="21"/>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="20"/>
+      <c r="A374" s="21"/>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A375" s="20"/>
+      <c r="A375" s="21"/>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A376" s="20"/>
+      <c r="A376" s="21"/>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A377" s="20"/>
+      <c r="A377" s="21"/>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A378" s="20"/>
+      <c r="A378" s="21"/>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A379" s="20"/>
+      <c r="A379" s="21"/>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A380" s="20"/>
+      <c r="A380" s="21"/>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A381" s="20"/>
+      <c r="A381" s="21"/>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A382" s="20"/>
+      <c r="A382" s="21"/>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="20"/>
+      <c r="A383" s="21"/>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A384" s="20"/>
+      <c r="A384" s="21"/>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A385" s="20"/>
+      <c r="A385" s="21"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A386" s="20"/>
+      <c r="A386" s="21"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="20"/>
+      <c r="A387" s="21"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A388" s="20"/>
+      <c r="A388" s="21"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="20"/>
+      <c r="A389" s="21"/>
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A390" s="20"/>
+      <c r="A390" s="21"/>
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="20"/>
+      <c r="A391" s="21"/>
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A392" s="20"/>
+      <c r="A392" s="21"/>
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A393" s="20"/>
+      <c r="A393" s="21"/>
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A394" s="20"/>
+      <c r="A394" s="21"/>
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A395" s="20"/>
+      <c r="A395" s="21"/>
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="20"/>
+      <c r="A396" s="21"/>
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A397" s="20"/>
+      <c r="A397" s="21"/>
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A398" s="20"/>
+      <c r="A398" s="21"/>
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A399" s="20"/>
+      <c r="A399" s="21"/>
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A400" s="20"/>
+      <c r="A400" s="21"/>
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A401" s="20"/>
+      <c r="A401" s="21"/>
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A402" s="20"/>
+      <c r="A402" s="21"/>
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="20"/>
+      <c r="A403" s="21"/>
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A404" s="20"/>
+      <c r="A404" s="21"/>
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="20"/>
+      <c r="A405" s="21"/>
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A406" s="20"/>
+      <c r="A406" s="21"/>
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A407" s="20"/>
+      <c r="A407" s="21"/>
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A408" s="20"/>
+      <c r="A408" s="21"/>
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="20"/>
+      <c r="A409" s="21"/>
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="20"/>
+      <c r="A410" s="21"/>
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="20"/>
+      <c r="A411" s="21"/>
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A412" s="20"/>
+      <c r="A412" s="21"/>
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="20"/>
+      <c r="A413" s="21"/>
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A414" s="20"/>
+      <c r="A414" s="21"/>
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A415" s="20"/>
+      <c r="A415" s="21"/>
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A416" s="20"/>
+      <c r="A416" s="21"/>
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A417" s="20"/>
+      <c r="A417" s="21"/>
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="20"/>
+      <c r="A418" s="21"/>
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A419" s="20"/>
+      <c r="A419" s="21"/>
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="20"/>
+      <c r="A420" s="21"/>
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A421" s="20"/>
+      <c r="A421" s="21"/>
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A422" s="20"/>
+      <c r="A422" s="21"/>
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="20"/>
+      <c r="A423" s="21"/>
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A424" s="20"/>
+      <c r="A424" s="21"/>
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A425" s="20"/>
+      <c r="A425" s="21"/>
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A426" s="20"/>
+      <c r="A426" s="21"/>
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A427" s="20"/>
+      <c r="A427" s="21"/>
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A428" s="20"/>
+      <c r="A428" s="21"/>
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="20"/>
+      <c r="A429" s="21"/>
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A430" s="20"/>
+      <c r="A430" s="21"/>
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="20"/>
+      <c r="A431" s="21"/>
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="20"/>
+      <c r="A432" s="21"/>
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="20"/>
+      <c r="A433" s="21"/>
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="20"/>
+      <c r="A434" s="21"/>
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="20"/>
+      <c r="A435" s="21"/>
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="20"/>
+      <c r="A436" s="21"/>
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="20"/>
+      <c r="A437" s="21"/>
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A438" s="20"/>
+      <c r="A438" s="21"/>
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A439" s="20"/>
+      <c r="A439" s="21"/>
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="20"/>
+      <c r="A440" s="21"/>
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="20"/>
+      <c r="A441" s="21"/>
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A442" s="20"/>
+      <c r="A442" s="21"/>
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="20"/>
+      <c r="A443" s="21"/>
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A444" s="20"/>
+      <c r="A444" s="21"/>
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A445" s="20"/>
+      <c r="A445" s="21"/>
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A446" s="20"/>
+      <c r="A446" s="21"/>
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A447" s="20"/>
+      <c r="A447" s="21"/>
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A448" s="20"/>
+      <c r="A448" s="21"/>
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="20"/>
+      <c r="A449" s="21"/>
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A450" s="20"/>
+      <c r="A450" s="21"/>
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A451" s="20"/>
+      <c r="A451" s="21"/>
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A452" s="20"/>
+      <c r="A452" s="21"/>
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A453" s="20"/>
+      <c r="A453" s="21"/>
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A454" s="20"/>
+      <c r="A454" s="21"/>
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A455" s="20"/>
+      <c r="A455" s="21"/>
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A456" s="20"/>
+      <c r="A456" s="21"/>
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A457" s="20"/>
+      <c r="A457" s="21"/>
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A458" s="20"/>
+      <c r="A458" s="21"/>
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A459" s="20"/>
+      <c r="A459" s="21"/>
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A460" s="20"/>
+      <c r="A460" s="21"/>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A461" s="20"/>
+      <c r="A461" s="21"/>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A462" s="20"/>
+      <c r="A462" s="21"/>
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A463" s="20"/>
+      <c r="A463" s="21"/>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A464" s="20"/>
+      <c r="A464" s="21"/>
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A465" s="20"/>
+      <c r="A465" s="21"/>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A466" s="20"/>
+      <c r="A466" s="21"/>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A467" s="20"/>
+      <c r="A467" s="21"/>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A468" s="20"/>
+      <c r="A468" s="21"/>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A469" s="20"/>
+      <c r="A469" s="21"/>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A470" s="20"/>
+      <c r="A470" s="21"/>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A471" s="20"/>
+      <c r="A471" s="21"/>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A472" s="20"/>
+      <c r="A472" s="21"/>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A473" s="20"/>
+      <c r="A473" s="21"/>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A474" s="20"/>
+      <c r="A474" s="21"/>
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="20"/>
+      <c r="A475" s="21"/>
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A476" s="20"/>
+      <c r="A476" s="21"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A477" s="20"/>
+      <c r="A477" s="21"/>
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A478" s="20"/>
+      <c r="A478" s="21"/>
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A479" s="20"/>
+      <c r="A479" s="21"/>
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A480" s="20"/>
+      <c r="A480" s="21"/>
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A481" s="20"/>
+      <c r="A481" s="21"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="20"/>
+      <c r="A482" s="21"/>
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A483" s="20"/>
+      <c r="A483" s="21"/>
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A484" s="20"/>
+      <c r="A484" s="21"/>
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A485" s="20"/>
+      <c r="A485" s="21"/>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A486" s="20"/>
+      <c r="A486" s="21"/>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A487" s="20"/>
+      <c r="A487" s="21"/>
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A488" s="20"/>
+      <c r="A488" s="21"/>
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A489" s="20"/>
+      <c r="A489" s="21"/>
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A490" s="20"/>
+      <c r="A490" s="21"/>
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A491" s="20"/>
+      <c r="A491" s="21"/>
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A492" s="20"/>
+      <c r="A492" s="21"/>
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A493" s="20"/>
+      <c r="A493" s="21"/>
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A494" s="20"/>
+      <c r="A494" s="21"/>
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A495" s="20"/>
+      <c r="A495" s="21"/>
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A496" s="20"/>
+      <c r="A496" s="21"/>
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A497" s="20"/>
+      <c r="A497" s="21"/>
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A498" s="20"/>
+      <c r="A498" s="21"/>
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A499" s="20"/>
+      <c r="A499" s="21"/>
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A500" s="20"/>
+      <c r="A500" s="21"/>
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A501" s="20"/>
+      <c r="A501" s="21"/>
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A502" s="20"/>
+      <c r="A502" s="21"/>
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A503" s="20"/>
+      <c r="A503" s="21"/>
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A504" s="20"/>
+      <c r="A504" s="21"/>
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A505" s="20"/>
+      <c r="A505" s="21"/>
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A506" s="20"/>
+      <c r="A506" s="21"/>
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A507" s="20"/>
+      <c r="A507" s="21"/>
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A508" s="20"/>
+      <c r="A508" s="21"/>
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A509" s="20"/>
+      <c r="A509" s="21"/>
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A510" s="20"/>
+      <c r="A510" s="21"/>
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A511" s="20"/>
+      <c r="A511" s="21"/>
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A512" s="20"/>
+      <c r="A512" s="21"/>
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A513" s="20"/>
+      <c r="A513" s="21"/>
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A514" s="20"/>
+      <c r="A514" s="21"/>
     </row>
     <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A515" s="20"/>
+      <c r="A515" s="21"/>
     </row>
     <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A516" s="20"/>
+      <c r="A516" s="21"/>
     </row>
     <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A517" s="20"/>
+      <c r="A517" s="21"/>
     </row>
     <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A518" s="20"/>
+      <c r="A518" s="21"/>
     </row>
     <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A519" s="20"/>
+      <c r="A519" s="21"/>
     </row>
     <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A520" s="20"/>
+      <c r="A520" s="21"/>
     </row>
     <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A521" s="20"/>
+      <c r="A521" s="21"/>
     </row>
     <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A522" s="20"/>
+      <c r="A522" s="21"/>
     </row>
     <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A523" s="20"/>
+      <c r="A523" s="21"/>
     </row>
     <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A524" s="20"/>
+      <c r="A524" s="21"/>
     </row>
     <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A525" s="20"/>
+      <c r="A525" s="21"/>
     </row>
     <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A526" s="20"/>
+      <c r="A526" s="21"/>
     </row>
     <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A527" s="20"/>
+      <c r="A527" s="21"/>
     </row>
     <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A528" s="20"/>
+      <c r="A528" s="21"/>
     </row>
     <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A529" s="20"/>
+      <c r="A529" s="21"/>
     </row>
     <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A530" s="20"/>
+      <c r="A530" s="21"/>
     </row>
     <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A531" s="20"/>
+      <c r="A531" s="21"/>
     </row>
     <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A532" s="20"/>
+      <c r="A532" s="21"/>
     </row>
     <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A533" s="20"/>
+      <c r="A533" s="21"/>
     </row>
     <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A534" s="20"/>
+      <c r="A534" s="21"/>
     </row>
     <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A535" s="20"/>
+      <c r="A535" s="21"/>
     </row>
     <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A536" s="20"/>
+      <c r="A536" s="21"/>
     </row>
     <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A537" s="20"/>
+      <c r="A537" s="21"/>
     </row>
     <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A538" s="20"/>
+      <c r="A538" s="21"/>
     </row>
     <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A539" s="20"/>
+      <c r="A539" s="21"/>
     </row>
     <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A540" s="20"/>
+      <c r="A540" s="21"/>
     </row>
     <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A541" s="20"/>
+      <c r="A541" s="21"/>
     </row>
     <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A542" s="20"/>
+      <c r="A542" s="21"/>
     </row>
     <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A543" s="20"/>
+      <c r="A543" s="21"/>
     </row>
     <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A544" s="20"/>
+      <c r="A544" s="21"/>
     </row>
     <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A545" s="20"/>
+      <c r="A545" s="21"/>
     </row>
     <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A546" s="20"/>
+      <c r="A546" s="21"/>
     </row>
     <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A547" s="20"/>
+      <c r="A547" s="21"/>
     </row>
     <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A548" s="20"/>
+      <c r="A548" s="21"/>
     </row>
     <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A549" s="20"/>
+      <c r="A549" s="21"/>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A550" s="20"/>
+      <c r="A550" s="21"/>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A551" s="20"/>
+      <c r="A551" s="21"/>
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A552" s="20"/>
+      <c r="A552" s="21"/>
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A553" s="20"/>
+      <c r="A553" s="21"/>
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A554" s="20"/>
+      <c r="A554" s="21"/>
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A555" s="20"/>
+      <c r="A555" s="21"/>
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A556" s="20"/>
+      <c r="A556" s="21"/>
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A557" s="20"/>
+      <c r="A557" s="21"/>
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A558" s="20"/>
+      <c r="A558" s="21"/>
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A559" s="20"/>
+      <c r="A559" s="21"/>
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A560" s="20"/>
+      <c r="A560" s="21"/>
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A561" s="20"/>
+      <c r="A561" s="21"/>
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A562" s="20"/>
+      <c r="A562" s="21"/>
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A563" s="20"/>
+      <c r="A563" s="21"/>
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A564" s="20"/>
+      <c r="A564" s="21"/>
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A565" s="20"/>
+      <c r="A565" s="21"/>
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A566" s="20"/>
+      <c r="A566" s="21"/>
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A567" s="20"/>
+      <c r="A567" s="21"/>
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A568" s="20"/>
+      <c r="A568" s="21"/>
     </row>
     <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A569" s="20"/>
+      <c r="A569" s="21"/>
     </row>
     <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A570" s="20"/>
+      <c r="A570" s="21"/>
     </row>
     <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A571" s="20"/>
+      <c r="A571" s="21"/>
     </row>
     <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A572" s="20"/>
+      <c r="A572" s="21"/>
     </row>
     <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A573" s="20"/>
+      <c r="A573" s="21"/>
     </row>
     <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A574" s="20"/>
+      <c r="A574" s="21"/>
     </row>
     <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A575" s="20"/>
+      <c r="A575" s="21"/>
     </row>
     <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A576" s="20"/>
+      <c r="A576" s="21"/>
     </row>
     <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A577" s="20"/>
+      <c r="A577" s="21"/>
     </row>
     <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A578" s="20"/>
+      <c r="A578" s="21"/>
     </row>
     <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A579" s="20"/>
+      <c r="A579" s="21"/>
     </row>
     <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A580" s="20"/>
+      <c r="A580" s="21"/>
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A581" s="20"/>
+      <c r="A581" s="21"/>
     </row>
     <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A582" s="20"/>
+      <c r="A582" s="21"/>
     </row>
     <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A583" s="20"/>
+      <c r="A583" s="21"/>
     </row>
     <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A584" s="20"/>
+      <c r="A584" s="21"/>
     </row>
     <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A585" s="20"/>
+      <c r="A585" s="21"/>
     </row>
     <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A586" s="20"/>
+      <c r="A586" s="21"/>
     </row>
     <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A587" s="20"/>
+      <c r="A587" s="21"/>
     </row>
     <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A588" s="20"/>
+      <c r="A588" s="21"/>
     </row>
     <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A589" s="20"/>
+      <c r="A589" s="21"/>
     </row>
     <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A590" s="20"/>
+      <c r="A590" s="21"/>
     </row>
     <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A591" s="20"/>
+      <c r="A591" s="21"/>
     </row>
     <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A592" s="20"/>
+      <c r="A592" s="21"/>
     </row>
     <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A593" s="20"/>
+      <c r="A593" s="21"/>
     </row>
     <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A594" s="20"/>
+      <c r="A594" s="21"/>
     </row>
     <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A595" s="20"/>
+      <c r="A595" s="21"/>
     </row>
     <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A596" s="20"/>
+      <c r="A596" s="21"/>
     </row>
     <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A597" s="20"/>
+      <c r="A597" s="21"/>
     </row>
     <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A598" s="20"/>
+      <c r="A598" s="21"/>
     </row>
     <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A599" s="20"/>
+      <c r="A599" s="21"/>
     </row>
     <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A600" s="20"/>
+      <c r="A600" s="21"/>
     </row>
     <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A601" s="20"/>
+      <c r="A601" s="21"/>
     </row>
     <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A602" s="20"/>
+      <c r="A602" s="21"/>
     </row>
     <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A603" s="20"/>
+      <c r="A603" s="21"/>
     </row>
     <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A604" s="20"/>
+      <c r="A604" s="21"/>
     </row>
     <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A605" s="20"/>
+      <c r="A605" s="21"/>
     </row>
     <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A606" s="20"/>
+      <c r="A606" s="21"/>
     </row>
     <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A607" s="20"/>
+      <c r="A607" s="21"/>
     </row>
     <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A608" s="20"/>
+      <c r="A608" s="21"/>
     </row>
     <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A609" s="20"/>
+      <c r="A609" s="21"/>
     </row>
     <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A610" s="20"/>
+      <c r="A610" s="21"/>
     </row>
     <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A611" s="20"/>
+      <c r="A611" s="21"/>
     </row>
     <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A612" s="20"/>
+      <c r="A612" s="21"/>
     </row>
     <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A613" s="20"/>
+      <c r="A613" s="21"/>
     </row>
     <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A614" s="20"/>
+      <c r="A614" s="21"/>
     </row>
     <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A615" s="20"/>
+      <c r="A615" s="21"/>
     </row>
     <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A616" s="20"/>
+      <c r="A616" s="21"/>
     </row>
     <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A617" s="20"/>
+      <c r="A617" s="21"/>
     </row>
     <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A618" s="20"/>
+      <c r="A618" s="21"/>
     </row>
     <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A619" s="20"/>
+      <c r="A619" s="21"/>
     </row>
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A620" s="20"/>
+      <c r="A620" s="21"/>
     </row>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A621" s="20"/>
+      <c r="A621" s="21"/>
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A622" s="20"/>
+      <c r="A622" s="21"/>
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A623" s="20"/>
+      <c r="A623" s="21"/>
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A624" s="20"/>
+      <c r="A624" s="21"/>
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A625" s="20"/>
+      <c r="A625" s="21"/>
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A626" s="20"/>
+      <c r="A626" s="21"/>
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A627" s="20"/>
+      <c r="A627" s="21"/>
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A628" s="20"/>
+      <c r="A628" s="21"/>
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A629" s="20"/>
+      <c r="A629" s="21"/>
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A630" s="20"/>
+      <c r="A630" s="21"/>
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A631" s="20"/>
+      <c r="A631" s="21"/>
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A632" s="20"/>
+      <c r="A632" s="21"/>
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A633" s="20"/>
+      <c r="A633" s="21"/>
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A634" s="20"/>
+      <c r="A634" s="21"/>
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A635" s="20"/>
+      <c r="A635" s="21"/>
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A636" s="20"/>
+      <c r="A636" s="21"/>
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A637" s="20"/>
+      <c r="A637" s="21"/>
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A638" s="20"/>
+      <c r="A638" s="21"/>
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A639" s="20"/>
+      <c r="A639" s="21"/>
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A640" s="20"/>
+      <c r="A640" s="21"/>
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A641" s="20"/>
+      <c r="A641" s="21"/>
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A642" s="20"/>
+      <c r="A642" s="21"/>
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A643" s="20"/>
+      <c r="A643" s="21"/>
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A644" s="20"/>
+      <c r="A644" s="21"/>
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A645" s="20"/>
+      <c r="A645" s="21"/>
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A646" s="20"/>
+      <c r="A646" s="21"/>
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A647" s="20"/>
+      <c r="A647" s="21"/>
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A648" s="20"/>
+      <c r="A648" s="21"/>
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A649" s="20"/>
+      <c r="A649" s="21"/>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A650" s="20"/>
+      <c r="A650" s="21"/>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A651" s="20"/>
+      <c r="A651" s="21"/>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A652" s="20"/>
+      <c r="A652" s="21"/>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A653" s="20"/>
+      <c r="A653" s="21"/>
     </row>
     <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A654" s="20"/>
+      <c r="A654" s="21"/>
     </row>
     <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A655" s="20"/>
+      <c r="A655" s="21"/>
     </row>
     <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A656" s="20"/>
+      <c r="A656" s="21"/>
     </row>
     <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A657" s="20"/>
+      <c r="A657" s="21"/>
     </row>
     <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A658" s="20"/>
+      <c r="A658" s="21"/>
     </row>
     <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A659" s="20"/>
+      <c r="A659" s="21"/>
     </row>
     <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A660" s="20"/>
+      <c r="A660" s="21"/>
     </row>
     <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A661" s="20"/>
+      <c r="A661" s="21"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A662" s="20"/>
+      <c r="A662" s="21"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A663" s="20"/>
+      <c r="A663" s="21"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A664" s="20"/>
+      <c r="A664" s="21"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A665" s="20"/>
+      <c r="A665" s="21"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A666" s="20"/>
+      <c r="A666" s="21"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A667" s="20"/>
+      <c r="A667" s="21"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A668" s="20"/>
+      <c r="A668" s="21"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A669" s="20"/>
+      <c r="A669" s="21"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A670" s="20"/>
+      <c r="A670" s="21"/>
     </row>
     <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A671" s="20"/>
+      <c r="A671" s="21"/>
     </row>
     <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A672" s="20"/>
+      <c r="A672" s="21"/>
     </row>
     <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A673" s="20"/>
+      <c r="A673" s="21"/>
     </row>
     <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A674" s="20"/>
+      <c r="A674" s="21"/>
     </row>
     <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A675" s="20"/>
+      <c r="A675" s="21"/>
     </row>
     <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A676" s="20"/>
+      <c r="A676" s="21"/>
     </row>
     <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A677" s="20"/>
+      <c r="A677" s="21"/>
     </row>
     <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A678" s="20"/>
+      <c r="A678" s="21"/>
     </row>
     <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A679" s="20"/>
+      <c r="A679" s="21"/>
     </row>
     <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A680" s="20"/>
+      <c r="A680" s="21"/>
     </row>
     <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A681" s="20"/>
+      <c r="A681" s="21"/>
     </row>
     <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A682" s="20"/>
+      <c r="A682" s="21"/>
     </row>
     <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A683" s="20"/>
+      <c r="A683" s="21"/>
     </row>
     <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A684" s="20"/>
+      <c r="A684" s="21"/>
     </row>
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A685" s="20"/>
+      <c r="A685" s="21"/>
     </row>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A686" s="20"/>
+      <c r="A686" s="21"/>
     </row>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A687" s="20"/>
+      <c r="A687" s="21"/>
     </row>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A688" s="20"/>
+      <c r="A688" s="21"/>
     </row>
     <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A689" s="20"/>
+      <c r="A689" s="21"/>
     </row>
     <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A690" s="20"/>
+      <c r="A690" s="21"/>
     </row>
     <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A691" s="20"/>
+      <c r="A691" s="21"/>
     </row>
     <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A692" s="20"/>
+      <c r="A692" s="21"/>
     </row>
     <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A693" s="20"/>
+      <c r="A693" s="21"/>
     </row>
     <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A694" s="20"/>
+      <c r="A694" s="21"/>
     </row>
     <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A695" s="20"/>
+      <c r="A695" s="21"/>
     </row>
     <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A696" s="20"/>
+      <c r="A696" s="21"/>
     </row>
     <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A697" s="20"/>
+      <c r="A697" s="21"/>
     </row>
     <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A698" s="20"/>
+      <c r="A698" s="21"/>
     </row>
     <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A699" s="20"/>
+      <c r="A699" s="21"/>
     </row>
     <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A700" s="20"/>
+      <c r="A700" s="21"/>
     </row>
     <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A701" s="20"/>
+      <c r="A701" s="21"/>
     </row>
     <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A702" s="20"/>
+      <c r="A702" s="21"/>
     </row>
     <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A703" s="20"/>
+      <c r="A703" s="21"/>
     </row>
     <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A704" s="20"/>
+      <c r="A704" s="21"/>
     </row>
     <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A705" s="20"/>
+      <c r="A705" s="21"/>
     </row>
     <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A706" s="20"/>
+      <c r="A706" s="21"/>
     </row>
     <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A707" s="20"/>
+      <c r="A707" s="21"/>
     </row>
     <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A708" s="20"/>
+      <c r="A708" s="21"/>
     </row>
     <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A709" s="20"/>
+      <c r="A709" s="21"/>
     </row>
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A710" s="20"/>
+      <c r="A710" s="21"/>
     </row>
     <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A711" s="20"/>
+      <c r="A711" s="21"/>
     </row>
     <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A712" s="20"/>
+      <c r="A712" s="21"/>
     </row>
     <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A713" s="20"/>
+      <c r="A713" s="21"/>
     </row>
     <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A714" s="20"/>
+      <c r="A714" s="21"/>
     </row>
     <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A715" s="20"/>
+      <c r="A715" s="21"/>
     </row>
     <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A716" s="20"/>
+      <c r="A716" s="21"/>
     </row>
     <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A717" s="20"/>
+      <c r="A717" s="21"/>
     </row>
     <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A718" s="20"/>
+      <c r="A718" s="21"/>
     </row>
     <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A719" s="20"/>
+      <c r="A719" s="21"/>
     </row>
     <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A720" s="20"/>
+      <c r="A720" s="21"/>
     </row>
     <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A721" s="20"/>
+      <c r="A721" s="21"/>
     </row>
     <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A722" s="20"/>
+      <c r="A722" s="21"/>
     </row>
     <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A723" s="20"/>
+      <c r="A723" s="21"/>
     </row>
     <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A724" s="20"/>
+      <c r="A724" s="21"/>
     </row>
     <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A725" s="20"/>
+      <c r="A725" s="21"/>
     </row>
     <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A726" s="20"/>
+      <c r="A726" s="21"/>
     </row>
     <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A727" s="20"/>
+      <c r="A727" s="21"/>
     </row>
     <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A728" s="20"/>
+      <c r="A728" s="21"/>
     </row>
     <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A729" s="20"/>
+      <c r="A729" s="21"/>
     </row>
     <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A730" s="20"/>
+      <c r="A730" s="21"/>
     </row>
     <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A731" s="20"/>
+      <c r="A731" s="21"/>
     </row>
     <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A732" s="20"/>
+      <c r="A732" s="21"/>
     </row>
     <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A733" s="20"/>
+      <c r="A733" s="21"/>
     </row>
     <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A734" s="20"/>
+      <c r="A734" s="21"/>
     </row>
     <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A735" s="20"/>
+      <c r="A735" s="21"/>
     </row>
     <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A736" s="20"/>
+      <c r="A736" s="21"/>
     </row>
     <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A737" s="20"/>
+      <c r="A737" s="21"/>
     </row>
     <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A738" s="20"/>
+      <c r="A738" s="21"/>
     </row>
     <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A739" s="20"/>
+      <c r="A739" s="21"/>
     </row>
     <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A740" s="20"/>
+      <c r="A740" s="21"/>
     </row>
     <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A741" s="20"/>
+      <c r="A741" s="21"/>
     </row>
     <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A742" s="20"/>
+      <c r="A742" s="21"/>
     </row>
     <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A743" s="20"/>
+      <c r="A743" s="21"/>
     </row>
     <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A744" s="20"/>
+      <c r="A744" s="21"/>
     </row>
     <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A745" s="20"/>
+      <c r="A745" s="21"/>
     </row>
     <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A746" s="20"/>
+      <c r="A746" s="21"/>
     </row>
     <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A747" s="20"/>
+      <c r="A747" s="21"/>
     </row>
     <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A748" s="20"/>
+      <c r="A748" s="21"/>
     </row>
     <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A749" s="20"/>
+      <c r="A749" s="21"/>
     </row>
     <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A750" s="20"/>
+      <c r="A750" s="21"/>
     </row>
     <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A751" s="20"/>
+      <c r="A751" s="21"/>
     </row>
     <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A752" s="20"/>
+      <c r="A752" s="21"/>
     </row>
     <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A753" s="20"/>
+      <c r="A753" s="21"/>
     </row>
     <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A754" s="20"/>
+      <c r="A754" s="21"/>
     </row>
     <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A755" s="20"/>
+      <c r="A755" s="21"/>
     </row>
     <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A756" s="20"/>
+      <c r="A756" s="21"/>
     </row>
     <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A757" s="20"/>
+      <c r="A757" s="21"/>
     </row>
     <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A758" s="20"/>
+      <c r="A758" s="21"/>
     </row>
     <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A759" s="20"/>
+      <c r="A759" s="21"/>
     </row>
     <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A760" s="20"/>
+      <c r="A760" s="21"/>
     </row>
     <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A761" s="20"/>
+      <c r="A761" s="21"/>
     </row>
     <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A762" s="20"/>
+      <c r="A762" s="21"/>
     </row>
     <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A763" s="20"/>
+      <c r="A763" s="21"/>
     </row>
     <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A764" s="20"/>
+      <c r="A764" s="21"/>
     </row>
     <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A765" s="20"/>
+      <c r="A765" s="21"/>
     </row>
     <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A766" s="20"/>
+      <c r="A766" s="21"/>
     </row>
     <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A767" s="20"/>
+      <c r="A767" s="21"/>
     </row>
     <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A768" s="20"/>
+      <c r="A768" s="21"/>
     </row>
     <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A769" s="20"/>
+      <c r="A769" s="21"/>
     </row>
     <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A770" s="20"/>
+      <c r="A770" s="21"/>
     </row>
     <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A771" s="20"/>
+      <c r="A771" s="21"/>
     </row>
     <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A772" s="20"/>
+      <c r="A772" s="21"/>
     </row>
     <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A773" s="20"/>
+      <c r="A773" s="21"/>
     </row>
     <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A774" s="20"/>
+      <c r="A774" s="21"/>
     </row>
     <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A775" s="20"/>
+      <c r="A775" s="21"/>
     </row>
     <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A776" s="20"/>
+      <c r="A776" s="21"/>
     </row>
     <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A777" s="20"/>
+      <c r="A777" s="21"/>
     </row>
     <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A778" s="20"/>
+      <c r="A778" s="21"/>
     </row>
     <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A779" s="20"/>
+      <c r="A779" s="21"/>
     </row>
     <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A780" s="20"/>
+      <c r="A780" s="21"/>
     </row>
     <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A781" s="20"/>
+      <c r="A781" s="21"/>
     </row>
     <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A782" s="20"/>
+      <c r="A782" s="21"/>
     </row>
     <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A783" s="20"/>
+      <c r="A783" s="21"/>
     </row>
     <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A784" s="20"/>
+      <c r="A784" s="21"/>
     </row>
     <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A785" s="20"/>
+      <c r="A785" s="21"/>
     </row>
     <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A786" s="20"/>
+      <c r="A786" s="21"/>
     </row>
     <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A787" s="20"/>
+      <c r="A787" s="21"/>
     </row>
     <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A788" s="20"/>
+      <c r="A788" s="21"/>
     </row>
     <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A789" s="20"/>
+      <c r="A789" s="21"/>
     </row>
     <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A790" s="20"/>
+      <c r="A790" s="21"/>
     </row>
     <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A791" s="20"/>
+      <c r="A791" s="21"/>
     </row>
     <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A792" s="20"/>
+      <c r="A792" s="21"/>
     </row>
     <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A793" s="20"/>
+      <c r="A793" s="21"/>
     </row>
     <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A794" s="20"/>
+      <c r="A794" s="21"/>
     </row>
     <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A795" s="20"/>
+      <c r="A795" s="21"/>
     </row>
     <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A796" s="20"/>
+      <c r="A796" s="21"/>
     </row>
     <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A797" s="20"/>
+      <c r="A797" s="21"/>
     </row>
     <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A798" s="20"/>
+      <c r="A798" s="21"/>
     </row>
     <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A799" s="20"/>
+      <c r="A799" s="21"/>
     </row>
     <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A800" s="20"/>
+      <c r="A800" s="21"/>
     </row>
     <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A801" s="20"/>
+      <c r="A801" s="21"/>
     </row>
     <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A802" s="20"/>
+      <c r="A802" s="21"/>
     </row>
     <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A803" s="20"/>
+      <c r="A803" s="21"/>
     </row>
     <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A804" s="20"/>
+      <c r="A804" s="21"/>
     </row>
     <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A805" s="20"/>
+      <c r="A805" s="21"/>
     </row>
     <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A806" s="20"/>
+      <c r="A806" s="21"/>
     </row>
     <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A807" s="20"/>
+      <c r="A807" s="21"/>
     </row>
     <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A808" s="20"/>
+      <c r="A808" s="21"/>
     </row>
     <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A809" s="20"/>
+      <c r="A809" s="21"/>
     </row>
     <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A810" s="20"/>
+      <c r="A810" s="21"/>
     </row>
     <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A811" s="20"/>
+      <c r="A811" s="21"/>
     </row>
     <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A812" s="20"/>
+      <c r="A812" s="21"/>
     </row>
     <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A813" s="20"/>
+      <c r="A813" s="21"/>
     </row>
     <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A814" s="20"/>
+      <c r="A814" s="21"/>
     </row>
     <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A815" s="20"/>
+      <c r="A815" s="21"/>
     </row>
     <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A816" s="20"/>
+      <c r="A816" s="21"/>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A817" s="20"/>
+      <c r="A817" s="21"/>
     </row>
     <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A818" s="20"/>
+      <c r="A818" s="21"/>
     </row>
     <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A819" s="20"/>
+      <c r="A819" s="21"/>
     </row>
     <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A820" s="20"/>
+      <c r="A820" s="21"/>
     </row>
     <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A821" s="20"/>
+      <c r="A821" s="21"/>
     </row>
     <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A822" s="20"/>
+      <c r="A822" s="21"/>
     </row>
     <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A823" s="20"/>
+      <c r="A823" s="21"/>
     </row>
     <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A824" s="20"/>
+      <c r="A824" s="21"/>
     </row>
     <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A825" s="20"/>
+      <c r="A825" s="21"/>
     </row>
     <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A826" s="20"/>
+      <c r="A826" s="21"/>
     </row>
     <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A827" s="20"/>
+      <c r="A827" s="21"/>
     </row>
     <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A828" s="20"/>
+      <c r="A828" s="21"/>
     </row>
     <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A829" s="20"/>
+      <c r="A829" s="21"/>
     </row>
     <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A830" s="20"/>
+      <c r="A830" s="21"/>
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A831" s="20"/>
+      <c r="A831" s="21"/>
     </row>
     <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A832" s="20"/>
+      <c r="A832" s="21"/>
     </row>
     <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A833" s="20"/>
+      <c r="A833" s="21"/>
     </row>
     <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A834" s="20"/>
+      <c r="A834" s="21"/>
     </row>
     <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A835" s="20"/>
+      <c r="A835" s="21"/>
     </row>
     <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A836" s="20"/>
+      <c r="A836" s="21"/>
     </row>
     <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A837" s="20"/>
+      <c r="A837" s="21"/>
     </row>
     <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A838" s="20"/>
+      <c r="A838" s="21"/>
     </row>
     <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A839" s="20"/>
+      <c r="A839" s="21"/>
     </row>
     <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A840" s="20"/>
+      <c r="A840" s="21"/>
     </row>
     <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A841" s="20"/>
+      <c r="A841" s="21"/>
     </row>
     <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A842" s="20"/>
+      <c r="A842" s="21"/>
     </row>
     <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A843" s="20"/>
+      <c r="A843" s="21"/>
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A844" s="20"/>
+      <c r="A844" s="21"/>
     </row>
     <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A845" s="20"/>
+      <c r="A845" s="21"/>
     </row>
     <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A846" s="20"/>
+      <c r="A846" s="21"/>
     </row>
     <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A847" s="20"/>
+      <c r="A847" s="21"/>
     </row>
     <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A848" s="20"/>
+      <c r="A848" s="21"/>
     </row>
     <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A849" s="20"/>
+      <c r="A849" s="21"/>
     </row>
     <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A850" s="20"/>
+      <c r="A850" s="21"/>
     </row>
     <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A851" s="20"/>
+      <c r="A851" s="21"/>
     </row>
     <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A852" s="20"/>
+      <c r="A852" s="21"/>
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A853" s="20"/>
+      <c r="A853" s="21"/>
     </row>
     <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A854" s="20"/>
+      <c r="A854" s="21"/>
     </row>
     <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A855" s="20"/>
+      <c r="A855" s="21"/>
     </row>
     <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A856" s="20"/>
+      <c r="A856" s="21"/>
     </row>
     <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A857" s="20"/>
+      <c r="A857" s="21"/>
     </row>
     <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A858" s="20"/>
+      <c r="A858" s="21"/>
     </row>
     <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A859" s="20"/>
+      <c r="A859" s="21"/>
     </row>
     <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A860" s="20"/>
+      <c r="A860" s="21"/>
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A861" s="20"/>
+      <c r="A861" s="21"/>
     </row>
     <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A862" s="20"/>
+      <c r="A862" s="21"/>
     </row>
     <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A863" s="20"/>
+      <c r="A863" s="21"/>
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A864" s="20"/>
+      <c r="A864" s="21"/>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A865" s="20"/>
+      <c r="A865" s="21"/>
     </row>
     <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A866" s="20"/>
+      <c r="A866" s="21"/>
     </row>
     <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A867" s="20"/>
+      <c r="A867" s="21"/>
     </row>
     <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A868" s="20"/>
+      <c r="A868" s="21"/>
     </row>
     <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A869" s="20"/>
+      <c r="A869" s="21"/>
     </row>
     <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A870" s="20"/>
+      <c r="A870" s="21"/>
     </row>
     <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A871" s="20"/>
+      <c r="A871" s="21"/>
     </row>
     <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A872" s="20"/>
+      <c r="A872" s="21"/>
     </row>
     <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A873" s="20"/>
+      <c r="A873" s="21"/>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A874" s="20"/>
+      <c r="A874" s="21"/>
     </row>
     <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A875" s="20"/>
+      <c r="A875" s="21"/>
     </row>
     <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A876" s="20"/>
+      <c r="A876" s="21"/>
     </row>
     <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A877" s="20"/>
+      <c r="A877" s="21"/>
     </row>
     <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A878" s="20"/>
+      <c r="A878" s="21"/>
     </row>
     <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A879" s="20"/>
+      <c r="A879" s="21"/>
     </row>
     <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A880" s="20"/>
+      <c r="A880" s="21"/>
     </row>
     <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A881" s="20"/>
+      <c r="A881" s="21"/>
     </row>
     <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A882" s="20"/>
+      <c r="A882" s="21"/>
     </row>
     <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A883" s="20"/>
+      <c r="A883" s="21"/>
     </row>
     <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A884" s="20"/>
+      <c r="A884" s="21"/>
     </row>
     <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A885" s="20"/>
+      <c r="A885" s="21"/>
     </row>
     <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A886" s="20"/>
+      <c r="A886" s="21"/>
     </row>
     <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A887" s="20"/>
+      <c r="A887" s="21"/>
     </row>
     <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A888" s="20"/>
+      <c r="A888" s="21"/>
     </row>
     <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A889" s="20"/>
+      <c r="A889" s="21"/>
     </row>
     <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A890" s="20"/>
+      <c r="A890" s="21"/>
     </row>
     <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A891" s="20"/>
+      <c r="A891" s="21"/>
     </row>
     <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A892" s="20"/>
+      <c r="A892" s="21"/>
     </row>
     <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A893" s="20"/>
+      <c r="A893" s="21"/>
     </row>
     <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A894" s="20"/>
+      <c r="A894" s="21"/>
     </row>
     <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A895" s="20"/>
+      <c r="A895" s="21"/>
     </row>
     <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A896" s="20"/>
+      <c r="A896" s="21"/>
     </row>
     <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A897" s="20"/>
+      <c r="A897" s="21"/>
     </row>
     <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A898" s="20"/>
+      <c r="A898" s="21"/>
     </row>
     <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A899" s="20"/>
+      <c r="A899" s="21"/>
     </row>
     <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A900" s="20"/>
+      <c r="A900" s="21"/>
     </row>
     <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A901" s="20"/>
+      <c r="A901" s="21"/>
     </row>
     <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A902" s="20"/>
+      <c r="A902" s="21"/>
     </row>
     <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A903" s="20"/>
+      <c r="A903" s="21"/>
     </row>
     <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A904" s="20"/>
+      <c r="A904" s="21"/>
     </row>
     <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A905" s="20"/>
+      <c r="A905" s="21"/>
     </row>
     <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A906" s="20"/>
+      <c r="A906" s="21"/>
     </row>
     <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A907" s="20"/>
+      <c r="A907" s="21"/>
     </row>
     <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A908" s="20"/>
+      <c r="A908" s="21"/>
     </row>
     <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A909" s="20"/>
+      <c r="A909" s="21"/>
     </row>
     <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A910" s="20"/>
+      <c r="A910" s="21"/>
     </row>
     <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A911" s="20"/>
+      <c r="A911" s="21"/>
     </row>
     <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A912" s="20"/>
+      <c r="A912" s="21"/>
     </row>
     <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A913" s="20"/>
+      <c r="A913" s="21"/>
     </row>
     <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A914" s="20"/>
+      <c r="A914" s="21"/>
     </row>
     <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A915" s="20"/>
+      <c r="A915" s="21"/>
     </row>
     <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A916" s="20"/>
+      <c r="A916" s="21"/>
     </row>
     <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A917" s="20"/>
+      <c r="A917" s="21"/>
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A918" s="20"/>
+      <c r="A918" s="21"/>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A919" s="20"/>
+      <c r="A919" s="21"/>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A920" s="20"/>
+      <c r="A920" s="21"/>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A921" s="20"/>
+      <c r="A921" s="21"/>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A922" s="20"/>
+      <c r="A922" s="21"/>
     </row>
     <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A923" s="20"/>
+      <c r="A923" s="21"/>
     </row>
     <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A924" s="20"/>
+      <c r="A924" s="21"/>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A925" s="20"/>
+      <c r="A925" s="21"/>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A926" s="20"/>
+      <c r="A926" s="21"/>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A927" s="20"/>
+      <c r="A927" s="21"/>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A928" s="20"/>
+      <c r="A928" s="21"/>
     </row>
     <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A929" s="20"/>
+      <c r="A929" s="21"/>
     </row>
     <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A930" s="20"/>
+      <c r="A930" s="21"/>
     </row>
     <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A931" s="20"/>
+      <c r="A931" s="21"/>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A932" s="20"/>
+      <c r="A932" s="21"/>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A933" s="20"/>
+      <c r="A933" s="21"/>
     </row>
     <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A934" s="20"/>
+      <c r="A934" s="21"/>
     </row>
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A935" s="20"/>
+      <c r="A935" s="21"/>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A936" s="20"/>
+      <c r="A936" s="21"/>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A937" s="20"/>
+      <c r="A937" s="21"/>
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A938" s="20"/>
+      <c r="A938" s="21"/>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A939" s="20"/>
+      <c r="A939" s="21"/>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A940" s="20"/>
+      <c r="A940" s="21"/>
     </row>
     <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A941" s="20"/>
+      <c r="A941" s="21"/>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A942" s="20"/>
+      <c r="A942" s="21"/>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A943" s="20"/>
+      <c r="A943" s="21"/>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A944" s="20"/>
+      <c r="A944" s="21"/>
     </row>
     <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A945" s="20"/>
+      <c r="A945" s="21"/>
     </row>
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A946" s="20"/>
+      <c r="A946" s="21"/>
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A947" s="20"/>
+      <c r="A947" s="21"/>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A948" s="20"/>
+      <c r="A948" s="21"/>
     </row>
     <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A949" s="20"/>
+      <c r="A949" s="21"/>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A950" s="20"/>
+      <c r="A950" s="21"/>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A951" s="20"/>
+      <c r="A951" s="21"/>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A952" s="20"/>
+      <c r="A952" s="21"/>
     </row>
     <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A953" s="20"/>
+      <c r="A953" s="21"/>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A954" s="20"/>
+      <c r="A954" s="21"/>
     </row>
     <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A955" s="20"/>
+      <c r="A955" s="21"/>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A956" s="20"/>
+      <c r="A956" s="21"/>
     </row>
     <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A957" s="20"/>
+      <c r="A957" s="21"/>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A958" s="20"/>
+      <c r="A958" s="21"/>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A959" s="20"/>
+      <c r="A959" s="21"/>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A960" s="20"/>
+      <c r="A960" s="21"/>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A961" s="20"/>
+      <c r="A961" s="21"/>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A962" s="20"/>
+      <c r="A962" s="21"/>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A963" s="20"/>
+      <c r="A963" s="21"/>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A964" s="20"/>
+      <c r="A964" s="21"/>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A965" s="20"/>
+      <c r="A965" s="21"/>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A966" s="20"/>
+      <c r="A966" s="21"/>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A967" s="20"/>
+      <c r="A967" s="21"/>
     </row>
     <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A968" s="20"/>
+      <c r="A968" s="21"/>
     </row>
     <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A969" s="20"/>
+      <c r="A969" s="21"/>
     </row>
     <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A970" s="20"/>
+      <c r="A970" s="21"/>
     </row>
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A971" s="20"/>
+      <c r="A971" s="21"/>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A972" s="20"/>
+      <c r="A972" s="21"/>
     </row>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A973" s="20"/>
+      <c r="A973" s="21"/>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A974" s="20"/>
+      <c r="A974" s="21"/>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A975" s="20"/>
+      <c r="A975" s="21"/>
     </row>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A976" s="20"/>
+      <c r="A976" s="21"/>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A977" s="20"/>
+      <c r="A977" s="21"/>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A978" s="20"/>
+      <c r="A978" s="21"/>
     </row>
     <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A979" s="20"/>
+      <c r="A979" s="21"/>
     </row>
     <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A980" s="20"/>
+      <c r="A980" s="21"/>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A981" s="20"/>
+      <c r="A981" s="21"/>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A982" s="20"/>
+      <c r="A982" s="21"/>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A983" s="20"/>
+      <c r="A983" s="21"/>
     </row>
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A984" s="20"/>
+      <c r="A984" s="21"/>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A985" s="20"/>
+      <c r="A985" s="21"/>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A986" s="20"/>
+      <c r="A986" s="21"/>
     </row>
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A987" s="20"/>
+      <c r="A987" s="21"/>
     </row>
     <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A988" s="20"/>
+      <c r="A988" s="21"/>
     </row>
     <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A989" s="20"/>
+      <c r="A989" s="21"/>
     </row>
     <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A990" s="20"/>
+      <c r="A990" s="21"/>
     </row>
     <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A991" s="20"/>
+      <c r="A991" s="21"/>
     </row>
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A992" s="20"/>
+      <c r="A992" s="21"/>
     </row>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A993" s="20"/>
+      <c r="A993" s="21"/>
     </row>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A994" s="20"/>
+      <c r="A994" s="21"/>
     </row>
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A995" s="20"/>
+      <c r="A995" s="21"/>
     </row>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A996" s="20"/>
+      <c r="A996" s="21"/>
     </row>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A997" s="20"/>
+      <c r="A997" s="21"/>
     </row>
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A998" s="20"/>
+      <c r="A998" s="21"/>
     </row>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A999" s="20"/>
+      <c r="A999" s="21"/>
     </row>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1000" s="20"/>
+      <c r="A1000" s="21"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add LeetCode solutions and update C++ config
Added Solution for Neetcode Blind 75 problems,  125, 141, 20, 206, 234, 3, 5, and 647.
</commit_message>
<xml_diff>
--- a/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -1148,12 +1148,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFFFEB9C"/>
       </patternFill>
@@ -1168,6 +1162,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1316,23 +1316,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1344,7 +1344,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1352,7 +1352,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="8" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1612,8 +1612,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1815,13 +1815,13 @@
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -1838,7 +1838,7 @@
       <c r="C13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="9" t="s">
@@ -1855,7 +1855,7 @@
       <c r="C14" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -1872,7 +1872,7 @@
       <c r="C15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>61</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -1889,7 +1889,7 @@
       <c r="C16" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="9" t="s">
@@ -1957,7 +1957,7 @@
       <c r="C20" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>82</v>
       </c>
       <c r="E20" s="9" t="s">
@@ -2158,7 +2158,7 @@
       <c r="B32" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>130</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -2169,13 +2169,13 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>134</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -2186,10 +2186,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C34" s="10" t="s">
@@ -2203,10 +2203,10 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C35" s="10" t="s">
@@ -2226,7 +2226,7 @@
       <c r="B36" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>147</v>
       </c>
       <c r="D36" s="8" t="s">
@@ -2274,7 +2274,7 @@
       <c r="A39" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="14" t="s">
         <v>146</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -2288,10 +2288,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="14" t="s">
         <v>146</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -2308,7 +2308,7 @@
       <c r="A41" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C41" s="7" t="s">
@@ -2362,7 +2362,7 @@
       <c r="B44" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="12" t="s">
         <v>180</v>
       </c>
       <c r="D44" s="8" t="s">
@@ -2478,7 +2478,7 @@
       <c r="A51" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="15" t="s">
         <v>209</v>
       </c>
       <c r="C51" s="10" t="s">
@@ -2515,7 +2515,7 @@
       <c r="B53" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="12" t="s">
         <v>218</v>
       </c>
       <c r="D53" s="8" t="s">
@@ -2563,7 +2563,7 @@
       <c r="A56" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="6" t="s">
         <v>209</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2580,7 +2580,7 @@
       <c r="A57" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="6" t="s">
         <v>209</v>
       </c>
       <c r="C57" s="7" t="s">
@@ -2628,10 +2628,10 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="14" t="s">
         <v>209</v>
       </c>
       <c r="C60" s="10" t="s">
@@ -2702,7 +2702,7 @@
       <c r="B64" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="12" t="s">
         <v>263</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -2736,7 +2736,7 @@
       <c r="B66" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="12" t="s">
         <v>271</v>
       </c>
       <c r="D66" s="8" t="s">
@@ -2872,7 +2872,7 @@
       <c r="B74" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="12" t="s">
         <v>303</v>
       </c>
       <c r="D74" s="8" t="s">
@@ -2889,7 +2889,7 @@
       <c r="B75" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="12" t="s">
         <v>180</v>
       </c>
       <c r="D75" s="8" t="s">
@@ -2923,10 +2923,10 @@
       <c r="B77" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="D77" s="12" t="s">
+      <c r="D77" s="11" t="s">
         <v>314</v>
       </c>
       <c r="E77" s="9" t="s">

</xml_diff>

<commit_message>
pushing house robber, LC49 and more problems
</commit_message>
<xml_diff>
--- a/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -1612,8 +1612,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2325,7 +2325,7 @@
       <c r="A42" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="15" t="s">
         <v>167</v>
       </c>
       <c r="C42" s="7" t="s">
@@ -2342,7 +2342,7 @@
       <c r="A43" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="15" t="s">
         <v>167</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -2478,7 +2478,7 @@
       <c r="A51" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="6" t="s">
         <v>209</v>
       </c>
       <c r="C51" s="10" t="s">
@@ -2597,7 +2597,7 @@
       <c r="A58" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="6" t="s">
         <v>209</v>
       </c>
       <c r="C58" s="10" t="s">
@@ -2614,7 +2614,7 @@
       <c r="A59" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="6" t="s">
         <v>209</v>
       </c>
       <c r="C59" s="10" t="s">

</xml_diff>

<commit_message>
pushing progress to Blind75 excel
</commit_message>
<xml_diff>
--- a/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -989,7 +989,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1012,7 +1011,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1021,21 +1019,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1043,14 +1038,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1058,14 +1051,12 @@
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1073,7 +1064,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1082,21 +1072,18 @@
       <color rgb="FF000000"/>
       <name val="Roboto"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1104,7 +1091,6 @@
       <color theme="4"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1112,7 +1098,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1148,6 +1133,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFFFEB9C"/>
       </patternFill>
@@ -1162,12 +1153,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1316,23 +1301,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1344,7 +1329,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1352,7 +1337,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1473,16 +1458,16 @@
         <a:srgbClr val="1155cc"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -1490,67 +1475,25 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -1569,35 +1512,11 @@
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -1607,13 +1526,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1624,7 +1542,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="146.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1641,7 +1559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1658,7 +1576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -1675,7 +1593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -1692,7 +1610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -1709,7 +1627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1726,7 +1644,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
@@ -1743,7 +1661,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -1760,7 +1678,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1777,7 +1695,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>38</v>
       </c>
@@ -1794,7 +1712,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
@@ -1811,24 +1729,24 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
@@ -1838,14 +1756,14 @@
       <c r="C13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
@@ -1855,14 +1773,14 @@
       <c r="C14" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="12" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
         <v>59</v>
       </c>
@@ -1872,14 +1790,14 @@
       <c r="C15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
@@ -1889,14 +1807,14 @@
       <c r="C16" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="12" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>67</v>
       </c>
@@ -1913,7 +1831,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1930,7 +1848,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
         <v>76</v>
       </c>
@@ -1947,7 +1865,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
         <v>80</v>
       </c>
@@ -1957,14 +1875,14 @@
       <c r="C20" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="12" t="s">
         <v>82</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
         <v>84</v>
       </c>
@@ -1981,7 +1899,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>88</v>
       </c>
@@ -1998,11 +1916,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="6" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -2015,7 +1933,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
         <v>96</v>
       </c>
@@ -2032,7 +1950,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
         <v>100</v>
       </c>
@@ -2049,7 +1967,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
         <v>104</v>
       </c>
@@ -2066,7 +1984,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
         <v>108</v>
       </c>
@@ -2083,7 +2001,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>112</v>
       </c>
@@ -2100,7 +2018,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
         <v>117</v>
       </c>
@@ -2117,7 +2035,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
         <v>121</v>
       </c>
@@ -2134,7 +2052,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
         <v>125</v>
       </c>
@@ -2151,14 +2069,14 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="13" t="s">
         <v>130</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -2168,14 +2086,14 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>134</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -2185,11 +2103,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="s">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C34" s="10" t="s">
@@ -2202,11 +2120,11 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13" t="s">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C35" s="10" t="s">
@@ -2219,14 +2137,14 @@
         <v>144</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
         <v>145</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="13" t="s">
         <v>147</v>
       </c>
       <c r="D36" s="8" t="s">
@@ -2236,7 +2154,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
         <v>150</v>
       </c>
@@ -2253,7 +2171,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
         <v>154</v>
       </c>
@@ -2270,11 +2188,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -2287,11 +2205,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13" t="s">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -2304,7 +2222,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
         <v>166</v>
       </c>
@@ -2321,11 +2239,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C42" s="7" t="s">
@@ -2338,11 +2256,11 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -2355,14 +2273,14 @@
         <v>178</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="13" t="s">
         <v>180</v>
       </c>
       <c r="D44" s="8" t="s">
@@ -2372,7 +2290,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
         <v>183</v>
       </c>
@@ -2389,11 +2307,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="11" t="s">
         <v>167</v>
       </c>
       <c r="C46" s="10" t="s">
@@ -2406,7 +2324,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
         <v>191</v>
       </c>
@@ -2423,7 +2341,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
         <v>196</v>
       </c>
@@ -2440,7 +2358,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
         <v>200</v>
       </c>
@@ -2457,7 +2375,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
         <v>204</v>
       </c>
@@ -2474,7 +2392,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
         <v>208</v>
       </c>
@@ -2491,11 +2409,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="6" t="s">
         <v>209</v>
       </c>
       <c r="C52" s="10" t="s">
@@ -2515,7 +2433,7 @@
       <c r="B53" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="13" t="s">
         <v>218</v>
       </c>
       <c r="D53" s="8" t="s">
@@ -2525,7 +2443,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
         <v>221</v>
       </c>
@@ -2542,11 +2460,11 @@
         <v>224</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="6" t="s">
         <v>209</v>
       </c>
       <c r="C55" s="10" t="s">
@@ -2559,7 +2477,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
         <v>229</v>
       </c>
@@ -2576,7 +2494,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
         <v>233</v>
       </c>
@@ -2593,7 +2511,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
         <v>237</v>
       </c>
@@ -2610,7 +2528,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
         <v>241</v>
       </c>
@@ -2627,11 +2545,11 @@
         <v>244</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="13" t="s">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="15" t="s">
         <v>209</v>
       </c>
       <c r="C60" s="10" t="s">
@@ -2644,7 +2562,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
         <v>249</v>
       </c>
@@ -2661,11 +2579,11 @@
         <v>253</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C62" s="7" t="s">
@@ -2678,7 +2596,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
         <v>258</v>
       </c>
@@ -2695,14 +2613,14 @@
         <v>261</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
         <v>262</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="13" t="s">
         <v>263</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -2712,7 +2630,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
         <v>266</v>
       </c>
@@ -2729,14 +2647,14 @@
         <v>269</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
         <v>270</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="13" t="s">
         <v>271</v>
       </c>
       <c r="D66" s="8" t="s">
@@ -2746,7 +2664,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
         <v>274</v>
       </c>
@@ -2763,7 +2681,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
         <v>278</v>
       </c>
@@ -2780,7 +2698,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
         <v>282</v>
       </c>
@@ -2797,7 +2715,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
         <v>286</v>
       </c>
@@ -2814,7 +2732,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
         <v>290</v>
       </c>
@@ -2831,7 +2749,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
         <v>294</v>
       </c>
@@ -2848,7 +2766,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
         <v>298</v>
       </c>
@@ -2865,14 +2783,14 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
         <v>302</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C74" s="12" t="s">
+      <c r="C74" s="13" t="s">
         <v>303</v>
       </c>
       <c r="D74" s="8" t="s">
@@ -2882,14 +2800,14 @@
         <v>305</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B75" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C75" s="12" t="s">
+      <c r="C75" s="13" t="s">
         <v>180</v>
       </c>
       <c r="D75" s="8" t="s">
@@ -2899,7 +2817,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
         <v>308</v>
       </c>
@@ -2916,17 +2834,17 @@
         <v>311</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
         <v>312</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C77" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="D77" s="11" t="s">
+      <c r="D77" s="12" t="s">
         <v>314</v>
       </c>
       <c r="E77" s="9" t="s">

</xml_diff>

<commit_message>
Pushing LC blind 75 problems
</commit_message>
<xml_diff>
--- a/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="319">
   <si>
     <t xml:space="preserve">Video Solution</t>
   </si>
@@ -974,6 +974,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://neetcode.io/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 remaining</t>
   </si>
 </sst>
 </file>
@@ -989,6 +992,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1011,6 +1015,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1019,18 +1024,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1038,12 +1046,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1051,12 +1061,14 @@
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1064,6 +1076,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1072,18 +1085,21 @@
       <color rgb="FF000000"/>
       <name val="Roboto"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1091,6 +1107,7 @@
       <color theme="4"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1098,9 +1115,10 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1134,7 +1152,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF38"/>
       </patternFill>
     </fill>
     <fill>
@@ -1153,6 +1171,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF38"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1256,7 +1280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1309,6 +1333,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1321,8 +1349,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1382,7 +1418,7 @@
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFFF38"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -1530,8 +1566,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E60" activeCellId="0" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1542,7 +1578,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="146.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1576,7 +1612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -1593,7 +1629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -1610,7 +1646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -1627,7 +1663,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1644,7 +1680,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
@@ -1661,7 +1697,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -1678,7 +1714,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1695,7 +1731,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>38</v>
       </c>
@@ -1712,7 +1748,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
@@ -1729,7 +1765,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
@@ -1746,7 +1782,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
@@ -1763,7 +1799,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
@@ -1780,7 +1816,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
         <v>59</v>
       </c>
@@ -1797,7 +1833,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
@@ -1814,7 +1850,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>67</v>
       </c>
@@ -1831,7 +1867,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1848,7 +1884,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
         <v>76</v>
       </c>
@@ -1865,7 +1901,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
         <v>80</v>
       </c>
@@ -1882,7 +1918,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
         <v>84</v>
       </c>
@@ -1899,11 +1935,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="13" t="s">
         <v>68</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -1916,7 +1952,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>92</v>
       </c>
@@ -1933,7 +1969,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
         <v>96</v>
       </c>
@@ -1950,7 +1986,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
         <v>100</v>
       </c>
@@ -1967,7 +2003,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
         <v>104</v>
       </c>
@@ -1984,7 +2020,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
         <v>108</v>
       </c>
@@ -2001,7 +2037,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>112</v>
       </c>
@@ -2018,7 +2054,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
         <v>117</v>
       </c>
@@ -2035,7 +2071,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
         <v>121</v>
       </c>
@@ -2052,7 +2088,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
         <v>125</v>
       </c>
@@ -2069,14 +2105,14 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="14" t="s">
         <v>130</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -2086,14 +2122,14 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="14" t="s">
         <v>134</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -2103,11 +2139,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="16" t="s">
         <v>113</v>
       </c>
       <c r="C34" s="10" t="s">
@@ -2120,11 +2156,11 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="16" t="s">
         <v>113</v>
       </c>
       <c r="C35" s="10" t="s">
@@ -2137,14 +2173,14 @@
         <v>144</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
         <v>145</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="14" t="s">
         <v>147</v>
       </c>
       <c r="D36" s="8" t="s">
@@ -2154,7 +2190,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
         <v>150</v>
       </c>
@@ -2171,7 +2207,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
         <v>154</v>
       </c>
@@ -2188,11 +2224,11 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="16" t="s">
         <v>146</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -2205,11 +2241,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14" t="s">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="16" t="s">
         <v>146</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -2222,7 +2258,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
         <v>166</v>
       </c>
@@ -2239,7 +2275,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
         <v>171</v>
       </c>
@@ -2256,7 +2292,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
         <v>175</v>
       </c>
@@ -2273,14 +2309,14 @@
         <v>178</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="14" t="s">
         <v>180</v>
       </c>
       <c r="D44" s="8" t="s">
@@ -2290,11 +2326,11 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="17" t="s">
         <v>167</v>
       </c>
       <c r="C45" s="10" t="s">
@@ -2307,11 +2343,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C46" s="10" t="s">
@@ -2324,11 +2360,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="17" t="s">
         <v>192</v>
       </c>
       <c r="C47" s="10" t="s">
@@ -2341,7 +2377,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
         <v>196</v>
       </c>
@@ -2358,11 +2394,11 @@
         <v>199</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="17" t="s">
         <v>192</v>
       </c>
       <c r="C49" s="10" t="s">
@@ -2375,7 +2411,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
         <v>204</v>
       </c>
@@ -2392,7 +2428,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
         <v>208</v>
       </c>
@@ -2409,7 +2445,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
         <v>213</v>
       </c>
@@ -2427,13 +2463,13 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="18" t="s">
         <v>217</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="14" t="s">
         <v>218</v>
       </c>
       <c r="D53" s="8" t="s">
@@ -2443,7 +2479,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
         <v>221</v>
       </c>
@@ -2460,7 +2496,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
         <v>225</v>
       </c>
@@ -2477,7 +2513,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
         <v>229</v>
       </c>
@@ -2494,7 +2530,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
         <v>233</v>
       </c>
@@ -2511,7 +2547,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
         <v>237</v>
       </c>
@@ -2528,7 +2564,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
         <v>241</v>
       </c>
@@ -2545,11 +2581,11 @@
         <v>244</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="14" t="s">
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="16" t="s">
         <v>209</v>
       </c>
       <c r="C60" s="10" t="s">
@@ -2562,11 +2598,11 @@
         <v>248</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C61" s="7" t="s">
@@ -2579,7 +2615,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
         <v>254</v>
       </c>
@@ -2596,11 +2632,11 @@
         <v>257</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C63" s="7" t="s">
@@ -2613,14 +2649,14 @@
         <v>261</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="14" t="s">
         <v>263</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -2630,11 +2666,11 @@
         <v>265</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C65" s="10" t="s">
@@ -2647,14 +2683,14 @@
         <v>269</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
         <v>270</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="14" t="s">
         <v>271</v>
       </c>
       <c r="D66" s="8" t="s">
@@ -2664,11 +2700,11 @@
         <v>273</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C67" s="7" t="s">
@@ -2681,7 +2717,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
         <v>278</v>
       </c>
@@ -2698,11 +2734,11 @@
         <v>281</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C69" s="10" t="s">
@@ -2715,11 +2751,11 @@
         <v>285</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C70" s="10" t="s">
@@ -2732,11 +2768,11 @@
         <v>289</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C71" s="7" t="s">
@@ -2749,11 +2785,11 @@
         <v>293</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C72" s="10" t="s">
@@ -2766,11 +2802,11 @@
         <v>297</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="6" t="s">
         <v>250</v>
       </c>
       <c r="C73" s="10" t="s">
@@ -2783,14 +2819,14 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
         <v>302</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="14" t="s">
         <v>303</v>
       </c>
       <c r="D74" s="8" t="s">
@@ -2800,14 +2836,14 @@
         <v>305</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B75" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="14" t="s">
         <v>180</v>
       </c>
       <c r="D75" s="8" t="s">
@@ -2817,7 +2853,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
         <v>308</v>
       </c>
@@ -2834,14 +2870,14 @@
         <v>311</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
         <v>312</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="14" t="s">
         <v>313</v>
       </c>
       <c r="D77" s="12" t="s">
@@ -2852,2779 +2888,2782 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="17"/>
-      <c r="B78" s="18"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="21"/>
     </row>
     <row r="79" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="B79" s="20" t="s">
+      <c r="B79" s="23" t="s">
         <v>317</v>
       </c>
+      <c r="C79" s="1" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="21"/>
+      <c r="A80" s="24"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="21"/>
+      <c r="A81" s="24"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="21"/>
+      <c r="A82" s="24"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="21"/>
+      <c r="A83" s="24"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="21"/>
+      <c r="A84" s="24"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="21"/>
+      <c r="A85" s="24"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="21"/>
+      <c r="A86" s="24"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="21"/>
+      <c r="A87" s="24"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="21"/>
+      <c r="A88" s="24"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="21"/>
+      <c r="A89" s="24"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="21"/>
+      <c r="A90" s="24"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="21"/>
+      <c r="A91" s="24"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="21"/>
+      <c r="A92" s="24"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="21"/>
+      <c r="A93" s="24"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="21"/>
+      <c r="A94" s="24"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="21"/>
+      <c r="A95" s="24"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="21"/>
+      <c r="A96" s="24"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="21"/>
+      <c r="A97" s="24"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="21"/>
+      <c r="A98" s="24"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="21"/>
+      <c r="A99" s="24"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="21"/>
+      <c r="A100" s="24"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="21"/>
+      <c r="A101" s="24"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="21"/>
+      <c r="A102" s="24"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="21"/>
+      <c r="A103" s="24"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="21"/>
+      <c r="A104" s="24"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="21"/>
+      <c r="A105" s="24"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="21"/>
+      <c r="A106" s="24"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="21"/>
+      <c r="A107" s="24"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="21"/>
+      <c r="A108" s="24"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="21"/>
+      <c r="A109" s="24"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="21"/>
+      <c r="A110" s="24"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="21"/>
+      <c r="A111" s="24"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="21"/>
+      <c r="A112" s="24"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="21"/>
+      <c r="A113" s="24"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="21"/>
+      <c r="A114" s="24"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="21"/>
+      <c r="A115" s="24"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="21"/>
+      <c r="A116" s="24"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="21"/>
+      <c r="A117" s="24"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="21"/>
+      <c r="A118" s="24"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="21"/>
+      <c r="A119" s="24"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="21"/>
+      <c r="A120" s="24"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="21"/>
+      <c r="A121" s="24"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="21"/>
+      <c r="A122" s="24"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="21"/>
+      <c r="A123" s="24"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="21"/>
+      <c r="A124" s="24"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="21"/>
+      <c r="A125" s="24"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="21"/>
+      <c r="A126" s="24"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="21"/>
+      <c r="A127" s="24"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="21"/>
+      <c r="A128" s="24"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="21"/>
+      <c r="A129" s="24"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="21"/>
+      <c r="A130" s="24"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="21"/>
+      <c r="A131" s="24"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="21"/>
+      <c r="A132" s="24"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="21"/>
+      <c r="A133" s="24"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="21"/>
+      <c r="A134" s="24"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="21"/>
+      <c r="A135" s="24"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="21"/>
+      <c r="A136" s="24"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="21"/>
+      <c r="A137" s="24"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="21"/>
+      <c r="A138" s="24"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="21"/>
+      <c r="A139" s="24"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="21"/>
+      <c r="A140" s="24"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="21"/>
+      <c r="A141" s="24"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="21"/>
+      <c r="A142" s="24"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="21"/>
+      <c r="A143" s="24"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="21"/>
+      <c r="A144" s="24"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="21"/>
+      <c r="A145" s="24"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="21"/>
+      <c r="A146" s="24"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="21"/>
+      <c r="A147" s="24"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="21"/>
+      <c r="A148" s="24"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="21"/>
+      <c r="A149" s="24"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="21"/>
+      <c r="A150" s="24"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="21"/>
+      <c r="A151" s="24"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="21"/>
+      <c r="A152" s="24"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="21"/>
+      <c r="A153" s="24"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="21"/>
+      <c r="A154" s="24"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="21"/>
+      <c r="A155" s="24"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="21"/>
+      <c r="A156" s="24"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="21"/>
+      <c r="A157" s="24"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="21"/>
+      <c r="A158" s="24"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="21"/>
+      <c r="A159" s="24"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="21"/>
+      <c r="A160" s="24"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="21"/>
+      <c r="A161" s="24"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="21"/>
+      <c r="A162" s="24"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="21"/>
+      <c r="A163" s="24"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="21"/>
+      <c r="A164" s="24"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="21"/>
+      <c r="A165" s="24"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="21"/>
+      <c r="A166" s="24"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="21"/>
+      <c r="A167" s="24"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="21"/>
+      <c r="A168" s="24"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="21"/>
+      <c r="A169" s="24"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="21"/>
+      <c r="A170" s="24"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="21"/>
+      <c r="A171" s="24"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="21"/>
+      <c r="A172" s="24"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="21"/>
+      <c r="A173" s="24"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="21"/>
+      <c r="A174" s="24"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="21"/>
+      <c r="A175" s="24"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="21"/>
+      <c r="A176" s="24"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="21"/>
+      <c r="A177" s="24"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="21"/>
+      <c r="A178" s="24"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="21"/>
+      <c r="A179" s="24"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="21"/>
+      <c r="A180" s="24"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="21"/>
+      <c r="A181" s="24"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="21"/>
+      <c r="A182" s="24"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="21"/>
+      <c r="A183" s="24"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="21"/>
+      <c r="A184" s="24"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="21"/>
+      <c r="A185" s="24"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="21"/>
+      <c r="A186" s="24"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="21"/>
+      <c r="A187" s="24"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="21"/>
+      <c r="A188" s="24"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="21"/>
+      <c r="A189" s="24"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="21"/>
+      <c r="A190" s="24"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="21"/>
+      <c r="A191" s="24"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="21"/>
+      <c r="A192" s="24"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="21"/>
+      <c r="A193" s="24"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="21"/>
+      <c r="A194" s="24"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="21"/>
+      <c r="A195" s="24"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="21"/>
+      <c r="A196" s="24"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="21"/>
+      <c r="A197" s="24"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="21"/>
+      <c r="A198" s="24"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="21"/>
+      <c r="A199" s="24"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="21"/>
+      <c r="A200" s="24"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="21"/>
+      <c r="A201" s="24"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="21"/>
+      <c r="A202" s="24"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="21"/>
+      <c r="A203" s="24"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="21"/>
+      <c r="A204" s="24"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="21"/>
+      <c r="A205" s="24"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="21"/>
+      <c r="A206" s="24"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="21"/>
+      <c r="A207" s="24"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="21"/>
+      <c r="A208" s="24"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="21"/>
+      <c r="A209" s="24"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="21"/>
+      <c r="A210" s="24"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="21"/>
+      <c r="A211" s="24"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="21"/>
+      <c r="A212" s="24"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="21"/>
+      <c r="A213" s="24"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="21"/>
+      <c r="A214" s="24"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="21"/>
+      <c r="A215" s="24"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="21"/>
+      <c r="A216" s="24"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="21"/>
+      <c r="A217" s="24"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="21"/>
+      <c r="A218" s="24"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="21"/>
+      <c r="A219" s="24"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="21"/>
+      <c r="A220" s="24"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="21"/>
+      <c r="A221" s="24"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="21"/>
+      <c r="A222" s="24"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="21"/>
+      <c r="A223" s="24"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="21"/>
+      <c r="A224" s="24"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="21"/>
+      <c r="A225" s="24"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="21"/>
+      <c r="A226" s="24"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="21"/>
+      <c r="A227" s="24"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="21"/>
+      <c r="A228" s="24"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="21"/>
+      <c r="A229" s="24"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="21"/>
+      <c r="A230" s="24"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="21"/>
+      <c r="A231" s="24"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="21"/>
+      <c r="A232" s="24"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="21"/>
+      <c r="A233" s="24"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="21"/>
+      <c r="A234" s="24"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="21"/>
+      <c r="A235" s="24"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="21"/>
+      <c r="A236" s="24"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="21"/>
+      <c r="A237" s="24"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="21"/>
+      <c r="A238" s="24"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="21"/>
+      <c r="A239" s="24"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="21"/>
+      <c r="A240" s="24"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="21"/>
+      <c r="A241" s="24"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="21"/>
+      <c r="A242" s="24"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="21"/>
+      <c r="A243" s="24"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="21"/>
+      <c r="A244" s="24"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="21"/>
+      <c r="A245" s="24"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="21"/>
+      <c r="A246" s="24"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="21"/>
+      <c r="A247" s="24"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="21"/>
+      <c r="A248" s="24"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="21"/>
+      <c r="A249" s="24"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="21"/>
+      <c r="A250" s="24"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="21"/>
+      <c r="A251" s="24"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="21"/>
+      <c r="A252" s="24"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="21"/>
+      <c r="A253" s="24"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="21"/>
+      <c r="A254" s="24"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="21"/>
+      <c r="A255" s="24"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="21"/>
+      <c r="A256" s="24"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="21"/>
+      <c r="A257" s="24"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="21"/>
+      <c r="A258" s="24"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="21"/>
+      <c r="A259" s="24"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="21"/>
+      <c r="A260" s="24"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="21"/>
+      <c r="A261" s="24"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="21"/>
+      <c r="A262" s="24"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="21"/>
+      <c r="A263" s="24"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="21"/>
+      <c r="A264" s="24"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="21"/>
+      <c r="A265" s="24"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="21"/>
+      <c r="A266" s="24"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="21"/>
+      <c r="A267" s="24"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="21"/>
+      <c r="A268" s="24"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="21"/>
+      <c r="A269" s="24"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="21"/>
+      <c r="A270" s="24"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="21"/>
+      <c r="A271" s="24"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="21"/>
+      <c r="A272" s="24"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="21"/>
+      <c r="A273" s="24"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="21"/>
+      <c r="A274" s="24"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="21"/>
+      <c r="A275" s="24"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="21"/>
+      <c r="A276" s="24"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="21"/>
+      <c r="A277" s="24"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="21"/>
+      <c r="A278" s="24"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="21"/>
+      <c r="A279" s="24"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="21"/>
+      <c r="A280" s="24"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="21"/>
+      <c r="A281" s="24"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="21"/>
+      <c r="A282" s="24"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="21"/>
+      <c r="A283" s="24"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="21"/>
+      <c r="A284" s="24"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="21"/>
+      <c r="A285" s="24"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="21"/>
+      <c r="A286" s="24"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="21"/>
+      <c r="A287" s="24"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="21"/>
+      <c r="A288" s="24"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="21"/>
+      <c r="A289" s="24"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="21"/>
+      <c r="A290" s="24"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="21"/>
+      <c r="A291" s="24"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="21"/>
+      <c r="A292" s="24"/>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="21"/>
+      <c r="A293" s="24"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="21"/>
+      <c r="A294" s="24"/>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="21"/>
+      <c r="A295" s="24"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="21"/>
+      <c r="A296" s="24"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="21"/>
+      <c r="A297" s="24"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="21"/>
+      <c r="A298" s="24"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="21"/>
+      <c r="A299" s="24"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="21"/>
+      <c r="A300" s="24"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="21"/>
+      <c r="A301" s="24"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="21"/>
+      <c r="A302" s="24"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="21"/>
+      <c r="A303" s="24"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="21"/>
+      <c r="A304" s="24"/>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="21"/>
+      <c r="A305" s="24"/>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="21"/>
+      <c r="A306" s="24"/>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="21"/>
+      <c r="A307" s="24"/>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="21"/>
+      <c r="A308" s="24"/>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="21"/>
+      <c r="A309" s="24"/>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="21"/>
+      <c r="A310" s="24"/>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="21"/>
+      <c r="A311" s="24"/>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="21"/>
+      <c r="A312" s="24"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="21"/>
+      <c r="A313" s="24"/>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="21"/>
+      <c r="A314" s="24"/>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="21"/>
+      <c r="A315" s="24"/>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="21"/>
+      <c r="A316" s="24"/>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="21"/>
+      <c r="A317" s="24"/>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="21"/>
+      <c r="A318" s="24"/>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="21"/>
+      <c r="A319" s="24"/>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="21"/>
+      <c r="A320" s="24"/>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="21"/>
+      <c r="A321" s="24"/>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="21"/>
+      <c r="A322" s="24"/>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="21"/>
+      <c r="A323" s="24"/>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="21"/>
+      <c r="A324" s="24"/>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="21"/>
+      <c r="A325" s="24"/>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="21"/>
+      <c r="A326" s="24"/>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A327" s="21"/>
+      <c r="A327" s="24"/>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="21"/>
+      <c r="A328" s="24"/>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="21"/>
+      <c r="A329" s="24"/>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="21"/>
+      <c r="A330" s="24"/>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="21"/>
+      <c r="A331" s="24"/>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="21"/>
+      <c r="A332" s="24"/>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A333" s="21"/>
+      <c r="A333" s="24"/>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A334" s="21"/>
+      <c r="A334" s="24"/>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="21"/>
+      <c r="A335" s="24"/>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="21"/>
+      <c r="A336" s="24"/>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="21"/>
+      <c r="A337" s="24"/>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="21"/>
+      <c r="A338" s="24"/>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="21"/>
+      <c r="A339" s="24"/>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A340" s="21"/>
+      <c r="A340" s="24"/>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="21"/>
+      <c r="A341" s="24"/>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="21"/>
+      <c r="A342" s="24"/>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A343" s="21"/>
+      <c r="A343" s="24"/>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A344" s="21"/>
+      <c r="A344" s="24"/>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A345" s="21"/>
+      <c r="A345" s="24"/>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="21"/>
+      <c r="A346" s="24"/>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A347" s="21"/>
+      <c r="A347" s="24"/>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A348" s="21"/>
+      <c r="A348" s="24"/>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="21"/>
+      <c r="A349" s="24"/>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="21"/>
+      <c r="A350" s="24"/>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="21"/>
+      <c r="A351" s="24"/>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="21"/>
+      <c r="A352" s="24"/>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="21"/>
+      <c r="A353" s="24"/>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="21"/>
+      <c r="A354" s="24"/>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="21"/>
+      <c r="A355" s="24"/>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="21"/>
+      <c r="A356" s="24"/>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="21"/>
+      <c r="A357" s="24"/>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="21"/>
+      <c r="A358" s="24"/>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="21"/>
+      <c r="A359" s="24"/>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="21"/>
+      <c r="A360" s="24"/>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="21"/>
+      <c r="A361" s="24"/>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="21"/>
+      <c r="A362" s="24"/>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A363" s="21"/>
+      <c r="A363" s="24"/>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A364" s="21"/>
+      <c r="A364" s="24"/>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A365" s="21"/>
+      <c r="A365" s="24"/>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A366" s="21"/>
+      <c r="A366" s="24"/>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A367" s="21"/>
+      <c r="A367" s="24"/>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A368" s="21"/>
+      <c r="A368" s="24"/>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A369" s="21"/>
+      <c r="A369" s="24"/>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A370" s="21"/>
+      <c r="A370" s="24"/>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A371" s="21"/>
+      <c r="A371" s="24"/>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A372" s="21"/>
+      <c r="A372" s="24"/>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A373" s="21"/>
+      <c r="A373" s="24"/>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="21"/>
+      <c r="A374" s="24"/>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A375" s="21"/>
+      <c r="A375" s="24"/>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A376" s="21"/>
+      <c r="A376" s="24"/>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A377" s="21"/>
+      <c r="A377" s="24"/>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A378" s="21"/>
+      <c r="A378" s="24"/>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A379" s="21"/>
+      <c r="A379" s="24"/>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A380" s="21"/>
+      <c r="A380" s="24"/>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A381" s="21"/>
+      <c r="A381" s="24"/>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A382" s="21"/>
+      <c r="A382" s="24"/>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="21"/>
+      <c r="A383" s="24"/>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A384" s="21"/>
+      <c r="A384" s="24"/>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A385" s="21"/>
+      <c r="A385" s="24"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A386" s="21"/>
+      <c r="A386" s="24"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="21"/>
+      <c r="A387" s="24"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A388" s="21"/>
+      <c r="A388" s="24"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="21"/>
+      <c r="A389" s="24"/>
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A390" s="21"/>
+      <c r="A390" s="24"/>
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="21"/>
+      <c r="A391" s="24"/>
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A392" s="21"/>
+      <c r="A392" s="24"/>
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A393" s="21"/>
+      <c r="A393" s="24"/>
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A394" s="21"/>
+      <c r="A394" s="24"/>
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A395" s="21"/>
+      <c r="A395" s="24"/>
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="21"/>
+      <c r="A396" s="24"/>
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A397" s="21"/>
+      <c r="A397" s="24"/>
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A398" s="21"/>
+      <c r="A398" s="24"/>
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A399" s="21"/>
+      <c r="A399" s="24"/>
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A400" s="21"/>
+      <c r="A400" s="24"/>
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A401" s="21"/>
+      <c r="A401" s="24"/>
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A402" s="21"/>
+      <c r="A402" s="24"/>
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="21"/>
+      <c r="A403" s="24"/>
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A404" s="21"/>
+      <c r="A404" s="24"/>
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="21"/>
+      <c r="A405" s="24"/>
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A406" s="21"/>
+      <c r="A406" s="24"/>
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A407" s="21"/>
+      <c r="A407" s="24"/>
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A408" s="21"/>
+      <c r="A408" s="24"/>
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="21"/>
+      <c r="A409" s="24"/>
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="21"/>
+      <c r="A410" s="24"/>
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="21"/>
+      <c r="A411" s="24"/>
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A412" s="21"/>
+      <c r="A412" s="24"/>
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="21"/>
+      <c r="A413" s="24"/>
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A414" s="21"/>
+      <c r="A414" s="24"/>
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A415" s="21"/>
+      <c r="A415" s="24"/>
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A416" s="21"/>
+      <c r="A416" s="24"/>
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A417" s="21"/>
+      <c r="A417" s="24"/>
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="21"/>
+      <c r="A418" s="24"/>
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A419" s="21"/>
+      <c r="A419" s="24"/>
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="21"/>
+      <c r="A420" s="24"/>
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A421" s="21"/>
+      <c r="A421" s="24"/>
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A422" s="21"/>
+      <c r="A422" s="24"/>
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="21"/>
+      <c r="A423" s="24"/>
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A424" s="21"/>
+      <c r="A424" s="24"/>
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A425" s="21"/>
+      <c r="A425" s="24"/>
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A426" s="21"/>
+      <c r="A426" s="24"/>
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A427" s="21"/>
+      <c r="A427" s="24"/>
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A428" s="21"/>
+      <c r="A428" s="24"/>
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="21"/>
+      <c r="A429" s="24"/>
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A430" s="21"/>
+      <c r="A430" s="24"/>
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="21"/>
+      <c r="A431" s="24"/>
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="21"/>
+      <c r="A432" s="24"/>
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="21"/>
+      <c r="A433" s="24"/>
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="21"/>
+      <c r="A434" s="24"/>
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="21"/>
+      <c r="A435" s="24"/>
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="21"/>
+      <c r="A436" s="24"/>
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="21"/>
+      <c r="A437" s="24"/>
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A438" s="21"/>
+      <c r="A438" s="24"/>
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A439" s="21"/>
+      <c r="A439" s="24"/>
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="21"/>
+      <c r="A440" s="24"/>
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="21"/>
+      <c r="A441" s="24"/>
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A442" s="21"/>
+      <c r="A442" s="24"/>
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="21"/>
+      <c r="A443" s="24"/>
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A444" s="21"/>
+      <c r="A444" s="24"/>
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A445" s="21"/>
+      <c r="A445" s="24"/>
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A446" s="21"/>
+      <c r="A446" s="24"/>
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A447" s="21"/>
+      <c r="A447" s="24"/>
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A448" s="21"/>
+      <c r="A448" s="24"/>
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="21"/>
+      <c r="A449" s="24"/>
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A450" s="21"/>
+      <c r="A450" s="24"/>
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A451" s="21"/>
+      <c r="A451" s="24"/>
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A452" s="21"/>
+      <c r="A452" s="24"/>
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A453" s="21"/>
+      <c r="A453" s="24"/>
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A454" s="21"/>
+      <c r="A454" s="24"/>
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A455" s="21"/>
+      <c r="A455" s="24"/>
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A456" s="21"/>
+      <c r="A456" s="24"/>
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A457" s="21"/>
+      <c r="A457" s="24"/>
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A458" s="21"/>
+      <c r="A458" s="24"/>
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A459" s="21"/>
+      <c r="A459" s="24"/>
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A460" s="21"/>
+      <c r="A460" s="24"/>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A461" s="21"/>
+      <c r="A461" s="24"/>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A462" s="21"/>
+      <c r="A462" s="24"/>
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A463" s="21"/>
+      <c r="A463" s="24"/>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A464" s="21"/>
+      <c r="A464" s="24"/>
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A465" s="21"/>
+      <c r="A465" s="24"/>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A466" s="21"/>
+      <c r="A466" s="24"/>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A467" s="21"/>
+      <c r="A467" s="24"/>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A468" s="21"/>
+      <c r="A468" s="24"/>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A469" s="21"/>
+      <c r="A469" s="24"/>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A470" s="21"/>
+      <c r="A470" s="24"/>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A471" s="21"/>
+      <c r="A471" s="24"/>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A472" s="21"/>
+      <c r="A472" s="24"/>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A473" s="21"/>
+      <c r="A473" s="24"/>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A474" s="21"/>
+      <c r="A474" s="24"/>
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="21"/>
+      <c r="A475" s="24"/>
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A476" s="21"/>
+      <c r="A476" s="24"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A477" s="21"/>
+      <c r="A477" s="24"/>
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A478" s="21"/>
+      <c r="A478" s="24"/>
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A479" s="21"/>
+      <c r="A479" s="24"/>
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A480" s="21"/>
+      <c r="A480" s="24"/>
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A481" s="21"/>
+      <c r="A481" s="24"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="21"/>
+      <c r="A482" s="24"/>
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A483" s="21"/>
+      <c r="A483" s="24"/>
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A484" s="21"/>
+      <c r="A484" s="24"/>
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A485" s="21"/>
+      <c r="A485" s="24"/>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A486" s="21"/>
+      <c r="A486" s="24"/>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A487" s="21"/>
+      <c r="A487" s="24"/>
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A488" s="21"/>
+      <c r="A488" s="24"/>
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A489" s="21"/>
+      <c r="A489" s="24"/>
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A490" s="21"/>
+      <c r="A490" s="24"/>
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A491" s="21"/>
+      <c r="A491" s="24"/>
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A492" s="21"/>
+      <c r="A492" s="24"/>
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A493" s="21"/>
+      <c r="A493" s="24"/>
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A494" s="21"/>
+      <c r="A494" s="24"/>
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A495" s="21"/>
+      <c r="A495" s="24"/>
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A496" s="21"/>
+      <c r="A496" s="24"/>
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A497" s="21"/>
+      <c r="A497" s="24"/>
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A498" s="21"/>
+      <c r="A498" s="24"/>
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A499" s="21"/>
+      <c r="A499" s="24"/>
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A500" s="21"/>
+      <c r="A500" s="24"/>
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A501" s="21"/>
+      <c r="A501" s="24"/>
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A502" s="21"/>
+      <c r="A502" s="24"/>
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A503" s="21"/>
+      <c r="A503" s="24"/>
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A504" s="21"/>
+      <c r="A504" s="24"/>
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A505" s="21"/>
+      <c r="A505" s="24"/>
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A506" s="21"/>
+      <c r="A506" s="24"/>
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A507" s="21"/>
+      <c r="A507" s="24"/>
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A508" s="21"/>
+      <c r="A508" s="24"/>
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A509" s="21"/>
+      <c r="A509" s="24"/>
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A510" s="21"/>
+      <c r="A510" s="24"/>
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A511" s="21"/>
+      <c r="A511" s="24"/>
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A512" s="21"/>
+      <c r="A512" s="24"/>
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A513" s="21"/>
+      <c r="A513" s="24"/>
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A514" s="21"/>
+      <c r="A514" s="24"/>
     </row>
     <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A515" s="21"/>
+      <c r="A515" s="24"/>
     </row>
     <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A516" s="21"/>
+      <c r="A516" s="24"/>
     </row>
     <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A517" s="21"/>
+      <c r="A517" s="24"/>
     </row>
     <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A518" s="21"/>
+      <c r="A518" s="24"/>
     </row>
     <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A519" s="21"/>
+      <c r="A519" s="24"/>
     </row>
     <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A520" s="21"/>
+      <c r="A520" s="24"/>
     </row>
     <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A521" s="21"/>
+      <c r="A521" s="24"/>
     </row>
     <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A522" s="21"/>
+      <c r="A522" s="24"/>
     </row>
     <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A523" s="21"/>
+      <c r="A523" s="24"/>
     </row>
     <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A524" s="21"/>
+      <c r="A524" s="24"/>
     </row>
     <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A525" s="21"/>
+      <c r="A525" s="24"/>
     </row>
     <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A526" s="21"/>
+      <c r="A526" s="24"/>
     </row>
     <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A527" s="21"/>
+      <c r="A527" s="24"/>
     </row>
     <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A528" s="21"/>
+      <c r="A528" s="24"/>
     </row>
     <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A529" s="21"/>
+      <c r="A529" s="24"/>
     </row>
     <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A530" s="21"/>
+      <c r="A530" s="24"/>
     </row>
     <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A531" s="21"/>
+      <c r="A531" s="24"/>
     </row>
     <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A532" s="21"/>
+      <c r="A532" s="24"/>
     </row>
     <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A533" s="21"/>
+      <c r="A533" s="24"/>
     </row>
     <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A534" s="21"/>
+      <c r="A534" s="24"/>
     </row>
     <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A535" s="21"/>
+      <c r="A535" s="24"/>
     </row>
     <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A536" s="21"/>
+      <c r="A536" s="24"/>
     </row>
     <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A537" s="21"/>
+      <c r="A537" s="24"/>
     </row>
     <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A538" s="21"/>
+      <c r="A538" s="24"/>
     </row>
     <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A539" s="21"/>
+      <c r="A539" s="24"/>
     </row>
     <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A540" s="21"/>
+      <c r="A540" s="24"/>
     </row>
     <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A541" s="21"/>
+      <c r="A541" s="24"/>
     </row>
     <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A542" s="21"/>
+      <c r="A542" s="24"/>
     </row>
     <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A543" s="21"/>
+      <c r="A543" s="24"/>
     </row>
     <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A544" s="21"/>
+      <c r="A544" s="24"/>
     </row>
     <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A545" s="21"/>
+      <c r="A545" s="24"/>
     </row>
     <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A546" s="21"/>
+      <c r="A546" s="24"/>
     </row>
     <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A547" s="21"/>
+      <c r="A547" s="24"/>
     </row>
     <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A548" s="21"/>
+      <c r="A548" s="24"/>
     </row>
     <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A549" s="21"/>
+      <c r="A549" s="24"/>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A550" s="21"/>
+      <c r="A550" s="24"/>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A551" s="21"/>
+      <c r="A551" s="24"/>
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A552" s="21"/>
+      <c r="A552" s="24"/>
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A553" s="21"/>
+      <c r="A553" s="24"/>
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A554" s="21"/>
+      <c r="A554" s="24"/>
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A555" s="21"/>
+      <c r="A555" s="24"/>
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A556" s="21"/>
+      <c r="A556" s="24"/>
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A557" s="21"/>
+      <c r="A557" s="24"/>
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A558" s="21"/>
+      <c r="A558" s="24"/>
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A559" s="21"/>
+      <c r="A559" s="24"/>
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A560" s="21"/>
+      <c r="A560" s="24"/>
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A561" s="21"/>
+      <c r="A561" s="24"/>
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A562" s="21"/>
+      <c r="A562" s="24"/>
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A563" s="21"/>
+      <c r="A563" s="24"/>
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A564" s="21"/>
+      <c r="A564" s="24"/>
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A565" s="21"/>
+      <c r="A565" s="24"/>
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A566" s="21"/>
+      <c r="A566" s="24"/>
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A567" s="21"/>
+      <c r="A567" s="24"/>
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A568" s="21"/>
+      <c r="A568" s="24"/>
     </row>
     <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A569" s="21"/>
+      <c r="A569" s="24"/>
     </row>
     <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A570" s="21"/>
+      <c r="A570" s="24"/>
     </row>
     <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A571" s="21"/>
+      <c r="A571" s="24"/>
     </row>
     <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A572" s="21"/>
+      <c r="A572" s="24"/>
     </row>
     <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A573" s="21"/>
+      <c r="A573" s="24"/>
     </row>
     <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A574" s="21"/>
+      <c r="A574" s="24"/>
     </row>
     <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A575" s="21"/>
+      <c r="A575" s="24"/>
     </row>
     <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A576" s="21"/>
+      <c r="A576" s="24"/>
     </row>
     <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A577" s="21"/>
+      <c r="A577" s="24"/>
     </row>
     <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A578" s="21"/>
+      <c r="A578" s="24"/>
     </row>
     <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A579" s="21"/>
+      <c r="A579" s="24"/>
     </row>
     <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A580" s="21"/>
+      <c r="A580" s="24"/>
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A581" s="21"/>
+      <c r="A581" s="24"/>
     </row>
     <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A582" s="21"/>
+      <c r="A582" s="24"/>
     </row>
     <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A583" s="21"/>
+      <c r="A583" s="24"/>
     </row>
     <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A584" s="21"/>
+      <c r="A584" s="24"/>
     </row>
     <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A585" s="21"/>
+      <c r="A585" s="24"/>
     </row>
     <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A586" s="21"/>
+      <c r="A586" s="24"/>
     </row>
     <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A587" s="21"/>
+      <c r="A587" s="24"/>
     </row>
     <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A588" s="21"/>
+      <c r="A588" s="24"/>
     </row>
     <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A589" s="21"/>
+      <c r="A589" s="24"/>
     </row>
     <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A590" s="21"/>
+      <c r="A590" s="24"/>
     </row>
     <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A591" s="21"/>
+      <c r="A591" s="24"/>
     </row>
     <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A592" s="21"/>
+      <c r="A592" s="24"/>
     </row>
     <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A593" s="21"/>
+      <c r="A593" s="24"/>
     </row>
     <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A594" s="21"/>
+      <c r="A594" s="24"/>
     </row>
     <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A595" s="21"/>
+      <c r="A595" s="24"/>
     </row>
     <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A596" s="21"/>
+      <c r="A596" s="24"/>
     </row>
     <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A597" s="21"/>
+      <c r="A597" s="24"/>
     </row>
     <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A598" s="21"/>
+      <c r="A598" s="24"/>
     </row>
     <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A599" s="21"/>
+      <c r="A599" s="24"/>
     </row>
     <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A600" s="21"/>
+      <c r="A600" s="24"/>
     </row>
     <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A601" s="21"/>
+      <c r="A601" s="24"/>
     </row>
     <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A602" s="21"/>
+      <c r="A602" s="24"/>
     </row>
     <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A603" s="21"/>
+      <c r="A603" s="24"/>
     </row>
     <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A604" s="21"/>
+      <c r="A604" s="24"/>
     </row>
     <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A605" s="21"/>
+      <c r="A605" s="24"/>
     </row>
     <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A606" s="21"/>
+      <c r="A606" s="24"/>
     </row>
     <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A607" s="21"/>
+      <c r="A607" s="24"/>
     </row>
     <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A608" s="21"/>
+      <c r="A608" s="24"/>
     </row>
     <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A609" s="21"/>
+      <c r="A609" s="24"/>
     </row>
     <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A610" s="21"/>
+      <c r="A610" s="24"/>
     </row>
     <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A611" s="21"/>
+      <c r="A611" s="24"/>
     </row>
     <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A612" s="21"/>
+      <c r="A612" s="24"/>
     </row>
     <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A613" s="21"/>
+      <c r="A613" s="24"/>
     </row>
     <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A614" s="21"/>
+      <c r="A614" s="24"/>
     </row>
     <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A615" s="21"/>
+      <c r="A615" s="24"/>
     </row>
     <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A616" s="21"/>
+      <c r="A616" s="24"/>
     </row>
     <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A617" s="21"/>
+      <c r="A617" s="24"/>
     </row>
     <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A618" s="21"/>
+      <c r="A618" s="24"/>
     </row>
     <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A619" s="21"/>
+      <c r="A619" s="24"/>
     </row>
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A620" s="21"/>
+      <c r="A620" s="24"/>
     </row>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A621" s="21"/>
+      <c r="A621" s="24"/>
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A622" s="21"/>
+      <c r="A622" s="24"/>
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A623" s="21"/>
+      <c r="A623" s="24"/>
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A624" s="21"/>
+      <c r="A624" s="24"/>
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A625" s="21"/>
+      <c r="A625" s="24"/>
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A626" s="21"/>
+      <c r="A626" s="24"/>
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A627" s="21"/>
+      <c r="A627" s="24"/>
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A628" s="21"/>
+      <c r="A628" s="24"/>
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A629" s="21"/>
+      <c r="A629" s="24"/>
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A630" s="21"/>
+      <c r="A630" s="24"/>
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A631" s="21"/>
+      <c r="A631" s="24"/>
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A632" s="21"/>
+      <c r="A632" s="24"/>
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A633" s="21"/>
+      <c r="A633" s="24"/>
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A634" s="21"/>
+      <c r="A634" s="24"/>
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A635" s="21"/>
+      <c r="A635" s="24"/>
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A636" s="21"/>
+      <c r="A636" s="24"/>
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A637" s="21"/>
+      <c r="A637" s="24"/>
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A638" s="21"/>
+      <c r="A638" s="24"/>
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A639" s="21"/>
+      <c r="A639" s="24"/>
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A640" s="21"/>
+      <c r="A640" s="24"/>
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A641" s="21"/>
+      <c r="A641" s="24"/>
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A642" s="21"/>
+      <c r="A642" s="24"/>
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A643" s="21"/>
+      <c r="A643" s="24"/>
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A644" s="21"/>
+      <c r="A644" s="24"/>
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A645" s="21"/>
+      <c r="A645" s="24"/>
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A646" s="21"/>
+      <c r="A646" s="24"/>
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A647" s="21"/>
+      <c r="A647" s="24"/>
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A648" s="21"/>
+      <c r="A648" s="24"/>
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A649" s="21"/>
+      <c r="A649" s="24"/>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A650" s="21"/>
+      <c r="A650" s="24"/>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A651" s="21"/>
+      <c r="A651" s="24"/>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A652" s="21"/>
+      <c r="A652" s="24"/>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A653" s="21"/>
+      <c r="A653" s="24"/>
     </row>
     <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A654" s="21"/>
+      <c r="A654" s="24"/>
     </row>
     <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A655" s="21"/>
+      <c r="A655" s="24"/>
     </row>
     <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A656" s="21"/>
+      <c r="A656" s="24"/>
     </row>
     <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A657" s="21"/>
+      <c r="A657" s="24"/>
     </row>
     <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A658" s="21"/>
+      <c r="A658" s="24"/>
     </row>
     <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A659" s="21"/>
+      <c r="A659" s="24"/>
     </row>
     <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A660" s="21"/>
+      <c r="A660" s="24"/>
     </row>
     <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A661" s="21"/>
+      <c r="A661" s="24"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A662" s="21"/>
+      <c r="A662" s="24"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A663" s="21"/>
+      <c r="A663" s="24"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A664" s="21"/>
+      <c r="A664" s="24"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A665" s="21"/>
+      <c r="A665" s="24"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A666" s="21"/>
+      <c r="A666" s="24"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A667" s="21"/>
+      <c r="A667" s="24"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A668" s="21"/>
+      <c r="A668" s="24"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A669" s="21"/>
+      <c r="A669" s="24"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A670" s="21"/>
+      <c r="A670" s="24"/>
     </row>
     <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A671" s="21"/>
+      <c r="A671" s="24"/>
     </row>
     <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A672" s="21"/>
+      <c r="A672" s="24"/>
     </row>
     <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A673" s="21"/>
+      <c r="A673" s="24"/>
     </row>
     <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A674" s="21"/>
+      <c r="A674" s="24"/>
     </row>
     <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A675" s="21"/>
+      <c r="A675" s="24"/>
     </row>
     <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A676" s="21"/>
+      <c r="A676" s="24"/>
     </row>
     <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A677" s="21"/>
+      <c r="A677" s="24"/>
     </row>
     <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A678" s="21"/>
+      <c r="A678" s="24"/>
     </row>
     <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A679" s="21"/>
+      <c r="A679" s="24"/>
     </row>
     <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A680" s="21"/>
+      <c r="A680" s="24"/>
     </row>
     <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A681" s="21"/>
+      <c r="A681" s="24"/>
     </row>
     <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A682" s="21"/>
+      <c r="A682" s="24"/>
     </row>
     <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A683" s="21"/>
+      <c r="A683" s="24"/>
     </row>
     <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A684" s="21"/>
+      <c r="A684" s="24"/>
     </row>
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A685" s="21"/>
+      <c r="A685" s="24"/>
     </row>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A686" s="21"/>
+      <c r="A686" s="24"/>
     </row>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A687" s="21"/>
+      <c r="A687" s="24"/>
     </row>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A688" s="21"/>
+      <c r="A688" s="24"/>
     </row>
     <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A689" s="21"/>
+      <c r="A689" s="24"/>
     </row>
     <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A690" s="21"/>
+      <c r="A690" s="24"/>
     </row>
     <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A691" s="21"/>
+      <c r="A691" s="24"/>
     </row>
     <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A692" s="21"/>
+      <c r="A692" s="24"/>
     </row>
     <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A693" s="21"/>
+      <c r="A693" s="24"/>
     </row>
     <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A694" s="21"/>
+      <c r="A694" s="24"/>
     </row>
     <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A695" s="21"/>
+      <c r="A695" s="24"/>
     </row>
     <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A696" s="21"/>
+      <c r="A696" s="24"/>
     </row>
     <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A697" s="21"/>
+      <c r="A697" s="24"/>
     </row>
     <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A698" s="21"/>
+      <c r="A698" s="24"/>
     </row>
     <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A699" s="21"/>
+      <c r="A699" s="24"/>
     </row>
     <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A700" s="21"/>
+      <c r="A700" s="24"/>
     </row>
     <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A701" s="21"/>
+      <c r="A701" s="24"/>
     </row>
     <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A702" s="21"/>
+      <c r="A702" s="24"/>
     </row>
     <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A703" s="21"/>
+      <c r="A703" s="24"/>
     </row>
     <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A704" s="21"/>
+      <c r="A704" s="24"/>
     </row>
     <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A705" s="21"/>
+      <c r="A705" s="24"/>
     </row>
     <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A706" s="21"/>
+      <c r="A706" s="24"/>
     </row>
     <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A707" s="21"/>
+      <c r="A707" s="24"/>
     </row>
     <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A708" s="21"/>
+      <c r="A708" s="24"/>
     </row>
     <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A709" s="21"/>
+      <c r="A709" s="24"/>
     </row>
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A710" s="21"/>
+      <c r="A710" s="24"/>
     </row>
     <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A711" s="21"/>
+      <c r="A711" s="24"/>
     </row>
     <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A712" s="21"/>
+      <c r="A712" s="24"/>
     </row>
     <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A713" s="21"/>
+      <c r="A713" s="24"/>
     </row>
     <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A714" s="21"/>
+      <c r="A714" s="24"/>
     </row>
     <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A715" s="21"/>
+      <c r="A715" s="24"/>
     </row>
     <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A716" s="21"/>
+      <c r="A716" s="24"/>
     </row>
     <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A717" s="21"/>
+      <c r="A717" s="24"/>
     </row>
     <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A718" s="21"/>
+      <c r="A718" s="24"/>
     </row>
     <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A719" s="21"/>
+      <c r="A719" s="24"/>
     </row>
     <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A720" s="21"/>
+      <c r="A720" s="24"/>
     </row>
     <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A721" s="21"/>
+      <c r="A721" s="24"/>
     </row>
     <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A722" s="21"/>
+      <c r="A722" s="24"/>
     </row>
     <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A723" s="21"/>
+      <c r="A723" s="24"/>
     </row>
     <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A724" s="21"/>
+      <c r="A724" s="24"/>
     </row>
     <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A725" s="21"/>
+      <c r="A725" s="24"/>
     </row>
     <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A726" s="21"/>
+      <c r="A726" s="24"/>
     </row>
     <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A727" s="21"/>
+      <c r="A727" s="24"/>
     </row>
     <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A728" s="21"/>
+      <c r="A728" s="24"/>
     </row>
     <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A729" s="21"/>
+      <c r="A729" s="24"/>
     </row>
     <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A730" s="21"/>
+      <c r="A730" s="24"/>
     </row>
     <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A731" s="21"/>
+      <c r="A731" s="24"/>
     </row>
     <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A732" s="21"/>
+      <c r="A732" s="24"/>
     </row>
     <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A733" s="21"/>
+      <c r="A733" s="24"/>
     </row>
     <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A734" s="21"/>
+      <c r="A734" s="24"/>
     </row>
     <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A735" s="21"/>
+      <c r="A735" s="24"/>
     </row>
     <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A736" s="21"/>
+      <c r="A736" s="24"/>
     </row>
     <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A737" s="21"/>
+      <c r="A737" s="24"/>
     </row>
     <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A738" s="21"/>
+      <c r="A738" s="24"/>
     </row>
     <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A739" s="21"/>
+      <c r="A739" s="24"/>
     </row>
     <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A740" s="21"/>
+      <c r="A740" s="24"/>
     </row>
     <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A741" s="21"/>
+      <c r="A741" s="24"/>
     </row>
     <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A742" s="21"/>
+      <c r="A742" s="24"/>
     </row>
     <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A743" s="21"/>
+      <c r="A743" s="24"/>
     </row>
     <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A744" s="21"/>
+      <c r="A744" s="24"/>
     </row>
     <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A745" s="21"/>
+      <c r="A745" s="24"/>
     </row>
     <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A746" s="21"/>
+      <c r="A746" s="24"/>
     </row>
     <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A747" s="21"/>
+      <c r="A747" s="24"/>
     </row>
     <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A748" s="21"/>
+      <c r="A748" s="24"/>
     </row>
     <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A749" s="21"/>
+      <c r="A749" s="24"/>
     </row>
     <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A750" s="21"/>
+      <c r="A750" s="24"/>
     </row>
     <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A751" s="21"/>
+      <c r="A751" s="24"/>
     </row>
     <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A752" s="21"/>
+      <c r="A752" s="24"/>
     </row>
     <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A753" s="21"/>
+      <c r="A753" s="24"/>
     </row>
     <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A754" s="21"/>
+      <c r="A754" s="24"/>
     </row>
     <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A755" s="21"/>
+      <c r="A755" s="24"/>
     </row>
     <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A756" s="21"/>
+      <c r="A756" s="24"/>
     </row>
     <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A757" s="21"/>
+      <c r="A757" s="24"/>
     </row>
     <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A758" s="21"/>
+      <c r="A758" s="24"/>
     </row>
     <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A759" s="21"/>
+      <c r="A759" s="24"/>
     </row>
     <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A760" s="21"/>
+      <c r="A760" s="24"/>
     </row>
     <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A761" s="21"/>
+      <c r="A761" s="24"/>
     </row>
     <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A762" s="21"/>
+      <c r="A762" s="24"/>
     </row>
     <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A763" s="21"/>
+      <c r="A763" s="24"/>
     </row>
     <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A764" s="21"/>
+      <c r="A764" s="24"/>
     </row>
     <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A765" s="21"/>
+      <c r="A765" s="24"/>
     </row>
     <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A766" s="21"/>
+      <c r="A766" s="24"/>
     </row>
     <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A767" s="21"/>
+      <c r="A767" s="24"/>
     </row>
     <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A768" s="21"/>
+      <c r="A768" s="24"/>
     </row>
     <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A769" s="21"/>
+      <c r="A769" s="24"/>
     </row>
     <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A770" s="21"/>
+      <c r="A770" s="24"/>
     </row>
     <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A771" s="21"/>
+      <c r="A771" s="24"/>
     </row>
     <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A772" s="21"/>
+      <c r="A772" s="24"/>
     </row>
     <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A773" s="21"/>
+      <c r="A773" s="24"/>
     </row>
     <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A774" s="21"/>
+      <c r="A774" s="24"/>
     </row>
     <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A775" s="21"/>
+      <c r="A775" s="24"/>
     </row>
     <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A776" s="21"/>
+      <c r="A776" s="24"/>
     </row>
     <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A777" s="21"/>
+      <c r="A777" s="24"/>
     </row>
     <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A778" s="21"/>
+      <c r="A778" s="24"/>
     </row>
     <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A779" s="21"/>
+      <c r="A779" s="24"/>
     </row>
     <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A780" s="21"/>
+      <c r="A780" s="24"/>
     </row>
     <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A781" s="21"/>
+      <c r="A781" s="24"/>
     </row>
     <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A782" s="21"/>
+      <c r="A782" s="24"/>
     </row>
     <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A783" s="21"/>
+      <c r="A783" s="24"/>
     </row>
     <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A784" s="21"/>
+      <c r="A784" s="24"/>
     </row>
     <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A785" s="21"/>
+      <c r="A785" s="24"/>
     </row>
     <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A786" s="21"/>
+      <c r="A786" s="24"/>
     </row>
     <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A787" s="21"/>
+      <c r="A787" s="24"/>
     </row>
     <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A788" s="21"/>
+      <c r="A788" s="24"/>
     </row>
     <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A789" s="21"/>
+      <c r="A789" s="24"/>
     </row>
     <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A790" s="21"/>
+      <c r="A790" s="24"/>
     </row>
     <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A791" s="21"/>
+      <c r="A791" s="24"/>
     </row>
     <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A792" s="21"/>
+      <c r="A792" s="24"/>
     </row>
     <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A793" s="21"/>
+      <c r="A793" s="24"/>
     </row>
     <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A794" s="21"/>
+      <c r="A794" s="24"/>
     </row>
     <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A795" s="21"/>
+      <c r="A795" s="24"/>
     </row>
     <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A796" s="21"/>
+      <c r="A796" s="24"/>
     </row>
     <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A797" s="21"/>
+      <c r="A797" s="24"/>
     </row>
     <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A798" s="21"/>
+      <c r="A798" s="24"/>
     </row>
     <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A799" s="21"/>
+      <c r="A799" s="24"/>
     </row>
     <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A800" s="21"/>
+      <c r="A800" s="24"/>
     </row>
     <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A801" s="21"/>
+      <c r="A801" s="24"/>
     </row>
     <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A802" s="21"/>
+      <c r="A802" s="24"/>
     </row>
     <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A803" s="21"/>
+      <c r="A803" s="24"/>
     </row>
     <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A804" s="21"/>
+      <c r="A804" s="24"/>
     </row>
     <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A805" s="21"/>
+      <c r="A805" s="24"/>
     </row>
     <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A806" s="21"/>
+      <c r="A806" s="24"/>
     </row>
     <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A807" s="21"/>
+      <c r="A807" s="24"/>
     </row>
     <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A808" s="21"/>
+      <c r="A808" s="24"/>
     </row>
     <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A809" s="21"/>
+      <c r="A809" s="24"/>
     </row>
     <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A810" s="21"/>
+      <c r="A810" s="24"/>
     </row>
     <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A811" s="21"/>
+      <c r="A811" s="24"/>
     </row>
     <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A812" s="21"/>
+      <c r="A812" s="24"/>
     </row>
     <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A813" s="21"/>
+      <c r="A813" s="24"/>
     </row>
     <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A814" s="21"/>
+      <c r="A814" s="24"/>
     </row>
     <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A815" s="21"/>
+      <c r="A815" s="24"/>
     </row>
     <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A816" s="21"/>
+      <c r="A816" s="24"/>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A817" s="21"/>
+      <c r="A817" s="24"/>
     </row>
     <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A818" s="21"/>
+      <c r="A818" s="24"/>
     </row>
     <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A819" s="21"/>
+      <c r="A819" s="24"/>
     </row>
     <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A820" s="21"/>
+      <c r="A820" s="24"/>
     </row>
     <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A821" s="21"/>
+      <c r="A821" s="24"/>
     </row>
     <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A822" s="21"/>
+      <c r="A822" s="24"/>
     </row>
     <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A823" s="21"/>
+      <c r="A823" s="24"/>
     </row>
     <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A824" s="21"/>
+      <c r="A824" s="24"/>
     </row>
     <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A825" s="21"/>
+      <c r="A825" s="24"/>
     </row>
     <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A826" s="21"/>
+      <c r="A826" s="24"/>
     </row>
     <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A827" s="21"/>
+      <c r="A827" s="24"/>
     </row>
     <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A828" s="21"/>
+      <c r="A828" s="24"/>
     </row>
     <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A829" s="21"/>
+      <c r="A829" s="24"/>
     </row>
     <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A830" s="21"/>
+      <c r="A830" s="24"/>
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A831" s="21"/>
+      <c r="A831" s="24"/>
     </row>
     <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A832" s="21"/>
+      <c r="A832" s="24"/>
     </row>
     <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A833" s="21"/>
+      <c r="A833" s="24"/>
     </row>
     <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A834" s="21"/>
+      <c r="A834" s="24"/>
     </row>
     <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A835" s="21"/>
+      <c r="A835" s="24"/>
     </row>
     <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A836" s="21"/>
+      <c r="A836" s="24"/>
     </row>
     <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A837" s="21"/>
+      <c r="A837" s="24"/>
     </row>
     <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A838" s="21"/>
+      <c r="A838" s="24"/>
     </row>
     <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A839" s="21"/>
+      <c r="A839" s="24"/>
     </row>
     <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A840" s="21"/>
+      <c r="A840" s="24"/>
     </row>
     <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A841" s="21"/>
+      <c r="A841" s="24"/>
     </row>
     <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A842" s="21"/>
+      <c r="A842" s="24"/>
     </row>
     <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A843" s="21"/>
+      <c r="A843" s="24"/>
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A844" s="21"/>
+      <c r="A844" s="24"/>
     </row>
     <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A845" s="21"/>
+      <c r="A845" s="24"/>
     </row>
     <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A846" s="21"/>
+      <c r="A846" s="24"/>
     </row>
     <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A847" s="21"/>
+      <c r="A847" s="24"/>
     </row>
     <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A848" s="21"/>
+      <c r="A848" s="24"/>
     </row>
     <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A849" s="21"/>
+      <c r="A849" s="24"/>
     </row>
     <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A850" s="21"/>
+      <c r="A850" s="24"/>
     </row>
     <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A851" s="21"/>
+      <c r="A851" s="24"/>
     </row>
     <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A852" s="21"/>
+      <c r="A852" s="24"/>
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A853" s="21"/>
+      <c r="A853" s="24"/>
     </row>
     <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A854" s="21"/>
+      <c r="A854" s="24"/>
     </row>
     <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A855" s="21"/>
+      <c r="A855" s="24"/>
     </row>
     <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A856" s="21"/>
+      <c r="A856" s="24"/>
     </row>
     <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A857" s="21"/>
+      <c r="A857" s="24"/>
     </row>
     <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A858" s="21"/>
+      <c r="A858" s="24"/>
     </row>
     <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A859" s="21"/>
+      <c r="A859" s="24"/>
     </row>
     <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A860" s="21"/>
+      <c r="A860" s="24"/>
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A861" s="21"/>
+      <c r="A861" s="24"/>
     </row>
     <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A862" s="21"/>
+      <c r="A862" s="24"/>
     </row>
     <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A863" s="21"/>
+      <c r="A863" s="24"/>
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A864" s="21"/>
+      <c r="A864" s="24"/>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A865" s="21"/>
+      <c r="A865" s="24"/>
     </row>
     <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A866" s="21"/>
+      <c r="A866" s="24"/>
     </row>
     <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A867" s="21"/>
+      <c r="A867" s="24"/>
     </row>
     <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A868" s="21"/>
+      <c r="A868" s="24"/>
     </row>
     <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A869" s="21"/>
+      <c r="A869" s="24"/>
     </row>
     <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A870" s="21"/>
+      <c r="A870" s="24"/>
     </row>
     <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A871" s="21"/>
+      <c r="A871" s="24"/>
     </row>
     <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A872" s="21"/>
+      <c r="A872" s="24"/>
     </row>
     <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A873" s="21"/>
+      <c r="A873" s="24"/>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A874" s="21"/>
+      <c r="A874" s="24"/>
     </row>
     <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A875" s="21"/>
+      <c r="A875" s="24"/>
     </row>
     <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A876" s="21"/>
+      <c r="A876" s="24"/>
     </row>
     <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A877" s="21"/>
+      <c r="A877" s="24"/>
     </row>
     <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A878" s="21"/>
+      <c r="A878" s="24"/>
     </row>
     <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A879" s="21"/>
+      <c r="A879" s="24"/>
     </row>
     <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A880" s="21"/>
+      <c r="A880" s="24"/>
     </row>
     <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A881" s="21"/>
+      <c r="A881" s="24"/>
     </row>
     <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A882" s="21"/>
+      <c r="A882" s="24"/>
     </row>
     <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A883" s="21"/>
+      <c r="A883" s="24"/>
     </row>
     <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A884" s="21"/>
+      <c r="A884" s="24"/>
     </row>
     <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A885" s="21"/>
+      <c r="A885" s="24"/>
     </row>
     <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A886" s="21"/>
+      <c r="A886" s="24"/>
     </row>
     <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A887" s="21"/>
+      <c r="A887" s="24"/>
     </row>
     <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A888" s="21"/>
+      <c r="A888" s="24"/>
     </row>
     <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A889" s="21"/>
+      <c r="A889" s="24"/>
     </row>
     <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A890" s="21"/>
+      <c r="A890" s="24"/>
     </row>
     <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A891" s="21"/>
+      <c r="A891" s="24"/>
     </row>
     <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A892" s="21"/>
+      <c r="A892" s="24"/>
     </row>
     <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A893" s="21"/>
+      <c r="A893" s="24"/>
     </row>
     <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A894" s="21"/>
+      <c r="A894" s="24"/>
     </row>
     <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A895" s="21"/>
+      <c r="A895" s="24"/>
     </row>
     <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A896" s="21"/>
+      <c r="A896" s="24"/>
     </row>
     <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A897" s="21"/>
+      <c r="A897" s="24"/>
     </row>
     <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A898" s="21"/>
+      <c r="A898" s="24"/>
     </row>
     <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A899" s="21"/>
+      <c r="A899" s="24"/>
     </row>
     <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A900" s="21"/>
+      <c r="A900" s="24"/>
     </row>
     <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A901" s="21"/>
+      <c r="A901" s="24"/>
     </row>
     <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A902" s="21"/>
+      <c r="A902" s="24"/>
     </row>
     <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A903" s="21"/>
+      <c r="A903" s="24"/>
     </row>
     <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A904" s="21"/>
+      <c r="A904" s="24"/>
     </row>
     <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A905" s="21"/>
+      <c r="A905" s="24"/>
     </row>
     <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A906" s="21"/>
+      <c r="A906" s="24"/>
     </row>
     <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A907" s="21"/>
+      <c r="A907" s="24"/>
     </row>
     <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A908" s="21"/>
+      <c r="A908" s="24"/>
     </row>
     <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A909" s="21"/>
+      <c r="A909" s="24"/>
     </row>
     <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A910" s="21"/>
+      <c r="A910" s="24"/>
     </row>
     <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A911" s="21"/>
+      <c r="A911" s="24"/>
     </row>
     <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A912" s="21"/>
+      <c r="A912" s="24"/>
     </row>
     <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A913" s="21"/>
+      <c r="A913" s="24"/>
     </row>
     <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A914" s="21"/>
+      <c r="A914" s="24"/>
     </row>
     <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A915" s="21"/>
+      <c r="A915" s="24"/>
     </row>
     <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A916" s="21"/>
+      <c r="A916" s="24"/>
     </row>
     <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A917" s="21"/>
+      <c r="A917" s="24"/>
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A918" s="21"/>
+      <c r="A918" s="24"/>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A919" s="21"/>
+      <c r="A919" s="24"/>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A920" s="21"/>
+      <c r="A920" s="24"/>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A921" s="21"/>
+      <c r="A921" s="24"/>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A922" s="21"/>
+      <c r="A922" s="24"/>
     </row>
     <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A923" s="21"/>
+      <c r="A923" s="24"/>
     </row>
     <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A924" s="21"/>
+      <c r="A924" s="24"/>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A925" s="21"/>
+      <c r="A925" s="24"/>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A926" s="21"/>
+      <c r="A926" s="24"/>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A927" s="21"/>
+      <c r="A927" s="24"/>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A928" s="21"/>
+      <c r="A928" s="24"/>
     </row>
     <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A929" s="21"/>
+      <c r="A929" s="24"/>
     </row>
     <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A930" s="21"/>
+      <c r="A930" s="24"/>
     </row>
     <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A931" s="21"/>
+      <c r="A931" s="24"/>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A932" s="21"/>
+      <c r="A932" s="24"/>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A933" s="21"/>
+      <c r="A933" s="24"/>
     </row>
     <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A934" s="21"/>
+      <c r="A934" s="24"/>
     </row>
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A935" s="21"/>
+      <c r="A935" s="24"/>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A936" s="21"/>
+      <c r="A936" s="24"/>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A937" s="21"/>
+      <c r="A937" s="24"/>
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A938" s="21"/>
+      <c r="A938" s="24"/>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A939" s="21"/>
+      <c r="A939" s="24"/>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A940" s="21"/>
+      <c r="A940" s="24"/>
     </row>
     <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A941" s="21"/>
+      <c r="A941" s="24"/>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A942" s="21"/>
+      <c r="A942" s="24"/>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A943" s="21"/>
+      <c r="A943" s="24"/>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A944" s="21"/>
+      <c r="A944" s="24"/>
     </row>
     <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A945" s="21"/>
+      <c r="A945" s="24"/>
     </row>
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A946" s="21"/>
+      <c r="A946" s="24"/>
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A947" s="21"/>
+      <c r="A947" s="24"/>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A948" s="21"/>
+      <c r="A948" s="24"/>
     </row>
     <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A949" s="21"/>
+      <c r="A949" s="24"/>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A950" s="21"/>
+      <c r="A950" s="24"/>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A951" s="21"/>
+      <c r="A951" s="24"/>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A952" s="21"/>
+      <c r="A952" s="24"/>
     </row>
     <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A953" s="21"/>
+      <c r="A953" s="24"/>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A954" s="21"/>
+      <c r="A954" s="24"/>
     </row>
     <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A955" s="21"/>
+      <c r="A955" s="24"/>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A956" s="21"/>
+      <c r="A956" s="24"/>
     </row>
     <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A957" s="21"/>
+      <c r="A957" s="24"/>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A958" s="21"/>
+      <c r="A958" s="24"/>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A959" s="21"/>
+      <c r="A959" s="24"/>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A960" s="21"/>
+      <c r="A960" s="24"/>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A961" s="21"/>
+      <c r="A961" s="24"/>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A962" s="21"/>
+      <c r="A962" s="24"/>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A963" s="21"/>
+      <c r="A963" s="24"/>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A964" s="21"/>
+      <c r="A964" s="24"/>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A965" s="21"/>
+      <c r="A965" s="24"/>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A966" s="21"/>
+      <c r="A966" s="24"/>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A967" s="21"/>
+      <c r="A967" s="24"/>
     </row>
     <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A968" s="21"/>
+      <c r="A968" s="24"/>
     </row>
     <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A969" s="21"/>
+      <c r="A969" s="24"/>
     </row>
     <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A970" s="21"/>
+      <c r="A970" s="24"/>
     </row>
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A971" s="21"/>
+      <c r="A971" s="24"/>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A972" s="21"/>
+      <c r="A972" s="24"/>
     </row>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A973" s="21"/>
+      <c r="A973" s="24"/>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A974" s="21"/>
+      <c r="A974" s="24"/>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A975" s="21"/>
+      <c r="A975" s="24"/>
     </row>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A976" s="21"/>
+      <c r="A976" s="24"/>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A977" s="21"/>
+      <c r="A977" s="24"/>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A978" s="21"/>
+      <c r="A978" s="24"/>
     </row>
     <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A979" s="21"/>
+      <c r="A979" s="24"/>
     </row>
     <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A980" s="21"/>
+      <c r="A980" s="24"/>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A981" s="21"/>
+      <c r="A981" s="24"/>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A982" s="21"/>
+      <c r="A982" s="24"/>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A983" s="21"/>
+      <c r="A983" s="24"/>
     </row>
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A984" s="21"/>
+      <c r="A984" s="24"/>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A985" s="21"/>
+      <c r="A985" s="24"/>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A986" s="21"/>
+      <c r="A986" s="24"/>
     </row>
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A987" s="21"/>
+      <c r="A987" s="24"/>
     </row>
     <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A988" s="21"/>
+      <c r="A988" s="24"/>
     </row>
     <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A989" s="21"/>
+      <c r="A989" s="24"/>
     </row>
     <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A990" s="21"/>
+      <c r="A990" s="24"/>
     </row>
     <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A991" s="21"/>
+      <c r="A991" s="24"/>
     </row>
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A992" s="21"/>
+      <c r="A992" s="24"/>
     </row>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A993" s="21"/>
+      <c r="A993" s="24"/>
     </row>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A994" s="21"/>
+      <c r="A994" s="24"/>
     </row>
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A995" s="21"/>
+      <c r="A995" s="24"/>
     </row>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A996" s="21"/>
+      <c r="A996" s="24"/>
     </row>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A997" s="21"/>
+      <c r="A997" s="24"/>
     </row>
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A998" s="21"/>
+      <c r="A998" s="24"/>
     </row>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A999" s="21"/>
+      <c r="A999" s="24"/>
     </row>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1000" s="21"/>
+      <c r="A1000" s="24"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
pushing netcode blind 75 problem solutions
LC 79, 322,102,300,322,347,48,54,73,79
</commit_message>
<xml_diff>
--- a/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/LeetCode Problems/Neetcode Blind 75 problems/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -976,7 +976,7 @@
     <t xml:space="preserve">https://neetcode.io/</t>
   </si>
   <si>
-    <t xml:space="preserve">36 remaining</t>
+    <t xml:space="preserve">32 remaining</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1330,10 +1330,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1566,8 +1562,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E60" activeCellId="0" sqref="E60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1871,7 +1867,7 @@
       <c r="A18" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -1888,7 +1884,7 @@
       <c r="A19" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -1939,7 +1935,7 @@
       <c r="A22" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="9" t="s">
         <v>68</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -2112,7 +2108,7 @@
       <c r="B32" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>130</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -2123,13 +2119,13 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>134</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -2140,10 +2136,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C34" s="10" t="s">
@@ -2157,10 +2153,10 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C35" s="10" t="s">
@@ -2180,7 +2176,7 @@
       <c r="B36" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>147</v>
       </c>
       <c r="D36" s="8" t="s">
@@ -2228,7 +2224,7 @@
       <c r="A39" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -2242,10 +2238,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -2316,7 +2312,7 @@
       <c r="B44" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>180</v>
       </c>
       <c r="D44" s="8" t="s">
@@ -2330,7 +2326,7 @@
       <c r="A45" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C45" s="10" t="s">
@@ -2364,7 +2360,7 @@
       <c r="A47" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="16" t="s">
         <v>192</v>
       </c>
       <c r="C47" s="10" t="s">
@@ -2381,7 +2377,7 @@
       <c r="A48" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="6" t="s">
         <v>192</v>
       </c>
       <c r="C48" s="10" t="s">
@@ -2398,7 +2394,7 @@
       <c r="A49" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="6" t="s">
         <v>192</v>
       </c>
       <c r="C49" s="10" t="s">
@@ -2415,7 +2411,7 @@
       <c r="A50" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="6" t="s">
         <v>192</v>
       </c>
       <c r="C50" s="10" t="s">
@@ -2463,13 +2459,13 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="17" t="s">
         <v>217</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="13" t="s">
         <v>218</v>
       </c>
       <c r="D53" s="8" t="s">
@@ -2582,10 +2578,10 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="15" t="s">
         <v>209</v>
       </c>
       <c r="C60" s="10" t="s">
@@ -2653,10 +2649,10 @@
       <c r="A64" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B64" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="13" t="s">
         <v>263</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -2690,7 +2686,7 @@
       <c r="B66" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="13" t="s">
         <v>271</v>
       </c>
       <c r="D66" s="8" t="s">
@@ -2826,7 +2822,7 @@
       <c r="B74" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C74" s="13" t="s">
         <v>303</v>
       </c>
       <c r="D74" s="8" t="s">
@@ -2843,7 +2839,7 @@
       <c r="B75" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C75" s="14" t="s">
+      <c r="C75" s="13" t="s">
         <v>180</v>
       </c>
       <c r="D75" s="8" t="s">
@@ -2877,7 +2873,7 @@
       <c r="B77" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C77" s="14" t="s">
+      <c r="C77" s="13" t="s">
         <v>313</v>
       </c>
       <c r="D77" s="12" t="s">
@@ -2888,14 +2884,14 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="20"/>
-      <c r="B78" s="21"/>
+      <c r="A78" s="19"/>
+      <c r="B78" s="20"/>
     </row>
     <row r="79" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="22" t="s">
+      <c r="A79" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="22" t="s">
         <v>317</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -2903,2767 +2899,2767 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="24"/>
+      <c r="A80" s="23"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="24"/>
+      <c r="A81" s="23"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="24"/>
+      <c r="A82" s="23"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="24"/>
+      <c r="A83" s="23"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="24"/>
+      <c r="A84" s="23"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="24"/>
+      <c r="A85" s="23"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="24"/>
+      <c r="A86" s="23"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="24"/>
+      <c r="A87" s="23"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="24"/>
+      <c r="A88" s="23"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="24"/>
+      <c r="A89" s="23"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="24"/>
+      <c r="A90" s="23"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="24"/>
+      <c r="A91" s="23"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="24"/>
+      <c r="A92" s="23"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="24"/>
+      <c r="A93" s="23"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="24"/>
+      <c r="A94" s="23"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="24"/>
+      <c r="A95" s="23"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="24"/>
+      <c r="A96" s="23"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="24"/>
+      <c r="A97" s="23"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="24"/>
+      <c r="A98" s="23"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="24"/>
+      <c r="A99" s="23"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="24"/>
+      <c r="A100" s="23"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="24"/>
+      <c r="A101" s="23"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="24"/>
+      <c r="A102" s="23"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="24"/>
+      <c r="A103" s="23"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="24"/>
+      <c r="A104" s="23"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="24"/>
+      <c r="A105" s="23"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="24"/>
+      <c r="A106" s="23"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="24"/>
+      <c r="A107" s="23"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="24"/>
+      <c r="A108" s="23"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="24"/>
+      <c r="A109" s="23"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="24"/>
+      <c r="A110" s="23"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="24"/>
+      <c r="A111" s="23"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="24"/>
+      <c r="A112" s="23"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="24"/>
+      <c r="A113" s="23"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="24"/>
+      <c r="A114" s="23"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="24"/>
+      <c r="A115" s="23"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="24"/>
+      <c r="A116" s="23"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="24"/>
+      <c r="A117" s="23"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="24"/>
+      <c r="A118" s="23"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="24"/>
+      <c r="A119" s="23"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="24"/>
+      <c r="A120" s="23"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="24"/>
+      <c r="A121" s="23"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="24"/>
+      <c r="A122" s="23"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="24"/>
+      <c r="A123" s="23"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="24"/>
+      <c r="A124" s="23"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="24"/>
+      <c r="A125" s="23"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="24"/>
+      <c r="A126" s="23"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="24"/>
+      <c r="A127" s="23"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="24"/>
+      <c r="A128" s="23"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="24"/>
+      <c r="A129" s="23"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="24"/>
+      <c r="A130" s="23"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="24"/>
+      <c r="A131" s="23"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="24"/>
+      <c r="A132" s="23"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="24"/>
+      <c r="A133" s="23"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="24"/>
+      <c r="A134" s="23"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="24"/>
+      <c r="A135" s="23"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="24"/>
+      <c r="A136" s="23"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="24"/>
+      <c r="A137" s="23"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="24"/>
+      <c r="A138" s="23"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="24"/>
+      <c r="A139" s="23"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="24"/>
+      <c r="A140" s="23"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="24"/>
+      <c r="A141" s="23"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="24"/>
+      <c r="A142" s="23"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="24"/>
+      <c r="A143" s="23"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="24"/>
+      <c r="A144" s="23"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="24"/>
+      <c r="A145" s="23"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="24"/>
+      <c r="A146" s="23"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="24"/>
+      <c r="A147" s="23"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="24"/>
+      <c r="A148" s="23"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="24"/>
+      <c r="A149" s="23"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="24"/>
+      <c r="A150" s="23"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="24"/>
+      <c r="A151" s="23"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="24"/>
+      <c r="A152" s="23"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="24"/>
+      <c r="A153" s="23"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="24"/>
+      <c r="A154" s="23"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="24"/>
+      <c r="A155" s="23"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="24"/>
+      <c r="A156" s="23"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="24"/>
+      <c r="A157" s="23"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="24"/>
+      <c r="A158" s="23"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="24"/>
+      <c r="A159" s="23"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="24"/>
+      <c r="A160" s="23"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="24"/>
+      <c r="A161" s="23"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="24"/>
+      <c r="A162" s="23"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="24"/>
+      <c r="A163" s="23"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="24"/>
+      <c r="A164" s="23"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="24"/>
+      <c r="A165" s="23"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="24"/>
+      <c r="A166" s="23"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="24"/>
+      <c r="A167" s="23"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="24"/>
+      <c r="A168" s="23"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="24"/>
+      <c r="A169" s="23"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="24"/>
+      <c r="A170" s="23"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="24"/>
+      <c r="A171" s="23"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="24"/>
+      <c r="A172" s="23"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="24"/>
+      <c r="A173" s="23"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="24"/>
+      <c r="A174" s="23"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="24"/>
+      <c r="A175" s="23"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="24"/>
+      <c r="A176" s="23"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="24"/>
+      <c r="A177" s="23"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="24"/>
+      <c r="A178" s="23"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="24"/>
+      <c r="A179" s="23"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="24"/>
+      <c r="A180" s="23"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="24"/>
+      <c r="A181" s="23"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="24"/>
+      <c r="A182" s="23"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="24"/>
+      <c r="A183" s="23"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="24"/>
+      <c r="A184" s="23"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="24"/>
+      <c r="A185" s="23"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="24"/>
+      <c r="A186" s="23"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="24"/>
+      <c r="A187" s="23"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="24"/>
+      <c r="A188" s="23"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="24"/>
+      <c r="A189" s="23"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="24"/>
+      <c r="A190" s="23"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="24"/>
+      <c r="A191" s="23"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="24"/>
+      <c r="A192" s="23"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="24"/>
+      <c r="A193" s="23"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="24"/>
+      <c r="A194" s="23"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="24"/>
+      <c r="A195" s="23"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="24"/>
+      <c r="A196" s="23"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="24"/>
+      <c r="A197" s="23"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="24"/>
+      <c r="A198" s="23"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="24"/>
+      <c r="A199" s="23"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="24"/>
+      <c r="A200" s="23"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="24"/>
+      <c r="A201" s="23"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="24"/>
+      <c r="A202" s="23"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="24"/>
+      <c r="A203" s="23"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="24"/>
+      <c r="A204" s="23"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="24"/>
+      <c r="A205" s="23"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="24"/>
+      <c r="A206" s="23"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="24"/>
+      <c r="A207" s="23"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="24"/>
+      <c r="A208" s="23"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="24"/>
+      <c r="A209" s="23"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="24"/>
+      <c r="A210" s="23"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="24"/>
+      <c r="A211" s="23"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="24"/>
+      <c r="A212" s="23"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="24"/>
+      <c r="A213" s="23"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="24"/>
+      <c r="A214" s="23"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="24"/>
+      <c r="A215" s="23"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="24"/>
+      <c r="A216" s="23"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="24"/>
+      <c r="A217" s="23"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="24"/>
+      <c r="A218" s="23"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="24"/>
+      <c r="A219" s="23"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="24"/>
+      <c r="A220" s="23"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="24"/>
+      <c r="A221" s="23"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="24"/>
+      <c r="A222" s="23"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="24"/>
+      <c r="A223" s="23"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="24"/>
+      <c r="A224" s="23"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="24"/>
+      <c r="A225" s="23"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="24"/>
+      <c r="A226" s="23"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="24"/>
+      <c r="A227" s="23"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="24"/>
+      <c r="A228" s="23"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="24"/>
+      <c r="A229" s="23"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="24"/>
+      <c r="A230" s="23"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="24"/>
+      <c r="A231" s="23"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="24"/>
+      <c r="A232" s="23"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="24"/>
+      <c r="A233" s="23"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="24"/>
+      <c r="A234" s="23"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="24"/>
+      <c r="A235" s="23"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="24"/>
+      <c r="A236" s="23"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="24"/>
+      <c r="A237" s="23"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="24"/>
+      <c r="A238" s="23"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="24"/>
+      <c r="A239" s="23"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="24"/>
+      <c r="A240" s="23"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="24"/>
+      <c r="A241" s="23"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="24"/>
+      <c r="A242" s="23"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="24"/>
+      <c r="A243" s="23"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="24"/>
+      <c r="A244" s="23"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="24"/>
+      <c r="A245" s="23"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="24"/>
+      <c r="A246" s="23"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="24"/>
+      <c r="A247" s="23"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="24"/>
+      <c r="A248" s="23"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="24"/>
+      <c r="A249" s="23"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="24"/>
+      <c r="A250" s="23"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="24"/>
+      <c r="A251" s="23"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="24"/>
+      <c r="A252" s="23"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="24"/>
+      <c r="A253" s="23"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="24"/>
+      <c r="A254" s="23"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="24"/>
+      <c r="A255" s="23"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="24"/>
+      <c r="A256" s="23"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="24"/>
+      <c r="A257" s="23"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="24"/>
+      <c r="A258" s="23"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="24"/>
+      <c r="A259" s="23"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="24"/>
+      <c r="A260" s="23"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="24"/>
+      <c r="A261" s="23"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="24"/>
+      <c r="A262" s="23"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="24"/>
+      <c r="A263" s="23"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="24"/>
+      <c r="A264" s="23"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="24"/>
+      <c r="A265" s="23"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="24"/>
+      <c r="A266" s="23"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="24"/>
+      <c r="A267" s="23"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="24"/>
+      <c r="A268" s="23"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="24"/>
+      <c r="A269" s="23"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="24"/>
+      <c r="A270" s="23"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="24"/>
+      <c r="A271" s="23"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="24"/>
+      <c r="A272" s="23"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="24"/>
+      <c r="A273" s="23"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="24"/>
+      <c r="A274" s="23"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="24"/>
+      <c r="A275" s="23"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="24"/>
+      <c r="A276" s="23"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="24"/>
+      <c r="A277" s="23"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="24"/>
+      <c r="A278" s="23"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="24"/>
+      <c r="A279" s="23"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="24"/>
+      <c r="A280" s="23"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="24"/>
+      <c r="A281" s="23"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="24"/>
+      <c r="A282" s="23"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="24"/>
+      <c r="A283" s="23"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="24"/>
+      <c r="A284" s="23"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="24"/>
+      <c r="A285" s="23"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="24"/>
+      <c r="A286" s="23"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="24"/>
+      <c r="A287" s="23"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="24"/>
+      <c r="A288" s="23"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="24"/>
+      <c r="A289" s="23"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="24"/>
+      <c r="A290" s="23"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="24"/>
+      <c r="A291" s="23"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="24"/>
+      <c r="A292" s="23"/>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="24"/>
+      <c r="A293" s="23"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="24"/>
+      <c r="A294" s="23"/>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="24"/>
+      <c r="A295" s="23"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="24"/>
+      <c r="A296" s="23"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="24"/>
+      <c r="A297" s="23"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="24"/>
+      <c r="A298" s="23"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="24"/>
+      <c r="A299" s="23"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="24"/>
+      <c r="A300" s="23"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="24"/>
+      <c r="A301" s="23"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="24"/>
+      <c r="A302" s="23"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="24"/>
+      <c r="A303" s="23"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="24"/>
+      <c r="A304" s="23"/>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="24"/>
+      <c r="A305" s="23"/>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="24"/>
+      <c r="A306" s="23"/>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="24"/>
+      <c r="A307" s="23"/>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="24"/>
+      <c r="A308" s="23"/>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="24"/>
+      <c r="A309" s="23"/>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="24"/>
+      <c r="A310" s="23"/>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="24"/>
+      <c r="A311" s="23"/>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="24"/>
+      <c r="A312" s="23"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="24"/>
+      <c r="A313" s="23"/>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="24"/>
+      <c r="A314" s="23"/>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="24"/>
+      <c r="A315" s="23"/>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="24"/>
+      <c r="A316" s="23"/>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="24"/>
+      <c r="A317" s="23"/>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="24"/>
+      <c r="A318" s="23"/>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="24"/>
+      <c r="A319" s="23"/>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="24"/>
+      <c r="A320" s="23"/>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="24"/>
+      <c r="A321" s="23"/>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="24"/>
+      <c r="A322" s="23"/>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="24"/>
+      <c r="A323" s="23"/>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="24"/>
+      <c r="A324" s="23"/>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="24"/>
+      <c r="A325" s="23"/>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="24"/>
+      <c r="A326" s="23"/>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A327" s="24"/>
+      <c r="A327" s="23"/>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="24"/>
+      <c r="A328" s="23"/>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="24"/>
+      <c r="A329" s="23"/>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="24"/>
+      <c r="A330" s="23"/>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="24"/>
+      <c r="A331" s="23"/>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="24"/>
+      <c r="A332" s="23"/>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A333" s="24"/>
+      <c r="A333" s="23"/>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A334" s="24"/>
+      <c r="A334" s="23"/>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="24"/>
+      <c r="A335" s="23"/>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="24"/>
+      <c r="A336" s="23"/>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="24"/>
+      <c r="A337" s="23"/>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="24"/>
+      <c r="A338" s="23"/>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="24"/>
+      <c r="A339" s="23"/>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A340" s="24"/>
+      <c r="A340" s="23"/>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="24"/>
+      <c r="A341" s="23"/>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="24"/>
+      <c r="A342" s="23"/>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A343" s="24"/>
+      <c r="A343" s="23"/>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A344" s="24"/>
+      <c r="A344" s="23"/>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A345" s="24"/>
+      <c r="A345" s="23"/>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="24"/>
+      <c r="A346" s="23"/>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A347" s="24"/>
+      <c r="A347" s="23"/>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A348" s="24"/>
+      <c r="A348" s="23"/>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="24"/>
+      <c r="A349" s="23"/>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="24"/>
+      <c r="A350" s="23"/>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="24"/>
+      <c r="A351" s="23"/>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="24"/>
+      <c r="A352" s="23"/>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="24"/>
+      <c r="A353" s="23"/>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="24"/>
+      <c r="A354" s="23"/>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="24"/>
+      <c r="A355" s="23"/>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="24"/>
+      <c r="A356" s="23"/>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="24"/>
+      <c r="A357" s="23"/>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="24"/>
+      <c r="A358" s="23"/>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="24"/>
+      <c r="A359" s="23"/>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="24"/>
+      <c r="A360" s="23"/>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="24"/>
+      <c r="A361" s="23"/>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="24"/>
+      <c r="A362" s="23"/>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A363" s="24"/>
+      <c r="A363" s="23"/>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A364" s="24"/>
+      <c r="A364" s="23"/>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A365" s="24"/>
+      <c r="A365" s="23"/>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A366" s="24"/>
+      <c r="A366" s="23"/>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A367" s="24"/>
+      <c r="A367" s="23"/>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A368" s="24"/>
+      <c r="A368" s="23"/>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A369" s="24"/>
+      <c r="A369" s="23"/>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A370" s="24"/>
+      <c r="A370" s="23"/>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A371" s="24"/>
+      <c r="A371" s="23"/>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A372" s="24"/>
+      <c r="A372" s="23"/>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A373" s="24"/>
+      <c r="A373" s="23"/>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="24"/>
+      <c r="A374" s="23"/>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A375" s="24"/>
+      <c r="A375" s="23"/>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A376" s="24"/>
+      <c r="A376" s="23"/>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A377" s="24"/>
+      <c r="A377" s="23"/>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A378" s="24"/>
+      <c r="A378" s="23"/>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A379" s="24"/>
+      <c r="A379" s="23"/>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A380" s="24"/>
+      <c r="A380" s="23"/>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A381" s="24"/>
+      <c r="A381" s="23"/>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A382" s="24"/>
+      <c r="A382" s="23"/>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="24"/>
+      <c r="A383" s="23"/>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A384" s="24"/>
+      <c r="A384" s="23"/>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A385" s="24"/>
+      <c r="A385" s="23"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A386" s="24"/>
+      <c r="A386" s="23"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="24"/>
+      <c r="A387" s="23"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A388" s="24"/>
+      <c r="A388" s="23"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="24"/>
+      <c r="A389" s="23"/>
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A390" s="24"/>
+      <c r="A390" s="23"/>
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="24"/>
+      <c r="A391" s="23"/>
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A392" s="24"/>
+      <c r="A392" s="23"/>
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A393" s="24"/>
+      <c r="A393" s="23"/>
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A394" s="24"/>
+      <c r="A394" s="23"/>
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A395" s="24"/>
+      <c r="A395" s="23"/>
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="24"/>
+      <c r="A396" s="23"/>
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A397" s="24"/>
+      <c r="A397" s="23"/>
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A398" s="24"/>
+      <c r="A398" s="23"/>
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A399" s="24"/>
+      <c r="A399" s="23"/>
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A400" s="24"/>
+      <c r="A400" s="23"/>
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A401" s="24"/>
+      <c r="A401" s="23"/>
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A402" s="24"/>
+      <c r="A402" s="23"/>
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="24"/>
+      <c r="A403" s="23"/>
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A404" s="24"/>
+      <c r="A404" s="23"/>
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="24"/>
+      <c r="A405" s="23"/>
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A406" s="24"/>
+      <c r="A406" s="23"/>
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A407" s="24"/>
+      <c r="A407" s="23"/>
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A408" s="24"/>
+      <c r="A408" s="23"/>
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="24"/>
+      <c r="A409" s="23"/>
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="24"/>
+      <c r="A410" s="23"/>
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="24"/>
+      <c r="A411" s="23"/>
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A412" s="24"/>
+      <c r="A412" s="23"/>
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="24"/>
+      <c r="A413" s="23"/>
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A414" s="24"/>
+      <c r="A414" s="23"/>
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A415" s="24"/>
+      <c r="A415" s="23"/>
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A416" s="24"/>
+      <c r="A416" s="23"/>
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A417" s="24"/>
+      <c r="A417" s="23"/>
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="24"/>
+      <c r="A418" s="23"/>
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A419" s="24"/>
+      <c r="A419" s="23"/>
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="24"/>
+      <c r="A420" s="23"/>
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A421" s="24"/>
+      <c r="A421" s="23"/>
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A422" s="24"/>
+      <c r="A422" s="23"/>
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="24"/>
+      <c r="A423" s="23"/>
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A424" s="24"/>
+      <c r="A424" s="23"/>
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A425" s="24"/>
+      <c r="A425" s="23"/>
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A426" s="24"/>
+      <c r="A426" s="23"/>
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A427" s="24"/>
+      <c r="A427" s="23"/>
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A428" s="24"/>
+      <c r="A428" s="23"/>
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="24"/>
+      <c r="A429" s="23"/>
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A430" s="24"/>
+      <c r="A430" s="23"/>
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="24"/>
+      <c r="A431" s="23"/>
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="24"/>
+      <c r="A432" s="23"/>
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="24"/>
+      <c r="A433" s="23"/>
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="24"/>
+      <c r="A434" s="23"/>
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="24"/>
+      <c r="A435" s="23"/>
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="24"/>
+      <c r="A436" s="23"/>
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="24"/>
+      <c r="A437" s="23"/>
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A438" s="24"/>
+      <c r="A438" s="23"/>
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A439" s="24"/>
+      <c r="A439" s="23"/>
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="24"/>
+      <c r="A440" s="23"/>
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="24"/>
+      <c r="A441" s="23"/>
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A442" s="24"/>
+      <c r="A442" s="23"/>
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="24"/>
+      <c r="A443" s="23"/>
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A444" s="24"/>
+      <c r="A444" s="23"/>
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A445" s="24"/>
+      <c r="A445" s="23"/>
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A446" s="24"/>
+      <c r="A446" s="23"/>
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A447" s="24"/>
+      <c r="A447" s="23"/>
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A448" s="24"/>
+      <c r="A448" s="23"/>
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="24"/>
+      <c r="A449" s="23"/>
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A450" s="24"/>
+      <c r="A450" s="23"/>
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A451" s="24"/>
+      <c r="A451" s="23"/>
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A452" s="24"/>
+      <c r="A452" s="23"/>
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A453" s="24"/>
+      <c r="A453" s="23"/>
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A454" s="24"/>
+      <c r="A454" s="23"/>
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A455" s="24"/>
+      <c r="A455" s="23"/>
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A456" s="24"/>
+      <c r="A456" s="23"/>
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A457" s="24"/>
+      <c r="A457" s="23"/>
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A458" s="24"/>
+      <c r="A458" s="23"/>
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A459" s="24"/>
+      <c r="A459" s="23"/>
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A460" s="24"/>
+      <c r="A460" s="23"/>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A461" s="24"/>
+      <c r="A461" s="23"/>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A462" s="24"/>
+      <c r="A462" s="23"/>
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A463" s="24"/>
+      <c r="A463" s="23"/>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A464" s="24"/>
+      <c r="A464" s="23"/>
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A465" s="24"/>
+      <c r="A465" s="23"/>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A466" s="24"/>
+      <c r="A466" s="23"/>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A467" s="24"/>
+      <c r="A467" s="23"/>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A468" s="24"/>
+      <c r="A468" s="23"/>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A469" s="24"/>
+      <c r="A469" s="23"/>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A470" s="24"/>
+      <c r="A470" s="23"/>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A471" s="24"/>
+      <c r="A471" s="23"/>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A472" s="24"/>
+      <c r="A472" s="23"/>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A473" s="24"/>
+      <c r="A473" s="23"/>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A474" s="24"/>
+      <c r="A474" s="23"/>
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="24"/>
+      <c r="A475" s="23"/>
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A476" s="24"/>
+      <c r="A476" s="23"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A477" s="24"/>
+      <c r="A477" s="23"/>
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A478" s="24"/>
+      <c r="A478" s="23"/>
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A479" s="24"/>
+      <c r="A479" s="23"/>
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A480" s="24"/>
+      <c r="A480" s="23"/>
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A481" s="24"/>
+      <c r="A481" s="23"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="24"/>
+      <c r="A482" s="23"/>
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A483" s="24"/>
+      <c r="A483" s="23"/>
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A484" s="24"/>
+      <c r="A484" s="23"/>
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A485" s="24"/>
+      <c r="A485" s="23"/>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A486" s="24"/>
+      <c r="A486" s="23"/>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A487" s="24"/>
+      <c r="A487" s="23"/>
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A488" s="24"/>
+      <c r="A488" s="23"/>
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A489" s="24"/>
+      <c r="A489" s="23"/>
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A490" s="24"/>
+      <c r="A490" s="23"/>
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A491" s="24"/>
+      <c r="A491" s="23"/>
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A492" s="24"/>
+      <c r="A492" s="23"/>
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A493" s="24"/>
+      <c r="A493" s="23"/>
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A494" s="24"/>
+      <c r="A494" s="23"/>
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A495" s="24"/>
+      <c r="A495" s="23"/>
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A496" s="24"/>
+      <c r="A496" s="23"/>
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A497" s="24"/>
+      <c r="A497" s="23"/>
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A498" s="24"/>
+      <c r="A498" s="23"/>
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A499" s="24"/>
+      <c r="A499" s="23"/>
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A500" s="24"/>
+      <c r="A500" s="23"/>
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A501" s="24"/>
+      <c r="A501" s="23"/>
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A502" s="24"/>
+      <c r="A502" s="23"/>
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A503" s="24"/>
+      <c r="A503" s="23"/>
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A504" s="24"/>
+      <c r="A504" s="23"/>
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A505" s="24"/>
+      <c r="A505" s="23"/>
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A506" s="24"/>
+      <c r="A506" s="23"/>
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A507" s="24"/>
+      <c r="A507" s="23"/>
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A508" s="24"/>
+      <c r="A508" s="23"/>
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A509" s="24"/>
+      <c r="A509" s="23"/>
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A510" s="24"/>
+      <c r="A510" s="23"/>
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A511" s="24"/>
+      <c r="A511" s="23"/>
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A512" s="24"/>
+      <c r="A512" s="23"/>
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A513" s="24"/>
+      <c r="A513" s="23"/>
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A514" s="24"/>
+      <c r="A514" s="23"/>
     </row>
     <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A515" s="24"/>
+      <c r="A515" s="23"/>
     </row>
     <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A516" s="24"/>
+      <c r="A516" s="23"/>
     </row>
     <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A517" s="24"/>
+      <c r="A517" s="23"/>
     </row>
     <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A518" s="24"/>
+      <c r="A518" s="23"/>
     </row>
     <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A519" s="24"/>
+      <c r="A519" s="23"/>
     </row>
     <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A520" s="24"/>
+      <c r="A520" s="23"/>
     </row>
     <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A521" s="24"/>
+      <c r="A521" s="23"/>
     </row>
     <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A522" s="24"/>
+      <c r="A522" s="23"/>
     </row>
     <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A523" s="24"/>
+      <c r="A523" s="23"/>
     </row>
     <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A524" s="24"/>
+      <c r="A524" s="23"/>
     </row>
     <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A525" s="24"/>
+      <c r="A525" s="23"/>
     </row>
     <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A526" s="24"/>
+      <c r="A526" s="23"/>
     </row>
     <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A527" s="24"/>
+      <c r="A527" s="23"/>
     </row>
     <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A528" s="24"/>
+      <c r="A528" s="23"/>
     </row>
     <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A529" s="24"/>
+      <c r="A529" s="23"/>
     </row>
     <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A530" s="24"/>
+      <c r="A530" s="23"/>
     </row>
     <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A531" s="24"/>
+      <c r="A531" s="23"/>
     </row>
     <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A532" s="24"/>
+      <c r="A532" s="23"/>
     </row>
     <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A533" s="24"/>
+      <c r="A533" s="23"/>
     </row>
     <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A534" s="24"/>
+      <c r="A534" s="23"/>
     </row>
     <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A535" s="24"/>
+      <c r="A535" s="23"/>
     </row>
     <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A536" s="24"/>
+      <c r="A536" s="23"/>
     </row>
     <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A537" s="24"/>
+      <c r="A537" s="23"/>
     </row>
     <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A538" s="24"/>
+      <c r="A538" s="23"/>
     </row>
     <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A539" s="24"/>
+      <c r="A539" s="23"/>
     </row>
     <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A540" s="24"/>
+      <c r="A540" s="23"/>
     </row>
     <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A541" s="24"/>
+      <c r="A541" s="23"/>
     </row>
     <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A542" s="24"/>
+      <c r="A542" s="23"/>
     </row>
     <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A543" s="24"/>
+      <c r="A543" s="23"/>
     </row>
     <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A544" s="24"/>
+      <c r="A544" s="23"/>
     </row>
     <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A545" s="24"/>
+      <c r="A545" s="23"/>
     </row>
     <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A546" s="24"/>
+      <c r="A546" s="23"/>
     </row>
     <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A547" s="24"/>
+      <c r="A547" s="23"/>
     </row>
     <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A548" s="24"/>
+      <c r="A548" s="23"/>
     </row>
     <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A549" s="24"/>
+      <c r="A549" s="23"/>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A550" s="24"/>
+      <c r="A550" s="23"/>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A551" s="24"/>
+      <c r="A551" s="23"/>
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A552" s="24"/>
+      <c r="A552" s="23"/>
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A553" s="24"/>
+      <c r="A553" s="23"/>
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A554" s="24"/>
+      <c r="A554" s="23"/>
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A555" s="24"/>
+      <c r="A555" s="23"/>
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A556" s="24"/>
+      <c r="A556" s="23"/>
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A557" s="24"/>
+      <c r="A557" s="23"/>
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A558" s="24"/>
+      <c r="A558" s="23"/>
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A559" s="24"/>
+      <c r="A559" s="23"/>
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A560" s="24"/>
+      <c r="A560" s="23"/>
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A561" s="24"/>
+      <c r="A561" s="23"/>
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A562" s="24"/>
+      <c r="A562" s="23"/>
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A563" s="24"/>
+      <c r="A563" s="23"/>
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A564" s="24"/>
+      <c r="A564" s="23"/>
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A565" s="24"/>
+      <c r="A565" s="23"/>
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A566" s="24"/>
+      <c r="A566" s="23"/>
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A567" s="24"/>
+      <c r="A567" s="23"/>
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A568" s="24"/>
+      <c r="A568" s="23"/>
     </row>
     <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A569" s="24"/>
+      <c r="A569" s="23"/>
     </row>
     <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A570" s="24"/>
+      <c r="A570" s="23"/>
     </row>
     <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A571" s="24"/>
+      <c r="A571" s="23"/>
     </row>
     <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A572" s="24"/>
+      <c r="A572" s="23"/>
     </row>
     <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A573" s="24"/>
+      <c r="A573" s="23"/>
     </row>
     <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A574" s="24"/>
+      <c r="A574" s="23"/>
     </row>
     <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A575" s="24"/>
+      <c r="A575" s="23"/>
     </row>
     <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A576" s="24"/>
+      <c r="A576" s="23"/>
     </row>
     <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A577" s="24"/>
+      <c r="A577" s="23"/>
     </row>
     <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A578" s="24"/>
+      <c r="A578" s="23"/>
     </row>
     <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A579" s="24"/>
+      <c r="A579" s="23"/>
     </row>
     <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A580" s="24"/>
+      <c r="A580" s="23"/>
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A581" s="24"/>
+      <c r="A581" s="23"/>
     </row>
     <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A582" s="24"/>
+      <c r="A582" s="23"/>
     </row>
     <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A583" s="24"/>
+      <c r="A583" s="23"/>
     </row>
     <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A584" s="24"/>
+      <c r="A584" s="23"/>
     </row>
     <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A585" s="24"/>
+      <c r="A585" s="23"/>
     </row>
     <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A586" s="24"/>
+      <c r="A586" s="23"/>
     </row>
     <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A587" s="24"/>
+      <c r="A587" s="23"/>
     </row>
     <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A588" s="24"/>
+      <c r="A588" s="23"/>
     </row>
     <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A589" s="24"/>
+      <c r="A589" s="23"/>
     </row>
     <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A590" s="24"/>
+      <c r="A590" s="23"/>
     </row>
     <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A591" s="24"/>
+      <c r="A591" s="23"/>
     </row>
     <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A592" s="24"/>
+      <c r="A592" s="23"/>
     </row>
     <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A593" s="24"/>
+      <c r="A593" s="23"/>
     </row>
     <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A594" s="24"/>
+      <c r="A594" s="23"/>
     </row>
     <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A595" s="24"/>
+      <c r="A595" s="23"/>
     </row>
     <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A596" s="24"/>
+      <c r="A596" s="23"/>
     </row>
     <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A597" s="24"/>
+      <c r="A597" s="23"/>
     </row>
     <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A598" s="24"/>
+      <c r="A598" s="23"/>
     </row>
     <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A599" s="24"/>
+      <c r="A599" s="23"/>
     </row>
     <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A600" s="24"/>
+      <c r="A600" s="23"/>
     </row>
     <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A601" s="24"/>
+      <c r="A601" s="23"/>
     </row>
     <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A602" s="24"/>
+      <c r="A602" s="23"/>
     </row>
     <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A603" s="24"/>
+      <c r="A603" s="23"/>
     </row>
     <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A604" s="24"/>
+      <c r="A604" s="23"/>
     </row>
     <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A605" s="24"/>
+      <c r="A605" s="23"/>
     </row>
     <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A606" s="24"/>
+      <c r="A606" s="23"/>
     </row>
     <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A607" s="24"/>
+      <c r="A607" s="23"/>
     </row>
     <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A608" s="24"/>
+      <c r="A608" s="23"/>
     </row>
     <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A609" s="24"/>
+      <c r="A609" s="23"/>
     </row>
     <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A610" s="24"/>
+      <c r="A610" s="23"/>
     </row>
     <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A611" s="24"/>
+      <c r="A611" s="23"/>
     </row>
     <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A612" s="24"/>
+      <c r="A612" s="23"/>
     </row>
     <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A613" s="24"/>
+      <c r="A613" s="23"/>
     </row>
     <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A614" s="24"/>
+      <c r="A614" s="23"/>
     </row>
     <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A615" s="24"/>
+      <c r="A615" s="23"/>
     </row>
     <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A616" s="24"/>
+      <c r="A616" s="23"/>
     </row>
     <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A617" s="24"/>
+      <c r="A617" s="23"/>
     </row>
     <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A618" s="24"/>
+      <c r="A618" s="23"/>
     </row>
     <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A619" s="24"/>
+      <c r="A619" s="23"/>
     </row>
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A620" s="24"/>
+      <c r="A620" s="23"/>
     </row>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A621" s="24"/>
+      <c r="A621" s="23"/>
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A622" s="24"/>
+      <c r="A622" s="23"/>
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A623" s="24"/>
+      <c r="A623" s="23"/>
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A624" s="24"/>
+      <c r="A624" s="23"/>
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A625" s="24"/>
+      <c r="A625" s="23"/>
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A626" s="24"/>
+      <c r="A626" s="23"/>
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A627" s="24"/>
+      <c r="A627" s="23"/>
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A628" s="24"/>
+      <c r="A628" s="23"/>
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A629" s="24"/>
+      <c r="A629" s="23"/>
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A630" s="24"/>
+      <c r="A630" s="23"/>
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A631" s="24"/>
+      <c r="A631" s="23"/>
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A632" s="24"/>
+      <c r="A632" s="23"/>
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A633" s="24"/>
+      <c r="A633" s="23"/>
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A634" s="24"/>
+      <c r="A634" s="23"/>
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A635" s="24"/>
+      <c r="A635" s="23"/>
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A636" s="24"/>
+      <c r="A636" s="23"/>
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A637" s="24"/>
+      <c r="A637" s="23"/>
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A638" s="24"/>
+      <c r="A638" s="23"/>
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A639" s="24"/>
+      <c r="A639" s="23"/>
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A640" s="24"/>
+      <c r="A640" s="23"/>
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A641" s="24"/>
+      <c r="A641" s="23"/>
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A642" s="24"/>
+      <c r="A642" s="23"/>
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A643" s="24"/>
+      <c r="A643" s="23"/>
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A644" s="24"/>
+      <c r="A644" s="23"/>
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A645" s="24"/>
+      <c r="A645" s="23"/>
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A646" s="24"/>
+      <c r="A646" s="23"/>
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A647" s="24"/>
+      <c r="A647" s="23"/>
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A648" s="24"/>
+      <c r="A648" s="23"/>
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A649" s="24"/>
+      <c r="A649" s="23"/>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A650" s="24"/>
+      <c r="A650" s="23"/>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A651" s="24"/>
+      <c r="A651" s="23"/>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A652" s="24"/>
+      <c r="A652" s="23"/>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A653" s="24"/>
+      <c r="A653" s="23"/>
     </row>
     <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A654" s="24"/>
+      <c r="A654" s="23"/>
     </row>
     <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A655" s="24"/>
+      <c r="A655" s="23"/>
     </row>
     <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A656" s="24"/>
+      <c r="A656" s="23"/>
     </row>
     <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A657" s="24"/>
+      <c r="A657" s="23"/>
     </row>
     <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A658" s="24"/>
+      <c r="A658" s="23"/>
     </row>
     <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A659" s="24"/>
+      <c r="A659" s="23"/>
     </row>
     <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A660" s="24"/>
+      <c r="A660" s="23"/>
     </row>
     <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A661" s="24"/>
+      <c r="A661" s="23"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A662" s="24"/>
+      <c r="A662" s="23"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A663" s="24"/>
+      <c r="A663" s="23"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A664" s="24"/>
+      <c r="A664" s="23"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A665" s="24"/>
+      <c r="A665" s="23"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A666" s="24"/>
+      <c r="A666" s="23"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A667" s="24"/>
+      <c r="A667" s="23"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A668" s="24"/>
+      <c r="A668" s="23"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A669" s="24"/>
+      <c r="A669" s="23"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A670" s="24"/>
+      <c r="A670" s="23"/>
     </row>
     <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A671" s="24"/>
+      <c r="A671" s="23"/>
     </row>
     <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A672" s="24"/>
+      <c r="A672" s="23"/>
     </row>
     <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A673" s="24"/>
+      <c r="A673" s="23"/>
     </row>
     <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A674" s="24"/>
+      <c r="A674" s="23"/>
     </row>
     <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A675" s="24"/>
+      <c r="A675" s="23"/>
     </row>
     <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A676" s="24"/>
+      <c r="A676" s="23"/>
     </row>
     <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A677" s="24"/>
+      <c r="A677" s="23"/>
     </row>
     <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A678" s="24"/>
+      <c r="A678" s="23"/>
     </row>
     <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A679" s="24"/>
+      <c r="A679" s="23"/>
     </row>
     <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A680" s="24"/>
+      <c r="A680" s="23"/>
     </row>
     <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A681" s="24"/>
+      <c r="A681" s="23"/>
     </row>
     <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A682" s="24"/>
+      <c r="A682" s="23"/>
     </row>
     <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A683" s="24"/>
+      <c r="A683" s="23"/>
     </row>
     <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A684" s="24"/>
+      <c r="A684" s="23"/>
     </row>
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A685" s="24"/>
+      <c r="A685" s="23"/>
     </row>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A686" s="24"/>
+      <c r="A686" s="23"/>
     </row>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A687" s="24"/>
+      <c r="A687" s="23"/>
     </row>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A688" s="24"/>
+      <c r="A688" s="23"/>
     </row>
     <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A689" s="24"/>
+      <c r="A689" s="23"/>
     </row>
     <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A690" s="24"/>
+      <c r="A690" s="23"/>
     </row>
     <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A691" s="24"/>
+      <c r="A691" s="23"/>
     </row>
     <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A692" s="24"/>
+      <c r="A692" s="23"/>
     </row>
     <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A693" s="24"/>
+      <c r="A693" s="23"/>
     </row>
     <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A694" s="24"/>
+      <c r="A694" s="23"/>
     </row>
     <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A695" s="24"/>
+      <c r="A695" s="23"/>
     </row>
     <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A696" s="24"/>
+      <c r="A696" s="23"/>
     </row>
     <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A697" s="24"/>
+      <c r="A697" s="23"/>
     </row>
     <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A698" s="24"/>
+      <c r="A698" s="23"/>
     </row>
     <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A699" s="24"/>
+      <c r="A699" s="23"/>
     </row>
     <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A700" s="24"/>
+      <c r="A700" s="23"/>
     </row>
     <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A701" s="24"/>
+      <c r="A701" s="23"/>
     </row>
     <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A702" s="24"/>
+      <c r="A702" s="23"/>
     </row>
     <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A703" s="24"/>
+      <c r="A703" s="23"/>
     </row>
     <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A704" s="24"/>
+      <c r="A704" s="23"/>
     </row>
     <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A705" s="24"/>
+      <c r="A705" s="23"/>
     </row>
     <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A706" s="24"/>
+      <c r="A706" s="23"/>
     </row>
     <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A707" s="24"/>
+      <c r="A707" s="23"/>
     </row>
     <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A708" s="24"/>
+      <c r="A708" s="23"/>
     </row>
     <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A709" s="24"/>
+      <c r="A709" s="23"/>
     </row>
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A710" s="24"/>
+      <c r="A710" s="23"/>
     </row>
     <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A711" s="24"/>
+      <c r="A711" s="23"/>
     </row>
     <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A712" s="24"/>
+      <c r="A712" s="23"/>
     </row>
     <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A713" s="24"/>
+      <c r="A713" s="23"/>
     </row>
     <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A714" s="24"/>
+      <c r="A714" s="23"/>
     </row>
     <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A715" s="24"/>
+      <c r="A715" s="23"/>
     </row>
     <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A716" s="24"/>
+      <c r="A716" s="23"/>
     </row>
     <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A717" s="24"/>
+      <c r="A717" s="23"/>
     </row>
     <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A718" s="24"/>
+      <c r="A718" s="23"/>
     </row>
     <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A719" s="24"/>
+      <c r="A719" s="23"/>
     </row>
     <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A720" s="24"/>
+      <c r="A720" s="23"/>
     </row>
     <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A721" s="24"/>
+      <c r="A721" s="23"/>
     </row>
     <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A722" s="24"/>
+      <c r="A722" s="23"/>
     </row>
     <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A723" s="24"/>
+      <c r="A723" s="23"/>
     </row>
     <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A724" s="24"/>
+      <c r="A724" s="23"/>
     </row>
     <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A725" s="24"/>
+      <c r="A725" s="23"/>
     </row>
     <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A726" s="24"/>
+      <c r="A726" s="23"/>
     </row>
     <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A727" s="24"/>
+      <c r="A727" s="23"/>
     </row>
     <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A728" s="24"/>
+      <c r="A728" s="23"/>
     </row>
     <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A729" s="24"/>
+      <c r="A729" s="23"/>
     </row>
     <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A730" s="24"/>
+      <c r="A730" s="23"/>
     </row>
     <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A731" s="24"/>
+      <c r="A731" s="23"/>
     </row>
     <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A732" s="24"/>
+      <c r="A732" s="23"/>
     </row>
     <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A733" s="24"/>
+      <c r="A733" s="23"/>
     </row>
     <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A734" s="24"/>
+      <c r="A734" s="23"/>
     </row>
     <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A735" s="24"/>
+      <c r="A735" s="23"/>
     </row>
     <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A736" s="24"/>
+      <c r="A736" s="23"/>
     </row>
     <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A737" s="24"/>
+      <c r="A737" s="23"/>
     </row>
     <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A738" s="24"/>
+      <c r="A738" s="23"/>
     </row>
     <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A739" s="24"/>
+      <c r="A739" s="23"/>
     </row>
     <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A740" s="24"/>
+      <c r="A740" s="23"/>
     </row>
     <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A741" s="24"/>
+      <c r="A741" s="23"/>
     </row>
     <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A742" s="24"/>
+      <c r="A742" s="23"/>
     </row>
     <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A743" s="24"/>
+      <c r="A743" s="23"/>
     </row>
     <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A744" s="24"/>
+      <c r="A744" s="23"/>
     </row>
     <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A745" s="24"/>
+      <c r="A745" s="23"/>
     </row>
     <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A746" s="24"/>
+      <c r="A746" s="23"/>
     </row>
     <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A747" s="24"/>
+      <c r="A747" s="23"/>
     </row>
     <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A748" s="24"/>
+      <c r="A748" s="23"/>
     </row>
     <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A749" s="24"/>
+      <c r="A749" s="23"/>
     </row>
     <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A750" s="24"/>
+      <c r="A750" s="23"/>
     </row>
     <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A751" s="24"/>
+      <c r="A751" s="23"/>
     </row>
     <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A752" s="24"/>
+      <c r="A752" s="23"/>
     </row>
     <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A753" s="24"/>
+      <c r="A753" s="23"/>
     </row>
     <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A754" s="24"/>
+      <c r="A754" s="23"/>
     </row>
     <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A755" s="24"/>
+      <c r="A755" s="23"/>
     </row>
     <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A756" s="24"/>
+      <c r="A756" s="23"/>
     </row>
     <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A757" s="24"/>
+      <c r="A757" s="23"/>
     </row>
     <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A758" s="24"/>
+      <c r="A758" s="23"/>
     </row>
     <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A759" s="24"/>
+      <c r="A759" s="23"/>
     </row>
     <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A760" s="24"/>
+      <c r="A760" s="23"/>
     </row>
     <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A761" s="24"/>
+      <c r="A761" s="23"/>
     </row>
     <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A762" s="24"/>
+      <c r="A762" s="23"/>
     </row>
     <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A763" s="24"/>
+      <c r="A763" s="23"/>
     </row>
     <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A764" s="24"/>
+      <c r="A764" s="23"/>
     </row>
     <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A765" s="24"/>
+      <c r="A765" s="23"/>
     </row>
     <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A766" s="24"/>
+      <c r="A766" s="23"/>
     </row>
     <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A767" s="24"/>
+      <c r="A767" s="23"/>
     </row>
     <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A768" s="24"/>
+      <c r="A768" s="23"/>
     </row>
     <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A769" s="24"/>
+      <c r="A769" s="23"/>
     </row>
     <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A770" s="24"/>
+      <c r="A770" s="23"/>
     </row>
     <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A771" s="24"/>
+      <c r="A771" s="23"/>
     </row>
     <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A772" s="24"/>
+      <c r="A772" s="23"/>
     </row>
     <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A773" s="24"/>
+      <c r="A773" s="23"/>
     </row>
     <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A774" s="24"/>
+      <c r="A774" s="23"/>
     </row>
     <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A775" s="24"/>
+      <c r="A775" s="23"/>
     </row>
     <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A776" s="24"/>
+      <c r="A776" s="23"/>
     </row>
     <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A777" s="24"/>
+      <c r="A777" s="23"/>
     </row>
     <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A778" s="24"/>
+      <c r="A778" s="23"/>
     </row>
     <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A779" s="24"/>
+      <c r="A779" s="23"/>
     </row>
     <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A780" s="24"/>
+      <c r="A780" s="23"/>
     </row>
     <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A781" s="24"/>
+      <c r="A781" s="23"/>
     </row>
     <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A782" s="24"/>
+      <c r="A782" s="23"/>
     </row>
     <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A783" s="24"/>
+      <c r="A783" s="23"/>
     </row>
     <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A784" s="24"/>
+      <c r="A784" s="23"/>
     </row>
     <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A785" s="24"/>
+      <c r="A785" s="23"/>
     </row>
     <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A786" s="24"/>
+      <c r="A786" s="23"/>
     </row>
     <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A787" s="24"/>
+      <c r="A787" s="23"/>
     </row>
     <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A788" s="24"/>
+      <c r="A788" s="23"/>
     </row>
     <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A789" s="24"/>
+      <c r="A789" s="23"/>
     </row>
     <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A790" s="24"/>
+      <c r="A790" s="23"/>
     </row>
     <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A791" s="24"/>
+      <c r="A791" s="23"/>
     </row>
     <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A792" s="24"/>
+      <c r="A792" s="23"/>
     </row>
     <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A793" s="24"/>
+      <c r="A793" s="23"/>
     </row>
     <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A794" s="24"/>
+      <c r="A794" s="23"/>
     </row>
     <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A795" s="24"/>
+      <c r="A795" s="23"/>
     </row>
     <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A796" s="24"/>
+      <c r="A796" s="23"/>
     </row>
     <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A797" s="24"/>
+      <c r="A797" s="23"/>
     </row>
     <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A798" s="24"/>
+      <c r="A798" s="23"/>
     </row>
     <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A799" s="24"/>
+      <c r="A799" s="23"/>
     </row>
     <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A800" s="24"/>
+      <c r="A800" s="23"/>
     </row>
     <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A801" s="24"/>
+      <c r="A801" s="23"/>
     </row>
     <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A802" s="24"/>
+      <c r="A802" s="23"/>
     </row>
     <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A803" s="24"/>
+      <c r="A803" s="23"/>
     </row>
     <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A804" s="24"/>
+      <c r="A804" s="23"/>
     </row>
     <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A805" s="24"/>
+      <c r="A805" s="23"/>
     </row>
     <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A806" s="24"/>
+      <c r="A806" s="23"/>
     </row>
     <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A807" s="24"/>
+      <c r="A807" s="23"/>
     </row>
     <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A808" s="24"/>
+      <c r="A808" s="23"/>
     </row>
     <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A809" s="24"/>
+      <c r="A809" s="23"/>
     </row>
     <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A810" s="24"/>
+      <c r="A810" s="23"/>
     </row>
     <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A811" s="24"/>
+      <c r="A811" s="23"/>
     </row>
     <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A812" s="24"/>
+      <c r="A812" s="23"/>
     </row>
     <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A813" s="24"/>
+      <c r="A813" s="23"/>
     </row>
     <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A814" s="24"/>
+      <c r="A814" s="23"/>
     </row>
     <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A815" s="24"/>
+      <c r="A815" s="23"/>
     </row>
     <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A816" s="24"/>
+      <c r="A816" s="23"/>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A817" s="24"/>
+      <c r="A817" s="23"/>
     </row>
     <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A818" s="24"/>
+      <c r="A818" s="23"/>
     </row>
     <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A819" s="24"/>
+      <c r="A819" s="23"/>
     </row>
     <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A820" s="24"/>
+      <c r="A820" s="23"/>
     </row>
     <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A821" s="24"/>
+      <c r="A821" s="23"/>
     </row>
     <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A822" s="24"/>
+      <c r="A822" s="23"/>
     </row>
     <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A823" s="24"/>
+      <c r="A823" s="23"/>
     </row>
     <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A824" s="24"/>
+      <c r="A824" s="23"/>
     </row>
     <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A825" s="24"/>
+      <c r="A825" s="23"/>
     </row>
     <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A826" s="24"/>
+      <c r="A826" s="23"/>
     </row>
     <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A827" s="24"/>
+      <c r="A827" s="23"/>
     </row>
     <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A828" s="24"/>
+      <c r="A828" s="23"/>
     </row>
     <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A829" s="24"/>
+      <c r="A829" s="23"/>
     </row>
     <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A830" s="24"/>
+      <c r="A830" s="23"/>
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A831" s="24"/>
+      <c r="A831" s="23"/>
     </row>
     <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A832" s="24"/>
+      <c r="A832" s="23"/>
     </row>
     <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A833" s="24"/>
+      <c r="A833" s="23"/>
     </row>
     <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A834" s="24"/>
+      <c r="A834" s="23"/>
     </row>
     <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A835" s="24"/>
+      <c r="A835" s="23"/>
     </row>
     <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A836" s="24"/>
+      <c r="A836" s="23"/>
     </row>
     <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A837" s="24"/>
+      <c r="A837" s="23"/>
     </row>
     <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A838" s="24"/>
+      <c r="A838" s="23"/>
     </row>
     <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A839" s="24"/>
+      <c r="A839" s="23"/>
     </row>
     <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A840" s="24"/>
+      <c r="A840" s="23"/>
     </row>
     <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A841" s="24"/>
+      <c r="A841" s="23"/>
     </row>
     <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A842" s="24"/>
+      <c r="A842" s="23"/>
     </row>
     <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A843" s="24"/>
+      <c r="A843" s="23"/>
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A844" s="24"/>
+      <c r="A844" s="23"/>
     </row>
     <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A845" s="24"/>
+      <c r="A845" s="23"/>
     </row>
     <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A846" s="24"/>
+      <c r="A846" s="23"/>
     </row>
     <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A847" s="24"/>
+      <c r="A847" s="23"/>
     </row>
     <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A848" s="24"/>
+      <c r="A848" s="23"/>
     </row>
     <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A849" s="24"/>
+      <c r="A849" s="23"/>
     </row>
     <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A850" s="24"/>
+      <c r="A850" s="23"/>
     </row>
     <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A851" s="24"/>
+      <c r="A851" s="23"/>
     </row>
     <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A852" s="24"/>
+      <c r="A852" s="23"/>
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A853" s="24"/>
+      <c r="A853" s="23"/>
     </row>
     <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A854" s="24"/>
+      <c r="A854" s="23"/>
     </row>
     <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A855" s="24"/>
+      <c r="A855" s="23"/>
     </row>
     <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A856" s="24"/>
+      <c r="A856" s="23"/>
     </row>
     <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A857" s="24"/>
+      <c r="A857" s="23"/>
     </row>
     <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A858" s="24"/>
+      <c r="A858" s="23"/>
     </row>
     <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A859" s="24"/>
+      <c r="A859" s="23"/>
     </row>
     <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A860" s="24"/>
+      <c r="A860" s="23"/>
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A861" s="24"/>
+      <c r="A861" s="23"/>
     </row>
     <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A862" s="24"/>
+      <c r="A862" s="23"/>
     </row>
     <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A863" s="24"/>
+      <c r="A863" s="23"/>
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A864" s="24"/>
+      <c r="A864" s="23"/>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A865" s="24"/>
+      <c r="A865" s="23"/>
     </row>
     <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A866" s="24"/>
+      <c r="A866" s="23"/>
     </row>
     <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A867" s="24"/>
+      <c r="A867" s="23"/>
     </row>
     <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A868" s="24"/>
+      <c r="A868" s="23"/>
     </row>
     <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A869" s="24"/>
+      <c r="A869" s="23"/>
     </row>
     <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A870" s="24"/>
+      <c r="A870" s="23"/>
     </row>
     <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A871" s="24"/>
+      <c r="A871" s="23"/>
     </row>
     <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A872" s="24"/>
+      <c r="A872" s="23"/>
     </row>
     <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A873" s="24"/>
+      <c r="A873" s="23"/>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A874" s="24"/>
+      <c r="A874" s="23"/>
     </row>
     <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A875" s="24"/>
+      <c r="A875" s="23"/>
     </row>
     <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A876" s="24"/>
+      <c r="A876" s="23"/>
     </row>
     <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A877" s="24"/>
+      <c r="A877" s="23"/>
     </row>
     <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A878" s="24"/>
+      <c r="A878" s="23"/>
     </row>
     <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A879" s="24"/>
+      <c r="A879" s="23"/>
     </row>
     <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A880" s="24"/>
+      <c r="A880" s="23"/>
     </row>
     <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A881" s="24"/>
+      <c r="A881" s="23"/>
     </row>
     <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A882" s="24"/>
+      <c r="A882" s="23"/>
     </row>
     <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A883" s="24"/>
+      <c r="A883" s="23"/>
     </row>
     <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A884" s="24"/>
+      <c r="A884" s="23"/>
     </row>
     <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A885" s="24"/>
+      <c r="A885" s="23"/>
     </row>
     <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A886" s="24"/>
+      <c r="A886" s="23"/>
     </row>
     <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A887" s="24"/>
+      <c r="A887" s="23"/>
     </row>
     <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A888" s="24"/>
+      <c r="A888" s="23"/>
     </row>
     <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A889" s="24"/>
+      <c r="A889" s="23"/>
     </row>
     <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A890" s="24"/>
+      <c r="A890" s="23"/>
     </row>
     <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A891" s="24"/>
+      <c r="A891" s="23"/>
     </row>
     <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A892" s="24"/>
+      <c r="A892" s="23"/>
     </row>
     <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A893" s="24"/>
+      <c r="A893" s="23"/>
     </row>
     <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A894" s="24"/>
+      <c r="A894" s="23"/>
     </row>
     <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A895" s="24"/>
+      <c r="A895" s="23"/>
     </row>
     <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A896" s="24"/>
+      <c r="A896" s="23"/>
     </row>
     <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A897" s="24"/>
+      <c r="A897" s="23"/>
     </row>
     <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A898" s="24"/>
+      <c r="A898" s="23"/>
     </row>
     <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A899" s="24"/>
+      <c r="A899" s="23"/>
     </row>
     <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A900" s="24"/>
+      <c r="A900" s="23"/>
     </row>
     <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A901" s="24"/>
+      <c r="A901" s="23"/>
     </row>
     <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A902" s="24"/>
+      <c r="A902" s="23"/>
     </row>
     <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A903" s="24"/>
+      <c r="A903" s="23"/>
     </row>
     <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A904" s="24"/>
+      <c r="A904" s="23"/>
     </row>
     <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A905" s="24"/>
+      <c r="A905" s="23"/>
     </row>
     <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A906" s="24"/>
+      <c r="A906" s="23"/>
     </row>
     <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A907" s="24"/>
+      <c r="A907" s="23"/>
     </row>
     <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A908" s="24"/>
+      <c r="A908" s="23"/>
     </row>
     <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A909" s="24"/>
+      <c r="A909" s="23"/>
     </row>
     <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A910" s="24"/>
+      <c r="A910" s="23"/>
     </row>
     <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A911" s="24"/>
+      <c r="A911" s="23"/>
     </row>
     <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A912" s="24"/>
+      <c r="A912" s="23"/>
     </row>
     <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A913" s="24"/>
+      <c r="A913" s="23"/>
     </row>
     <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A914" s="24"/>
+      <c r="A914" s="23"/>
     </row>
     <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A915" s="24"/>
+      <c r="A915" s="23"/>
     </row>
     <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A916" s="24"/>
+      <c r="A916" s="23"/>
     </row>
     <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A917" s="24"/>
+      <c r="A917" s="23"/>
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A918" s="24"/>
+      <c r="A918" s="23"/>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A919" s="24"/>
+      <c r="A919" s="23"/>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A920" s="24"/>
+      <c r="A920" s="23"/>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A921" s="24"/>
+      <c r="A921" s="23"/>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A922" s="24"/>
+      <c r="A922" s="23"/>
     </row>
     <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A923" s="24"/>
+      <c r="A923" s="23"/>
     </row>
     <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A924" s="24"/>
+      <c r="A924" s="23"/>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A925" s="24"/>
+      <c r="A925" s="23"/>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A926" s="24"/>
+      <c r="A926" s="23"/>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A927" s="24"/>
+      <c r="A927" s="23"/>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A928" s="24"/>
+      <c r="A928" s="23"/>
     </row>
     <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A929" s="24"/>
+      <c r="A929" s="23"/>
     </row>
     <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A930" s="24"/>
+      <c r="A930" s="23"/>
     </row>
     <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A931" s="24"/>
+      <c r="A931" s="23"/>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A932" s="24"/>
+      <c r="A932" s="23"/>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A933" s="24"/>
+      <c r="A933" s="23"/>
     </row>
     <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A934" s="24"/>
+      <c r="A934" s="23"/>
     </row>
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A935" s="24"/>
+      <c r="A935" s="23"/>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A936" s="24"/>
+      <c r="A936" s="23"/>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A937" s="24"/>
+      <c r="A937" s="23"/>
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A938" s="24"/>
+      <c r="A938" s="23"/>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A939" s="24"/>
+      <c r="A939" s="23"/>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A940" s="24"/>
+      <c r="A940" s="23"/>
     </row>
     <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A941" s="24"/>
+      <c r="A941" s="23"/>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A942" s="24"/>
+      <c r="A942" s="23"/>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A943" s="24"/>
+      <c r="A943" s="23"/>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A944" s="24"/>
+      <c r="A944" s="23"/>
     </row>
     <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A945" s="24"/>
+      <c r="A945" s="23"/>
     </row>
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A946" s="24"/>
+      <c r="A946" s="23"/>
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A947" s="24"/>
+      <c r="A947" s="23"/>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A948" s="24"/>
+      <c r="A948" s="23"/>
     </row>
     <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A949" s="24"/>
+      <c r="A949" s="23"/>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A950" s="24"/>
+      <c r="A950" s="23"/>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A951" s="24"/>
+      <c r="A951" s="23"/>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A952" s="24"/>
+      <c r="A952" s="23"/>
     </row>
     <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A953" s="24"/>
+      <c r="A953" s="23"/>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A954" s="24"/>
+      <c r="A954" s="23"/>
     </row>
     <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A955" s="24"/>
+      <c r="A955" s="23"/>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A956" s="24"/>
+      <c r="A956" s="23"/>
     </row>
     <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A957" s="24"/>
+      <c r="A957" s="23"/>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A958" s="24"/>
+      <c r="A958" s="23"/>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A959" s="24"/>
+      <c r="A959" s="23"/>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A960" s="24"/>
+      <c r="A960" s="23"/>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A961" s="24"/>
+      <c r="A961" s="23"/>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A962" s="24"/>
+      <c r="A962" s="23"/>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A963" s="24"/>
+      <c r="A963" s="23"/>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A964" s="24"/>
+      <c r="A964" s="23"/>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A965" s="24"/>
+      <c r="A965" s="23"/>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A966" s="24"/>
+      <c r="A966" s="23"/>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A967" s="24"/>
+      <c r="A967" s="23"/>
     </row>
     <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A968" s="24"/>
+      <c r="A968" s="23"/>
     </row>
     <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A969" s="24"/>
+      <c r="A969" s="23"/>
     </row>
     <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A970" s="24"/>
+      <c r="A970" s="23"/>
     </row>
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A971" s="24"/>
+      <c r="A971" s="23"/>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A972" s="24"/>
+      <c r="A972" s="23"/>
     </row>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A973" s="24"/>
+      <c r="A973" s="23"/>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A974" s="24"/>
+      <c r="A974" s="23"/>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A975" s="24"/>
+      <c r="A975" s="23"/>
     </row>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A976" s="24"/>
+      <c r="A976" s="23"/>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A977" s="24"/>
+      <c r="A977" s="23"/>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A978" s="24"/>
+      <c r="A978" s="23"/>
     </row>
     <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A979" s="24"/>
+      <c r="A979" s="23"/>
     </row>
     <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A980" s="24"/>
+      <c r="A980" s="23"/>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A981" s="24"/>
+      <c r="A981" s="23"/>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A982" s="24"/>
+      <c r="A982" s="23"/>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A983" s="24"/>
+      <c r="A983" s="23"/>
     </row>
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A984" s="24"/>
+      <c r="A984" s="23"/>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A985" s="24"/>
+      <c r="A985" s="23"/>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A986" s="24"/>
+      <c r="A986" s="23"/>
     </row>
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A987" s="24"/>
+      <c r="A987" s="23"/>
     </row>
     <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A988" s="24"/>
+      <c r="A988" s="23"/>
     </row>
     <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A989" s="24"/>
+      <c r="A989" s="23"/>
     </row>
     <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A990" s="24"/>
+      <c r="A990" s="23"/>
     </row>
     <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A991" s="24"/>
+      <c r="A991" s="23"/>
     </row>
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A992" s="24"/>
+      <c r="A992" s="23"/>
     </row>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A993" s="24"/>
+      <c r="A993" s="23"/>
     </row>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A994" s="24"/>
+      <c r="A994" s="23"/>
     </row>
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A995" s="24"/>
+      <c r="A995" s="23"/>
     </row>
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A996" s="24"/>
+      <c r="A996" s="23"/>
     </row>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A997" s="24"/>
+      <c r="A997" s="23"/>
     </row>
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A998" s="24"/>
+      <c r="A998" s="23"/>
     </row>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A999" s="24"/>
+      <c r="A999" s="23"/>
     </row>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1000" s="24"/>
+      <c r="A1000" s="23"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>